<commit_message>
update of timeline working schedule
</commit_message>
<xml_diff>
--- a/Documentation/Gannt Chart.xlsx
+++ b/Documentation/Gannt Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5625" tabRatio="403"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="15315" windowHeight="5625" tabRatio="403" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Plan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Start</t>
   </si>
@@ -55,43 +55,10 @@
     <t>Project Deliverable 5</t>
   </si>
   <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>% Compl.</t>
   </si>
   <si>
-    <t>ACE Daily Sales Record</t>
-  </si>
-  <si>
-    <t>BOTLAIDS campaign requirement</t>
-  </si>
-  <si>
-    <t>Additional Remark</t>
-  </si>
-  <si>
     <t>1.0</t>
-  </si>
-  <si>
-    <t>Any format of excel</t>
-  </si>
-  <si>
-    <t>Text file in a fixed sequence, fixed number of fields</t>
-  </si>
-  <si>
-    <t>Output field</t>
-  </si>
-  <si>
-    <t>Days required</t>
-  </si>
-  <si>
-    <t>Tag for every line need to be named.</t>
-  </si>
-  <si>
-    <t>Any rpt file generated.</t>
-  </si>
-  <si>
-    <t>Not needed</t>
   </si>
   <si>
     <t>Version 0.1</t>
@@ -107,21 +74,6 @@
   </si>
   <si>
     <t>Project 2.0</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>Text file in any sequence, fixed number of fields</t>
-  </si>
-  <si>
-    <t>Text file in any sequence, any number of fields</t>
   </si>
   <si>
     <t>Version 0.2</t>
@@ -160,27 +112,76 @@
     <t>Overseas Leave</t>
   </si>
   <si>
-    <t>Single campaign code</t>
+    <t>Version Number</t>
   </si>
   <si>
-    <t>Single campaign code; Recognise field by name, not cell number</t>
+    <t>Estimated Date of completion</t>
   </si>
   <si>
-    <t>Single campaign code; Recognise missing field &amp; extra redundant information</t>
+    <t>Number of Days</t>
   </si>
   <si>
-    <t>Single campaign code; Need to find excel API</t>
+    <t>Task Description/ Change Log</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>System 6 Legacy</t>
+  </si>
+  <si>
+    <t>Building of API (Currently 10% done)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parsing of BOTLAIDS </t>
+  </si>
+  <si>
+    <t>Creating Data Template</t>
+  </si>
+  <si>
+    <t>Integration of API and BOTLAIDS</t>
+  </si>
+  <si>
+    <t>Integration of BOTLAID and Sample Data</t>
+  </si>
+  <si>
+    <t>Include UI, system integration</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Adapted a branch out ready for System 6 Renovation</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>1.0R</t>
+  </si>
+  <si>
+    <t>2.0R</t>
+  </si>
+  <si>
+    <t>Able to take in multiple BOTLAIDS (back end)</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Able to read multiple campagin in 1 excel file, change in UI to select multiple BOTLAID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="166" formatCode="mmm"/>
     <numFmt numFmtId="167" formatCode="m/d;@"/>
+    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1061,7 +1062,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1113,9 +1114,6 @@
     <xf numFmtId="167" fontId="4" fillId="4" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -1283,6 +1281,33 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1301,35 +1326,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4984,11 +4991,11 @@
   </sheetPr>
   <dimension ref="A1:CT53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
       <pane xSplit="7" ySplit="8" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5005,10 +5012,10 @@
     <row r="1" spans="1:98" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:98" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="108"/>
+      <c r="C2" s="116"/>
       <c r="D2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5016,105 +5023,105 @@
         <v>1</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="114" t="s">
+      <c r="H2" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
-      <c r="K2" s="115"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="115"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="115"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="115"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="115"/>
-      <c r="U2" s="115"/>
-      <c r="V2" s="115"/>
-      <c r="W2" s="115"/>
-      <c r="X2" s="115"/>
-      <c r="Y2" s="115"/>
-      <c r="Z2" s="115"/>
-      <c r="AA2" s="115"/>
-      <c r="AB2" s="115"/>
-      <c r="AC2" s="115"/>
-      <c r="AD2" s="115"/>
-      <c r="AE2" s="115"/>
-      <c r="AF2" s="115"/>
-      <c r="AG2" s="115"/>
-      <c r="AH2" s="115"/>
-      <c r="AI2" s="115"/>
-      <c r="AJ2" s="115"/>
-      <c r="AK2" s="115"/>
-      <c r="AL2" s="115"/>
-      <c r="AM2" s="115"/>
-      <c r="AN2" s="115"/>
-      <c r="AO2" s="115"/>
-      <c r="AP2" s="115"/>
-      <c r="AQ2" s="115"/>
-      <c r="AR2" s="115"/>
-      <c r="AS2" s="115"/>
-      <c r="AT2" s="115"/>
-      <c r="AU2" s="115"/>
-      <c r="AV2" s="115"/>
-      <c r="AW2" s="115"/>
-      <c r="AX2" s="115"/>
-      <c r="AY2" s="115"/>
-      <c r="AZ2" s="115"/>
-      <c r="BA2" s="115"/>
-      <c r="BB2" s="115"/>
-      <c r="BC2" s="115"/>
-      <c r="BD2" s="115"/>
-      <c r="BE2" s="115"/>
-      <c r="BF2" s="115"/>
-      <c r="BG2" s="115"/>
-      <c r="BH2" s="115"/>
-      <c r="BI2" s="115"/>
-      <c r="BJ2" s="115"/>
-      <c r="BK2" s="115"/>
-      <c r="BL2" s="115"/>
-      <c r="BM2" s="115"/>
-      <c r="BN2" s="115"/>
-      <c r="BO2" s="115"/>
-      <c r="BP2" s="115"/>
-      <c r="BQ2" s="115"/>
-      <c r="BR2" s="115"/>
-      <c r="BS2" s="115"/>
-      <c r="BT2" s="115"/>
-      <c r="BU2" s="115"/>
-      <c r="BV2" s="115"/>
-      <c r="BW2" s="115"/>
-      <c r="BX2" s="115"/>
-      <c r="BY2" s="115"/>
-      <c r="BZ2" s="115"/>
-      <c r="CA2" s="115"/>
-      <c r="CB2" s="115"/>
-      <c r="CC2" s="115"/>
-      <c r="CD2" s="115"/>
-      <c r="CE2" s="115"/>
-      <c r="CF2" s="115"/>
-      <c r="CG2" s="115"/>
-      <c r="CH2" s="115"/>
-      <c r="CI2" s="115"/>
-      <c r="CJ2" s="115"/>
-      <c r="CK2" s="115"/>
-      <c r="CL2" s="115"/>
-      <c r="CM2" s="115"/>
-      <c r="CN2" s="115"/>
-      <c r="CO2" s="115"/>
-      <c r="CP2" s="115"/>
-      <c r="CQ2" s="115"/>
-      <c r="CR2" s="115"/>
-      <c r="CS2" s="115"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="108"/>
+      <c r="P2" s="108"/>
+      <c r="Q2" s="108"/>
+      <c r="R2" s="108"/>
+      <c r="S2" s="108"/>
+      <c r="T2" s="108"/>
+      <c r="U2" s="108"/>
+      <c r="V2" s="108"/>
+      <c r="W2" s="108"/>
+      <c r="X2" s="108"/>
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="108"/>
+      <c r="AA2" s="108"/>
+      <c r="AB2" s="108"/>
+      <c r="AC2" s="108"/>
+      <c r="AD2" s="108"/>
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="108"/>
+      <c r="AG2" s="108"/>
+      <c r="AH2" s="108"/>
+      <c r="AI2" s="108"/>
+      <c r="AJ2" s="108"/>
+      <c r="AK2" s="108"/>
+      <c r="AL2" s="108"/>
+      <c r="AM2" s="108"/>
+      <c r="AN2" s="108"/>
+      <c r="AO2" s="108"/>
+      <c r="AP2" s="108"/>
+      <c r="AQ2" s="108"/>
+      <c r="AR2" s="108"/>
+      <c r="AS2" s="108"/>
+      <c r="AT2" s="108"/>
+      <c r="AU2" s="108"/>
+      <c r="AV2" s="108"/>
+      <c r="AW2" s="108"/>
+      <c r="AX2" s="108"/>
+      <c r="AY2" s="108"/>
+      <c r="AZ2" s="108"/>
+      <c r="BA2" s="108"/>
+      <c r="BB2" s="108"/>
+      <c r="BC2" s="108"/>
+      <c r="BD2" s="108"/>
+      <c r="BE2" s="108"/>
+      <c r="BF2" s="108"/>
+      <c r="BG2" s="108"/>
+      <c r="BH2" s="108"/>
+      <c r="BI2" s="108"/>
+      <c r="BJ2" s="108"/>
+      <c r="BK2" s="108"/>
+      <c r="BL2" s="108"/>
+      <c r="BM2" s="108"/>
+      <c r="BN2" s="108"/>
+      <c r="BO2" s="108"/>
+      <c r="BP2" s="108"/>
+      <c r="BQ2" s="108"/>
+      <c r="BR2" s="108"/>
+      <c r="BS2" s="108"/>
+      <c r="BT2" s="108"/>
+      <c r="BU2" s="108"/>
+      <c r="BV2" s="108"/>
+      <c r="BW2" s="108"/>
+      <c r="BX2" s="108"/>
+      <c r="BY2" s="108"/>
+      <c r="BZ2" s="108"/>
+      <c r="CA2" s="108"/>
+      <c r="CB2" s="108"/>
+      <c r="CC2" s="108"/>
+      <c r="CD2" s="108"/>
+      <c r="CE2" s="108"/>
+      <c r="CF2" s="108"/>
+      <c r="CG2" s="108"/>
+      <c r="CH2" s="108"/>
+      <c r="CI2" s="108"/>
+      <c r="CJ2" s="108"/>
+      <c r="CK2" s="108"/>
+      <c r="CL2" s="108"/>
+      <c r="CM2" s="108"/>
+      <c r="CN2" s="108"/>
+      <c r="CO2" s="108"/>
+      <c r="CP2" s="108"/>
+      <c r="CQ2" s="108"/>
+      <c r="CR2" s="108"/>
+      <c r="CS2" s="108"/>
     </row>
     <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="109" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="109"/>
+      <c r="B3" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="117"/>
       <c r="D3" s="14">
         <v>41112</v>
       </c>
@@ -5122,461 +5129,461 @@
         <v>41115</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="117"/>
-      <c r="J3" s="117"/>
-      <c r="K3" s="117"/>
-      <c r="L3" s="117"/>
-      <c r="M3" s="117"/>
-      <c r="N3" s="117"/>
-      <c r="O3" s="117"/>
-      <c r="P3" s="117"/>
-      <c r="Q3" s="117"/>
-      <c r="R3" s="117"/>
-      <c r="S3" s="117"/>
-      <c r="T3" s="117"/>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
-      <c r="W3" s="117"/>
-      <c r="X3" s="117"/>
-      <c r="Y3" s="117"/>
-      <c r="Z3" s="117"/>
-      <c r="AA3" s="117"/>
-      <c r="AB3" s="117"/>
-      <c r="AC3" s="117"/>
-      <c r="AD3" s="117"/>
-      <c r="AE3" s="117"/>
-      <c r="AF3" s="117"/>
-      <c r="AG3" s="117"/>
-      <c r="AH3" s="117"/>
-      <c r="AI3" s="117"/>
-      <c r="AJ3" s="117"/>
-      <c r="AK3" s="117"/>
-      <c r="AL3" s="117"/>
-      <c r="AM3" s="117"/>
-      <c r="AN3" s="117"/>
-      <c r="AO3" s="117"/>
-      <c r="AP3" s="117"/>
-      <c r="AQ3" s="117"/>
-      <c r="AR3" s="117"/>
-      <c r="AS3" s="117"/>
-      <c r="AT3" s="117"/>
-      <c r="AU3" s="117"/>
-      <c r="AV3" s="117"/>
-      <c r="AW3" s="117"/>
-      <c r="AX3" s="117"/>
-      <c r="AY3" s="117"/>
-      <c r="AZ3" s="117"/>
-      <c r="BA3" s="117"/>
-      <c r="BB3" s="117"/>
-      <c r="BC3" s="117"/>
-      <c r="BD3" s="117"/>
-      <c r="BE3" s="117"/>
-      <c r="BF3" s="117"/>
-      <c r="BG3" s="117"/>
-      <c r="BH3" s="117"/>
-      <c r="BI3" s="117"/>
-      <c r="BJ3" s="117"/>
-      <c r="BK3" s="117"/>
-      <c r="BL3" s="117"/>
-      <c r="BM3" s="117"/>
-      <c r="BN3" s="117"/>
-      <c r="BO3" s="117"/>
-      <c r="BP3" s="117"/>
-      <c r="BQ3" s="117"/>
-      <c r="BR3" s="117"/>
-      <c r="BS3" s="117"/>
-      <c r="BT3" s="117"/>
-      <c r="BU3" s="117"/>
-      <c r="BV3" s="117"/>
-      <c r="BW3" s="117"/>
-      <c r="BX3" s="117"/>
-      <c r="BY3" s="117"/>
-      <c r="BZ3" s="117"/>
-      <c r="CA3" s="117"/>
-      <c r="CB3" s="117"/>
-      <c r="CC3" s="117"/>
-      <c r="CD3" s="117"/>
-      <c r="CE3" s="117"/>
-      <c r="CF3" s="117"/>
-      <c r="CG3" s="117"/>
-      <c r="CH3" s="117"/>
-      <c r="CI3" s="117"/>
-      <c r="CJ3" s="117"/>
-      <c r="CK3" s="117"/>
-      <c r="CL3" s="117"/>
-      <c r="CM3" s="117"/>
-      <c r="CN3" s="117"/>
-      <c r="CO3" s="117"/>
-      <c r="CP3" s="117"/>
-      <c r="CQ3" s="117"/>
-      <c r="CR3" s="117"/>
-      <c r="CS3" s="117"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="110"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="110"/>
+      <c r="N3" s="110"/>
+      <c r="O3" s="110"/>
+      <c r="P3" s="110"/>
+      <c r="Q3" s="110"/>
+      <c r="R3" s="110"/>
+      <c r="S3" s="110"/>
+      <c r="T3" s="110"/>
+      <c r="U3" s="110"/>
+      <c r="V3" s="110"/>
+      <c r="W3" s="110"/>
+      <c r="X3" s="110"/>
+      <c r="Y3" s="110"/>
+      <c r="Z3" s="110"/>
+      <c r="AA3" s="110"/>
+      <c r="AB3" s="110"/>
+      <c r="AC3" s="110"/>
+      <c r="AD3" s="110"/>
+      <c r="AE3" s="110"/>
+      <c r="AF3" s="110"/>
+      <c r="AG3" s="110"/>
+      <c r="AH3" s="110"/>
+      <c r="AI3" s="110"/>
+      <c r="AJ3" s="110"/>
+      <c r="AK3" s="110"/>
+      <c r="AL3" s="110"/>
+      <c r="AM3" s="110"/>
+      <c r="AN3" s="110"/>
+      <c r="AO3" s="110"/>
+      <c r="AP3" s="110"/>
+      <c r="AQ3" s="110"/>
+      <c r="AR3" s="110"/>
+      <c r="AS3" s="110"/>
+      <c r="AT3" s="110"/>
+      <c r="AU3" s="110"/>
+      <c r="AV3" s="110"/>
+      <c r="AW3" s="110"/>
+      <c r="AX3" s="110"/>
+      <c r="AY3" s="110"/>
+      <c r="AZ3" s="110"/>
+      <c r="BA3" s="110"/>
+      <c r="BB3" s="110"/>
+      <c r="BC3" s="110"/>
+      <c r="BD3" s="110"/>
+      <c r="BE3" s="110"/>
+      <c r="BF3" s="110"/>
+      <c r="BG3" s="110"/>
+      <c r="BH3" s="110"/>
+      <c r="BI3" s="110"/>
+      <c r="BJ3" s="110"/>
+      <c r="BK3" s="110"/>
+      <c r="BL3" s="110"/>
+      <c r="BM3" s="110"/>
+      <c r="BN3" s="110"/>
+      <c r="BO3" s="110"/>
+      <c r="BP3" s="110"/>
+      <c r="BQ3" s="110"/>
+      <c r="BR3" s="110"/>
+      <c r="BS3" s="110"/>
+      <c r="BT3" s="110"/>
+      <c r="BU3" s="110"/>
+      <c r="BV3" s="110"/>
+      <c r="BW3" s="110"/>
+      <c r="BX3" s="110"/>
+      <c r="BY3" s="110"/>
+      <c r="BZ3" s="110"/>
+      <c r="CA3" s="110"/>
+      <c r="CB3" s="110"/>
+      <c r="CC3" s="110"/>
+      <c r="CD3" s="110"/>
+      <c r="CE3" s="110"/>
+      <c r="CF3" s="110"/>
+      <c r="CG3" s="110"/>
+      <c r="CH3" s="110"/>
+      <c r="CI3" s="110"/>
+      <c r="CJ3" s="110"/>
+      <c r="CK3" s="110"/>
+      <c r="CL3" s="110"/>
+      <c r="CM3" s="110"/>
+      <c r="CN3" s="110"/>
+      <c r="CO3" s="110"/>
+      <c r="CP3" s="110"/>
+      <c r="CQ3" s="110"/>
+      <c r="CR3" s="110"/>
+      <c r="CS3" s="110"/>
     </row>
     <row r="4" spans="1:98" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="110"/>
-      <c r="C4" s="110"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
       <c r="D4" s="14"/>
       <c r="E4" s="15"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="113">
+      <c r="H4" s="104">
         <f>IF(MONTH(H6)&lt;&gt;MONTH(E6),H6,"")</f>
         <v>41057</v>
       </c>
-      <c r="I4" s="113" t="str">
+      <c r="I4" s="104" t="str">
         <f t="shared" ref="I4:BT4" si="0">IF(MONTH(I6)&lt;&gt;MONTH(H6),I6,"")</f>
         <v/>
       </c>
-      <c r="J4" s="113" t="str">
+      <c r="J4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="113" t="str">
+      <c r="K4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L4" s="113">
+      <c r="L4" s="104">
         <f t="shared" si="0"/>
         <v>41061</v>
       </c>
-      <c r="M4" s="118" t="str">
+      <c r="M4" s="105" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N4" s="118" t="str">
+      <c r="N4" s="105" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="O4" s="113" t="str">
+      <c r="O4" s="104" t="str">
         <f>IF(MONTH(O6)&lt;&gt;MONTH(N6),O6,"")</f>
         <v/>
       </c>
-      <c r="P4" s="113" t="str">
+      <c r="P4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q4" s="113" t="str">
+      <c r="Q4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R4" s="113" t="str">
+      <c r="R4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S4" s="113" t="str">
+      <c r="S4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="T4" s="113" t="str">
+      <c r="T4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="U4" s="113" t="str">
+      <c r="U4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V4" s="113" t="str">
+      <c r="V4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="W4" s="113" t="str">
+      <c r="W4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="X4" s="113" t="str">
+      <c r="X4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Y4" s="113" t="str">
+      <c r="Y4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Z4" s="113" t="str">
+      <c r="Z4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AA4" s="113" t="str">
+      <c r="AA4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AB4" s="113" t="str">
+      <c r="AB4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AC4" s="113" t="str">
+      <c r="AC4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AD4" s="113" t="str">
+      <c r="AD4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE4" s="113" t="str">
+      <c r="AE4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AF4" s="113" t="str">
+      <c r="AF4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AG4" s="113">
+      <c r="AG4" s="104">
         <f t="shared" si="0"/>
         <v>41092</v>
       </c>
-      <c r="AH4" s="113" t="str">
+      <c r="AH4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AI4" s="113" t="str">
+      <c r="AI4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AJ4" s="113" t="str">
+      <c r="AJ4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AK4" s="113" t="str">
+      <c r="AK4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AL4" s="113" t="str">
+      <c r="AL4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AM4" s="113" t="str">
+      <c r="AM4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AN4" s="113" t="str">
+      <c r="AN4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AO4" s="113" t="str">
+      <c r="AO4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AP4" s="113" t="str">
+      <c r="AP4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AQ4" s="113" t="str">
+      <c r="AQ4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AR4" s="113" t="str">
+      <c r="AR4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AS4" s="113" t="str">
+      <c r="AS4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AT4" s="113" t="str">
+      <c r="AT4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AU4" s="113" t="str">
+      <c r="AU4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AV4" s="113" t="str">
+      <c r="AV4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AW4" s="113" t="str">
+      <c r="AW4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AX4" s="113" t="str">
+      <c r="AX4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AY4" s="113" t="str">
+      <c r="AY4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AZ4" s="113" t="str">
+      <c r="AZ4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BA4" s="113" t="str">
+      <c r="BA4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BB4" s="113" t="str">
+      <c r="BB4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BC4" s="113">
+      <c r="BC4" s="104">
         <f t="shared" si="0"/>
         <v>41122</v>
       </c>
-      <c r="BD4" s="113" t="str">
+      <c r="BD4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BE4" s="113" t="str">
+      <c r="BE4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BF4" s="113" t="str">
+      <c r="BF4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BG4" s="113" t="str">
+      <c r="BG4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BH4" s="113" t="str">
+      <c r="BH4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BI4" s="113" t="str">
+      <c r="BI4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BJ4" s="113" t="str">
+      <c r="BJ4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BK4" s="113" t="str">
+      <c r="BK4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BL4" s="113" t="str">
+      <c r="BL4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BM4" s="113" t="str">
+      <c r="BM4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BN4" s="113" t="str">
+      <c r="BN4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BO4" s="113" t="str">
+      <c r="BO4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BP4" s="113" t="str">
+      <c r="BP4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BQ4" s="113" t="str">
+      <c r="BQ4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BR4" s="113" t="str">
+      <c r="BR4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BS4" s="113" t="str">
+      <c r="BS4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BT4" s="113" t="str">
+      <c r="BT4" s="104" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BU4" s="113" t="str">
+      <c r="BU4" s="104" t="str">
         <f t="shared" ref="BU4:CS4" si="1">IF(MONTH(BU6)&lt;&gt;MONTH(BT6),BU6,"")</f>
         <v/>
       </c>
-      <c r="BV4" s="113" t="str">
+      <c r="BV4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BW4" s="113" t="str">
+      <c r="BW4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BX4" s="113" t="str">
+      <c r="BX4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BY4" s="113" t="str">
+      <c r="BY4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BZ4" s="113">
+      <c r="BZ4" s="104">
         <f t="shared" si="1"/>
         <v>41155</v>
       </c>
-      <c r="CA4" s="113" t="str">
+      <c r="CA4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CB4" s="113" t="str">
+      <c r="CB4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CC4" s="113" t="str">
+      <c r="CC4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CD4" s="113" t="str">
+      <c r="CD4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CE4" s="113" t="str">
+      <c r="CE4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CF4" s="113" t="str">
+      <c r="CF4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CG4" s="113" t="str">
+      <c r="CG4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CH4" s="113" t="str">
+      <c r="CH4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CI4" s="113" t="str">
+      <c r="CI4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CJ4" s="113" t="str">
+      <c r="CJ4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CK4" s="113" t="str">
+      <c r="CK4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CL4" s="113" t="str">
+      <c r="CL4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CM4" s="113" t="str">
+      <c r="CM4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CN4" s="113" t="str">
+      <c r="CN4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CO4" s="113" t="str">
+      <c r="CO4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CP4" s="113" t="str">
+      <c r="CP4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CQ4" s="113" t="str">
+      <c r="CQ4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CR4" s="113" t="str">
+      <c r="CR4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CS4" s="113" t="str">
+      <c r="CS4" s="104" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5584,107 +5591,107 @@
     </row>
     <row r="5" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="110"/>
-      <c r="C5" s="110"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
       <c r="D5" s="14"/>
       <c r="E5" s="15"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="113"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="113"/>
-      <c r="K5" s="113"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="119"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="113"/>
-      <c r="P5" s="113"/>
-      <c r="Q5" s="113"/>
-      <c r="R5" s="113"/>
-      <c r="S5" s="113"/>
-      <c r="T5" s="113"/>
-      <c r="U5" s="113"/>
-      <c r="V5" s="113"/>
-      <c r="W5" s="113"/>
-      <c r="X5" s="113"/>
-      <c r="Y5" s="113"/>
-      <c r="Z5" s="113"/>
-      <c r="AA5" s="113"/>
-      <c r="AB5" s="113"/>
-      <c r="AC5" s="113"/>
-      <c r="AD5" s="113"/>
-      <c r="AE5" s="113"/>
-      <c r="AF5" s="113"/>
-      <c r="AG5" s="113"/>
-      <c r="AH5" s="113"/>
-      <c r="AI5" s="113"/>
-      <c r="AJ5" s="113"/>
-      <c r="AK5" s="113"/>
-      <c r="AL5" s="113"/>
-      <c r="AM5" s="113"/>
-      <c r="AN5" s="113"/>
-      <c r="AO5" s="113"/>
-      <c r="AP5" s="113"/>
-      <c r="AQ5" s="113"/>
-      <c r="AR5" s="113"/>
-      <c r="AS5" s="113"/>
-      <c r="AT5" s="113"/>
-      <c r="AU5" s="113"/>
-      <c r="AV5" s="113"/>
-      <c r="AW5" s="113"/>
-      <c r="AX5" s="113"/>
-      <c r="AY5" s="113"/>
-      <c r="AZ5" s="113"/>
-      <c r="BA5" s="113"/>
-      <c r="BB5" s="113"/>
-      <c r="BC5" s="113"/>
-      <c r="BD5" s="113"/>
-      <c r="BE5" s="113"/>
-      <c r="BF5" s="113"/>
-      <c r="BG5" s="113"/>
-      <c r="BH5" s="113"/>
-      <c r="BI5" s="113"/>
-      <c r="BJ5" s="113"/>
-      <c r="BK5" s="113"/>
-      <c r="BL5" s="113"/>
-      <c r="BM5" s="113"/>
-      <c r="BN5" s="113"/>
-      <c r="BO5" s="113"/>
-      <c r="BP5" s="113"/>
-      <c r="BQ5" s="113"/>
-      <c r="BR5" s="113"/>
-      <c r="BS5" s="113"/>
-      <c r="BT5" s="113"/>
-      <c r="BU5" s="113"/>
-      <c r="BV5" s="113"/>
-      <c r="BW5" s="113"/>
-      <c r="BX5" s="113"/>
-      <c r="BY5" s="113"/>
-      <c r="BZ5" s="113"/>
-      <c r="CA5" s="113"/>
-      <c r="CB5" s="113"/>
-      <c r="CC5" s="113"/>
-      <c r="CD5" s="113"/>
-      <c r="CE5" s="113"/>
-      <c r="CF5" s="113"/>
-      <c r="CG5" s="113"/>
-      <c r="CH5" s="113"/>
-      <c r="CI5" s="113"/>
-      <c r="CJ5" s="113"/>
-      <c r="CK5" s="113"/>
-      <c r="CL5" s="113"/>
-      <c r="CM5" s="113"/>
-      <c r="CN5" s="113"/>
-      <c r="CO5" s="113"/>
-      <c r="CP5" s="113"/>
-      <c r="CQ5" s="113"/>
-      <c r="CR5" s="113"/>
-      <c r="CS5" s="113"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="104"/>
+      <c r="P5" s="104"/>
+      <c r="Q5" s="104"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="104"/>
+      <c r="V5" s="104"/>
+      <c r="W5" s="104"/>
+      <c r="X5" s="104"/>
+      <c r="Y5" s="104"/>
+      <c r="Z5" s="104"/>
+      <c r="AA5" s="104"/>
+      <c r="AB5" s="104"/>
+      <c r="AC5" s="104"/>
+      <c r="AD5" s="104"/>
+      <c r="AE5" s="104"/>
+      <c r="AF5" s="104"/>
+      <c r="AG5" s="104"/>
+      <c r="AH5" s="104"/>
+      <c r="AI5" s="104"/>
+      <c r="AJ5" s="104"/>
+      <c r="AK5" s="104"/>
+      <c r="AL5" s="104"/>
+      <c r="AM5" s="104"/>
+      <c r="AN5" s="104"/>
+      <c r="AO5" s="104"/>
+      <c r="AP5" s="104"/>
+      <c r="AQ5" s="104"/>
+      <c r="AR5" s="104"/>
+      <c r="AS5" s="104"/>
+      <c r="AT5" s="104"/>
+      <c r="AU5" s="104"/>
+      <c r="AV5" s="104"/>
+      <c r="AW5" s="104"/>
+      <c r="AX5" s="104"/>
+      <c r="AY5" s="104"/>
+      <c r="AZ5" s="104"/>
+      <c r="BA5" s="104"/>
+      <c r="BB5" s="104"/>
+      <c r="BC5" s="104"/>
+      <c r="BD5" s="104"/>
+      <c r="BE5" s="104"/>
+      <c r="BF5" s="104"/>
+      <c r="BG5" s="104"/>
+      <c r="BH5" s="104"/>
+      <c r="BI5" s="104"/>
+      <c r="BJ5" s="104"/>
+      <c r="BK5" s="104"/>
+      <c r="BL5" s="104"/>
+      <c r="BM5" s="104"/>
+      <c r="BN5" s="104"/>
+      <c r="BO5" s="104"/>
+      <c r="BP5" s="104"/>
+      <c r="BQ5" s="104"/>
+      <c r="BR5" s="104"/>
+      <c r="BS5" s="104"/>
+      <c r="BT5" s="104"/>
+      <c r="BU5" s="104"/>
+      <c r="BV5" s="104"/>
+      <c r="BW5" s="104"/>
+      <c r="BX5" s="104"/>
+      <c r="BY5" s="104"/>
+      <c r="BZ5" s="104"/>
+      <c r="CA5" s="104"/>
+      <c r="CB5" s="104"/>
+      <c r="CC5" s="104"/>
+      <c r="CD5" s="104"/>
+      <c r="CE5" s="104"/>
+      <c r="CF5" s="104"/>
+      <c r="CG5" s="104"/>
+      <c r="CH5" s="104"/>
+      <c r="CI5" s="104"/>
+      <c r="CJ5" s="104"/>
+      <c r="CK5" s="104"/>
+      <c r="CL5" s="104"/>
+      <c r="CM5" s="104"/>
+      <c r="CN5" s="104"/>
+      <c r="CO5" s="104"/>
+      <c r="CP5" s="104"/>
+      <c r="CQ5" s="104"/>
+      <c r="CR5" s="104"/>
+      <c r="CS5" s="104"/>
       <c r="CT5" s="12"/>
     </row>
     <row r="6" spans="1:98" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="110"/>
-      <c r="C6" s="110"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15"/>
       <c r="F6" s="29"/>
@@ -6052,8 +6059,8 @@
     </row>
     <row r="7" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="110"/>
-      <c r="C7" s="110"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
       <c r="H7" s="112"/>
@@ -6157,18 +6164,18 @@
         <v>1</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:98" x14ac:dyDescent="0.25">
-      <c r="A10" s="105" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="106"/>
-      <c r="C10" s="106"/>
+      <c r="A10" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="114"/>
+      <c r="C10" s="114"/>
       <c r="D10" s="35">
         <f ca="1">MIN(D11:D18)</f>
-        <v>41058</v>
+        <v>41066</v>
       </c>
       <c r="E10" s="35">
         <f ca="1">MAX(E11:E18)</f>
@@ -6215,9 +6222,9 @@
       <c r="AS10" s="4"/>
       <c r="AT10" s="4"/>
       <c r="AU10" s="4"/>
-      <c r="AV10" s="87"/>
-      <c r="AW10" s="87"/>
-      <c r="AX10" s="87"/>
+      <c r="AV10" s="86"/>
+      <c r="AW10" s="86"/>
+      <c r="AX10" s="86"/>
       <c r="AY10" s="4"/>
       <c r="AZ10" s="4"/>
       <c r="BA10" s="4"/>
@@ -6268,11 +6275,11 @@
     </row>
     <row r="11" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="44"/>
+      <c r="D11" s="43"/>
       <c r="E11" s="21"/>
       <c r="F11" s="27">
         <v>0.8</v>
@@ -6317,9 +6324,9 @@
       <c r="AS11" s="10"/>
       <c r="AT11" s="10"/>
       <c r="AU11" s="10"/>
-      <c r="AV11" s="88"/>
-      <c r="AW11" s="88"/>
-      <c r="AX11" s="88"/>
+      <c r="AV11" s="87"/>
+      <c r="AW11" s="87"/>
+      <c r="AX11" s="87"/>
       <c r="AY11" s="10"/>
       <c r="AZ11" s="10"/>
       <c r="BA11" s="10"/>
@@ -6371,16 +6378,16 @@
     <row r="12" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="14">
         <f ca="1">TODAY()</f>
-        <v>41058</v>
+        <v>41066</v>
       </c>
       <c r="E12" s="21">
         <f ca="1">D12+5+CHOOSE(WEEKDAY(D12+5,2),0,0,0,0,0,2,1)</f>
-        <v>41064</v>
+        <v>41071</v>
       </c>
       <c r="F12" s="37">
         <v>0.6</v>
@@ -6425,9 +6432,9 @@
       <c r="AS12" s="10"/>
       <c r="AT12" s="10"/>
       <c r="AU12" s="10"/>
-      <c r="AV12" s="88"/>
-      <c r="AW12" s="88"/>
-      <c r="AX12" s="88"/>
+      <c r="AV12" s="87"/>
+      <c r="AW12" s="87"/>
+      <c r="AX12" s="87"/>
       <c r="AY12" s="10"/>
       <c r="AZ12" s="10"/>
       <c r="BA12" s="10"/>
@@ -6479,16 +6486,16 @@
     <row r="13" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="14">
         <f ca="1">E12+1</f>
-        <v>41065</v>
+        <v>41072</v>
       </c>
       <c r="E13" s="21">
         <f ca="1">D13+6+CHOOSE(WEEKDAY(D13+5,2),0,0,0,0,0,2,1)</f>
-        <v>41072</v>
+        <v>41079</v>
       </c>
       <c r="F13" s="37"/>
       <c r="H13" s="10"/>
@@ -6531,9 +6538,9 @@
       <c r="AS13" s="10"/>
       <c r="AT13" s="10"/>
       <c r="AU13" s="10"/>
-      <c r="AV13" s="88"/>
-      <c r="AW13" s="88"/>
-      <c r="AX13" s="88"/>
+      <c r="AV13" s="87"/>
+      <c r="AW13" s="87"/>
+      <c r="AX13" s="87"/>
       <c r="AY13" s="10"/>
       <c r="AZ13" s="10"/>
       <c r="BA13" s="10"/>
@@ -6585,16 +6592,16 @@
     <row r="14" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="14">
         <f ca="1">E13</f>
-        <v>41072</v>
+        <v>41079</v>
       </c>
       <c r="E14" s="21">
         <f ca="1">D14+3</f>
-        <v>41075</v>
+        <v>41082</v>
       </c>
       <c r="F14" s="37"/>
       <c r="H14" s="10"/>
@@ -6637,9 +6644,9 @@
       <c r="AS14" s="10"/>
       <c r="AT14" s="10"/>
       <c r="AU14" s="10"/>
-      <c r="AV14" s="88"/>
-      <c r="AW14" s="88"/>
-      <c r="AX14" s="88"/>
+      <c r="AV14" s="87"/>
+      <c r="AW14" s="87"/>
+      <c r="AX14" s="87"/>
       <c r="AY14" s="10"/>
       <c r="AZ14" s="10"/>
       <c r="BA14" s="10"/>
@@ -6690,7 +6697,7 @@
     </row>
     <row r="15" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -6713,9 +6720,9 @@
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="V15" s="10"/>
-      <c r="W15" s="50"/>
-      <c r="X15" s="50"/>
-      <c r="Y15" s="50"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="49"/>
+      <c r="Y15" s="49"/>
       <c r="Z15" s="10"/>
       <c r="AA15" s="10"/>
       <c r="AB15" s="10"/>
@@ -6738,9 +6745,9 @@
       <c r="AS15" s="10"/>
       <c r="AT15" s="10"/>
       <c r="AU15" s="10"/>
-      <c r="AV15" s="88"/>
-      <c r="AW15" s="88"/>
-      <c r="AX15" s="88"/>
+      <c r="AV15" s="87"/>
+      <c r="AW15" s="87"/>
+      <c r="AX15" s="87"/>
       <c r="AY15" s="10"/>
       <c r="AZ15" s="10"/>
       <c r="BA15" s="10"/>
@@ -6792,7 +6799,7 @@
     <row r="16" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="14">
@@ -6813,9 +6820,9 @@
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="V16" s="10"/>
-      <c r="W16" s="49"/>
-      <c r="X16" s="49"/>
-      <c r="Y16" s="50"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="49"/>
       <c r="Z16" s="10"/>
       <c r="AA16" s="10"/>
       <c r="AB16" s="10"/>
@@ -6838,9 +6845,9 @@
       <c r="AS16" s="10"/>
       <c r="AT16" s="10"/>
       <c r="AU16" s="10"/>
-      <c r="AV16" s="88"/>
-      <c r="AW16" s="88"/>
-      <c r="AX16" s="88"/>
+      <c r="AV16" s="87"/>
+      <c r="AW16" s="87"/>
+      <c r="AX16" s="87"/>
       <c r="AY16" s="10"/>
       <c r="AZ16" s="10"/>
       <c r="BA16" s="10"/>
@@ -6890,11 +6897,11 @@
       <c r="CS16" s="10"/>
     </row>
     <row r="17" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
+      <c r="A17" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="14">
         <f>E16+1</f>
         <v>41081</v>
@@ -6919,16 +6926,16 @@
       <c r="R17" s="10"/>
       <c r="S17" s="10"/>
       <c r="T17" s="10"/>
-      <c r="Z17" s="48"/>
-      <c r="AA17" s="48"/>
-      <c r="AB17" s="48"/>
-      <c r="AC17" s="48"/>
-      <c r="AD17" s="48"/>
-      <c r="AE17" s="48"/>
-      <c r="AF17" s="48"/>
-      <c r="AG17" s="48"/>
-      <c r="AH17" s="48"/>
-      <c r="AI17" s="46"/>
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="47"/>
+      <c r="AD17" s="47"/>
+      <c r="AE17" s="47"/>
+      <c r="AF17" s="47"/>
+      <c r="AG17" s="47"/>
+      <c r="AH17" s="47"/>
+      <c r="AI17" s="45"/>
       <c r="AJ17" s="10"/>
       <c r="AK17" s="10"/>
       <c r="AL17" s="10"/>
@@ -6941,9 +6948,9 @@
       <c r="AS17" s="10"/>
       <c r="AT17" s="10"/>
       <c r="AU17" s="10"/>
-      <c r="AV17" s="88"/>
-      <c r="AW17" s="88"/>
-      <c r="AX17" s="88"/>
+      <c r="AV17" s="87"/>
+      <c r="AW17" s="87"/>
+      <c r="AX17" s="87"/>
       <c r="AY17" s="10"/>
       <c r="AZ17" s="10"/>
       <c r="BA17" s="10"/>
@@ -7039,9 +7046,9 @@
       <c r="AS18" s="10"/>
       <c r="AT18" s="10"/>
       <c r="AU18" s="10"/>
-      <c r="AV18" s="88"/>
-      <c r="AW18" s="88"/>
-      <c r="AX18" s="88"/>
+      <c r="AV18" s="87"/>
+      <c r="AW18" s="87"/>
+      <c r="AX18" s="87"/>
       <c r="AY18" s="10"/>
       <c r="AZ18" s="10"/>
       <c r="BA18" s="10"/>
@@ -7137,9 +7144,9 @@
       <c r="AS19" s="3"/>
       <c r="AT19" s="3"/>
       <c r="AU19" s="3"/>
-      <c r="AV19" s="89"/>
-      <c r="AW19" s="89"/>
-      <c r="AX19" s="89"/>
+      <c r="AV19" s="88"/>
+      <c r="AW19" s="88"/>
+      <c r="AX19" s="88"/>
       <c r="AY19" s="3"/>
       <c r="AZ19" s="3"/>
       <c r="BA19" s="3"/>
@@ -7189,18 +7196,18 @@
       <c r="CS19" s="3"/>
     </row>
     <row r="20" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A20" s="105" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="106"/>
-      <c r="C20" s="106"/>
+      <c r="A20" s="113" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="114"/>
+      <c r="C20" s="114"/>
       <c r="D20" s="35">
         <f>MIN(D21:D28)</f>
         <v>41095</v>
       </c>
       <c r="E20" s="35">
         <f>MAX(E21:E28)</f>
-        <v>41137</v>
+        <v>41124</v>
       </c>
       <c r="F20" s="38"/>
       <c r="H20" s="11"/>
@@ -7225,8 +7232,8 @@
       <c r="AA20" s="11"/>
       <c r="AB20" s="11"/>
       <c r="AC20" s="11"/>
-      <c r="AD20" s="47"/>
-      <c r="AE20" s="47"/>
+      <c r="AD20" s="46"/>
+      <c r="AE20" s="46"/>
       <c r="AF20" s="11"/>
       <c r="AG20" s="11"/>
       <c r="AH20" s="11"/>
@@ -7243,9 +7250,9 @@
       <c r="AS20" s="11"/>
       <c r="AT20" s="11"/>
       <c r="AU20" s="11"/>
-      <c r="AV20" s="90"/>
-      <c r="AW20" s="90"/>
-      <c r="AX20" s="90"/>
+      <c r="AV20" s="89"/>
+      <c r="AW20" s="89"/>
+      <c r="AX20" s="89"/>
       <c r="AY20" s="11"/>
       <c r="AZ20" s="11"/>
       <c r="BA20" s="11"/>
@@ -7296,7 +7303,7 @@
     </row>
     <row r="21" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="23">
@@ -7305,7 +7312,7 @@
       </c>
       <c r="E21" s="24">
         <f>D21+Versioning!E3+1</f>
-        <v>41101</v>
+        <v>41096</v>
       </c>
       <c r="F21" s="30">
         <v>0.25</v>
@@ -7332,11 +7339,11 @@
       <c r="AA21" s="10"/>
       <c r="AB21" s="10"/>
       <c r="AC21" s="10"/>
-      <c r="AJ21" s="50"/>
-      <c r="AK21" s="50"/>
-      <c r="AL21" s="50"/>
-      <c r="AM21" s="50"/>
-      <c r="AN21" s="51"/>
+      <c r="AJ21" s="49"/>
+      <c r="AK21" s="49"/>
+      <c r="AL21" s="49"/>
+      <c r="AM21" s="49"/>
+      <c r="AN21" s="50"/>
       <c r="AO21" s="10"/>
       <c r="AP21" s="10"/>
       <c r="AQ21" s="10"/>
@@ -7344,9 +7351,9 @@
       <c r="AS21" s="10"/>
       <c r="AT21" s="10"/>
       <c r="AU21" s="10"/>
-      <c r="AV21" s="88"/>
-      <c r="AW21" s="88"/>
-      <c r="AX21" s="88"/>
+      <c r="AV21" s="87"/>
+      <c r="AW21" s="87"/>
+      <c r="AX21" s="87"/>
       <c r="AY21" s="10"/>
       <c r="AZ21" s="10"/>
       <c r="BA21" s="10"/>
@@ -7398,16 +7405,16 @@
     <row r="22" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="23">
         <f>E21</f>
-        <v>41101</v>
+        <v>41096</v>
       </c>
       <c r="E22" s="24">
         <f>D22+2++CHOOSE(WEEKDAY(D22+2,2),0,0,0,0,0,2,1)</f>
-        <v>41103</v>
+        <v>41099</v>
       </c>
       <c r="F22" s="30"/>
       <c r="H22" s="10"/>
@@ -7433,20 +7440,20 @@
       <c r="AB22" s="10"/>
       <c r="AC22" s="10"/>
       <c r="AJ22" s="10"/>
-      <c r="AK22" s="71"/>
-      <c r="AL22" s="71"/>
-      <c r="AM22" s="78"/>
-      <c r="AN22" s="58"/>
-      <c r="AO22" s="55"/>
-      <c r="AP22" s="53"/>
-      <c r="AQ22" s="71"/>
-      <c r="AR22" s="71"/>
-      <c r="AS22" s="65"/>
-      <c r="AT22" s="61"/>
-      <c r="AU22" s="62"/>
-      <c r="AV22" s="92"/>
-      <c r="AW22" s="92"/>
-      <c r="AX22" s="88"/>
+      <c r="AK22" s="70"/>
+      <c r="AL22" s="70"/>
+      <c r="AM22" s="77"/>
+      <c r="AN22" s="57"/>
+      <c r="AO22" s="54"/>
+      <c r="AP22" s="52"/>
+      <c r="AQ22" s="70"/>
+      <c r="AR22" s="70"/>
+      <c r="AS22" s="64"/>
+      <c r="AT22" s="60"/>
+      <c r="AU22" s="61"/>
+      <c r="AV22" s="91"/>
+      <c r="AW22" s="91"/>
+      <c r="AX22" s="87"/>
       <c r="AY22" s="10"/>
       <c r="AZ22" s="10"/>
       <c r="BA22" s="10"/>
@@ -7497,16 +7504,16 @@
     </row>
     <row r="23" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="14">
         <f>E22+1+CHOOSE(WEEKDAY(E22+1,2),0,0,0,0,0,2,1)</f>
-        <v>41106</v>
+        <v>41100</v>
       </c>
       <c r="E23" s="24">
         <f>D23+Versioning!E4-1</f>
-        <v>41110</v>
+        <v>41099</v>
       </c>
       <c r="F23" s="30">
         <v>0.4</v>
@@ -7537,32 +7544,32 @@
       <c r="AE23" s="10"/>
       <c r="AF23" s="10"/>
       <c r="AG23" s="10"/>
-      <c r="AI23" s="49"/>
-      <c r="AJ23" s="52"/>
-      <c r="AK23" s="52"/>
-      <c r="AL23" s="52"/>
-      <c r="AM23" s="57"/>
-      <c r="AN23" s="54"/>
-      <c r="AO23" s="56"/>
-      <c r="AP23" s="76"/>
-      <c r="AQ23" s="77"/>
-      <c r="AR23" s="77"/>
-      <c r="AS23" s="73"/>
-      <c r="AT23" s="55"/>
-      <c r="AU23" s="53"/>
-      <c r="AV23" s="91"/>
-      <c r="AW23" s="91"/>
-      <c r="AX23" s="97"/>
-      <c r="AY23" s="62"/>
-      <c r="AZ23" s="71"/>
-      <c r="BA23" s="71"/>
-      <c r="BB23" s="71"/>
-      <c r="BC23" s="71"/>
-      <c r="BD23" s="71"/>
-      <c r="BE23" s="71"/>
-      <c r="BF23" s="71"/>
-      <c r="BG23" s="71"/>
-      <c r="BH23" s="71"/>
+      <c r="AI23" s="48"/>
+      <c r="AJ23" s="51"/>
+      <c r="AK23" s="51"/>
+      <c r="AL23" s="51"/>
+      <c r="AM23" s="56"/>
+      <c r="AN23" s="53"/>
+      <c r="AO23" s="55"/>
+      <c r="AP23" s="75"/>
+      <c r="AQ23" s="76"/>
+      <c r="AR23" s="76"/>
+      <c r="AS23" s="72"/>
+      <c r="AT23" s="54"/>
+      <c r="AU23" s="52"/>
+      <c r="AV23" s="90"/>
+      <c r="AW23" s="90"/>
+      <c r="AX23" s="96"/>
+      <c r="AY23" s="61"/>
+      <c r="AZ23" s="70"/>
+      <c r="BA23" s="70"/>
+      <c r="BB23" s="70"/>
+      <c r="BC23" s="70"/>
+      <c r="BD23" s="70"/>
+      <c r="BE23" s="70"/>
+      <c r="BF23" s="70"/>
+      <c r="BG23" s="70"/>
+      <c r="BH23" s="70"/>
       <c r="BI23" s="10"/>
       <c r="BJ23" s="10"/>
       <c r="BK23" s="10"/>
@@ -7604,7 +7611,7 @@
     <row r="24" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="14">
@@ -7642,27 +7649,27 @@
       <c r="AF24" s="10"/>
       <c r="AG24" s="10"/>
       <c r="AI24" s="10"/>
-      <c r="AJ24" s="52"/>
-      <c r="AK24" s="52"/>
-      <c r="AL24" s="52"/>
-      <c r="AM24" s="52"/>
+      <c r="AJ24" s="51"/>
+      <c r="AK24" s="51"/>
+      <c r="AL24" s="51"/>
+      <c r="AM24" s="51"/>
       <c r="AN24" s="10"/>
       <c r="AO24" s="10"/>
       <c r="AP24" s="10"/>
       <c r="AQ24" s="10"/>
       <c r="AR24" s="10"/>
       <c r="AS24" s="10"/>
-      <c r="AT24" s="75"/>
-      <c r="AU24" s="64"/>
-      <c r="AV24" s="93"/>
-      <c r="AW24" s="94"/>
-      <c r="AX24" s="98"/>
-      <c r="AY24" s="73"/>
-      <c r="AZ24" s="66"/>
-      <c r="BA24" s="104"/>
-      <c r="BB24" s="70"/>
-      <c r="BC24" s="63"/>
-      <c r="BD24" s="67"/>
+      <c r="AT24" s="74"/>
+      <c r="AU24" s="63"/>
+      <c r="AV24" s="92"/>
+      <c r="AW24" s="93"/>
+      <c r="AX24" s="97"/>
+      <c r="AY24" s="72"/>
+      <c r="AZ24" s="65"/>
+      <c r="BA24" s="103"/>
+      <c r="BB24" s="69"/>
+      <c r="BC24" s="62"/>
+      <c r="BD24" s="66"/>
       <c r="BF24" s="10"/>
       <c r="BG24" s="10"/>
       <c r="BH24" s="10"/>
@@ -7706,7 +7713,7 @@
     </row>
     <row r="25" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="14">
@@ -7715,7 +7722,7 @@
       </c>
       <c r="E25" s="24">
         <f>D25+Versioning!E5+CHOOSE(WEEKDAY(D25+Versioning!E5,2),0,0,0,0,0,2,1)</f>
-        <v>41127</v>
+        <v>41121</v>
       </c>
       <c r="F25" s="31"/>
       <c r="H25" s="10"/>
@@ -7750,25 +7757,25 @@
       <c r="AK25" s="10"/>
       <c r="AL25" s="10"/>
       <c r="AM25" s="10"/>
-      <c r="AN25" s="52"/>
-      <c r="AO25" s="52"/>
-      <c r="AP25" s="52"/>
-      <c r="AQ25" s="52"/>
-      <c r="AR25" s="52"/>
-      <c r="AS25" s="74"/>
-      <c r="AT25" s="99"/>
-      <c r="AU25" s="60"/>
-      <c r="AV25" s="93"/>
-      <c r="AW25" s="95"/>
-      <c r="AX25" s="93"/>
-      <c r="BA25" s="80"/>
-      <c r="BB25" s="103"/>
-      <c r="BC25" s="102"/>
-      <c r="BD25" s="100"/>
-      <c r="BE25" s="100"/>
-      <c r="BF25" s="96"/>
-      <c r="BG25" s="71"/>
-      <c r="BH25" s="71"/>
+      <c r="AN25" s="51"/>
+      <c r="AO25" s="51"/>
+      <c r="AP25" s="51"/>
+      <c r="AQ25" s="51"/>
+      <c r="AR25" s="51"/>
+      <c r="AS25" s="73"/>
+      <c r="AT25" s="98"/>
+      <c r="AU25" s="59"/>
+      <c r="AV25" s="92"/>
+      <c r="AW25" s="94"/>
+      <c r="AX25" s="92"/>
+      <c r="BA25" s="79"/>
+      <c r="BB25" s="102"/>
+      <c r="BC25" s="101"/>
+      <c r="BD25" s="99"/>
+      <c r="BE25" s="99"/>
+      <c r="BF25" s="95"/>
+      <c r="BG25" s="70"/>
+      <c r="BH25" s="70"/>
       <c r="BI25" s="10"/>
       <c r="BJ25" s="10"/>
       <c r="BK25" s="10"/>
@@ -7810,16 +7817,16 @@
     <row r="26" spans="1:97" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="14">
         <f>E25</f>
-        <v>41127</v>
+        <v>41121</v>
       </c>
       <c r="E26" s="24">
         <f>D26+2+CHOOSE(WEEKDAY(D26+3,2),0,0,0,0,0,2,1)</f>
-        <v>41129</v>
+        <v>41123</v>
       </c>
       <c r="F26" s="31"/>
       <c r="H26" s="10"/>
@@ -7854,29 +7861,29 @@
       <c r="AK26" s="10"/>
       <c r="AL26" s="10"/>
       <c r="AM26" s="10"/>
-      <c r="AN26" s="52"/>
-      <c r="AO26" s="52"/>
-      <c r="AP26" s="52"/>
-      <c r="AQ26" s="52"/>
-      <c r="AR26" s="52"/>
+      <c r="AN26" s="51"/>
+      <c r="AO26" s="51"/>
+      <c r="AP26" s="51"/>
+      <c r="AQ26" s="51"/>
+      <c r="AR26" s="51"/>
       <c r="AS26" s="10"/>
-      <c r="AT26" s="72"/>
-      <c r="AU26" s="65"/>
-      <c r="AV26" s="95"/>
-      <c r="AW26" s="94"/>
-      <c r="AX26" s="94"/>
-      <c r="AY26" s="68"/>
-      <c r="AZ26" s="69"/>
-      <c r="BB26" s="80"/>
-      <c r="BC26" s="101"/>
-      <c r="BD26" s="101"/>
-      <c r="BE26" s="69"/>
+      <c r="AT26" s="71"/>
+      <c r="AU26" s="64"/>
+      <c r="AV26" s="94"/>
+      <c r="AW26" s="93"/>
+      <c r="AX26" s="93"/>
+      <c r="AY26" s="67"/>
+      <c r="AZ26" s="68"/>
+      <c r="BB26" s="79"/>
+      <c r="BC26" s="100"/>
+      <c r="BD26" s="100"/>
+      <c r="BE26" s="68"/>
       <c r="BF26" s="10"/>
-      <c r="BG26" s="55"/>
-      <c r="BH26" s="53"/>
-      <c r="BI26" s="70"/>
-      <c r="BJ26" s="70"/>
-      <c r="BK26" s="67"/>
+      <c r="BG26" s="54"/>
+      <c r="BH26" s="52"/>
+      <c r="BI26" s="69"/>
+      <c r="BJ26" s="69"/>
+      <c r="BK26" s="66"/>
       <c r="BL26" s="10"/>
       <c r="BM26" s="10"/>
       <c r="BN26" s="10"/>
@@ -7914,15 +7921,15 @@
     </row>
     <row r="27" spans="1:97" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D27" s="14">
         <f>E26+1</f>
-        <v>41130</v>
+        <v>41124</v>
       </c>
       <c r="E27" s="24">
         <f>D27+Versioning!E6+CHOOSE(WEEKDAY(D27+Versioning!E6,2),0,0,0,0,0,2,1)</f>
-        <v>41137</v>
+        <v>41124</v>
       </c>
       <c r="F27" s="31">
         <v>0</v>
@@ -7966,22 +7973,22 @@
       <c r="AS27" s="10"/>
       <c r="AT27" s="10"/>
       <c r="AU27" s="10"/>
-      <c r="AV27" s="95"/>
-      <c r="AW27" s="94"/>
-      <c r="AX27" s="88"/>
+      <c r="AV27" s="94"/>
+      <c r="AW27" s="93"/>
+      <c r="AX27" s="87"/>
       <c r="AY27" s="10"/>
       <c r="AZ27" s="10"/>
       <c r="BA27" s="10"/>
-      <c r="BB27" s="72"/>
-      <c r="BC27" s="64"/>
-      <c r="BD27" s="71"/>
-      <c r="BE27" s="71"/>
-      <c r="BF27" s="64"/>
-      <c r="BG27" s="71"/>
-      <c r="BH27" s="62"/>
-      <c r="BI27" s="71"/>
-      <c r="BJ27" s="71"/>
-      <c r="BK27" s="65"/>
+      <c r="BB27" s="71"/>
+      <c r="BC27" s="63"/>
+      <c r="BD27" s="70"/>
+      <c r="BE27" s="70"/>
+      <c r="BF27" s="63"/>
+      <c r="BG27" s="70"/>
+      <c r="BH27" s="61"/>
+      <c r="BI27" s="70"/>
+      <c r="BJ27" s="70"/>
+      <c r="BK27" s="64"/>
       <c r="BL27" s="10"/>
       <c r="BM27" s="10"/>
       <c r="BN27" s="10"/>
@@ -8064,14 +8071,14 @@
       <c r="AS28" s="10"/>
       <c r="AT28" s="10"/>
       <c r="AU28" s="10"/>
-      <c r="AV28" s="88"/>
-      <c r="AW28" s="88"/>
-      <c r="AX28" s="88"/>
+      <c r="AV28" s="87"/>
+      <c r="AW28" s="87"/>
+      <c r="AX28" s="87"/>
       <c r="AY28" s="10"/>
       <c r="AZ28" s="10"/>
       <c r="BA28" s="10"/>
-      <c r="BB28" s="75"/>
-      <c r="BC28" s="59"/>
+      <c r="BB28" s="74"/>
+      <c r="BC28" s="58"/>
       <c r="BD28" s="10"/>
       <c r="BE28" s="10"/>
       <c r="BF28" s="10"/>
@@ -8168,8 +8175,8 @@
       <c r="AY29" s="2"/>
       <c r="AZ29" s="2"/>
       <c r="BA29" s="2"/>
-      <c r="BB29" s="79"/>
-      <c r="BC29" s="80"/>
+      <c r="BB29" s="78"/>
+      <c r="BC29" s="79"/>
       <c r="BD29" s="2"/>
       <c r="BE29" s="2"/>
       <c r="BF29" s="2"/>
@@ -8214,18 +8221,18 @@
       <c r="CS29" s="2"/>
     </row>
     <row r="30" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="105" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="106"/>
-      <c r="C30" s="106"/>
+      <c r="A30" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="114"/>
+      <c r="C30" s="114"/>
       <c r="D30" s="35">
         <f>MIN(D31:D34)</f>
-        <v>41138</v>
+        <v>41125</v>
       </c>
       <c r="E30" s="35">
         <f>MAX(E31:E34)</f>
-        <v>41166</v>
+        <v>41155</v>
       </c>
       <c r="F30" s="38"/>
       <c r="H30" s="4"/>
@@ -8274,8 +8281,8 @@
       <c r="AY30" s="4"/>
       <c r="AZ30" s="4"/>
       <c r="BA30" s="4"/>
-      <c r="BB30" s="81"/>
-      <c r="BC30" s="82"/>
+      <c r="BB30" s="80"/>
+      <c r="BC30" s="81"/>
       <c r="BD30" s="4"/>
       <c r="BE30" s="4"/>
       <c r="BF30" s="4"/>
@@ -8322,16 +8329,16 @@
     <row r="31" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="23">
         <f>E27+1</f>
-        <v>41138</v>
+        <v>41125</v>
       </c>
       <c r="E31" s="24">
         <f>D31+7+CHOOSE(WEEKDAY(D31+7,2),0,0,0,0,0,2,1)</f>
-        <v>41145</v>
+        <v>41134</v>
       </c>
       <c r="F31" s="32">
         <v>0</v>
@@ -8382,8 +8389,8 @@
       <c r="AY31" s="10"/>
       <c r="AZ31" s="10"/>
       <c r="BA31" s="10"/>
-      <c r="BB31" s="75"/>
-      <c r="BC31" s="59"/>
+      <c r="BB31" s="74"/>
+      <c r="BC31" s="58"/>
       <c r="BD31" s="10"/>
       <c r="BE31" s="10"/>
       <c r="BF31" s="10"/>
@@ -8430,16 +8437,16 @@
     <row r="32" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="23">
         <f>E31+1</f>
-        <v>41146</v>
+        <v>41135</v>
       </c>
       <c r="E32" s="24">
         <f>D32+7+CHOOSE(WEEKDAY(D32+7,2),0,0,0,0,0,2,1)</f>
-        <v>41155</v>
+        <v>41142</v>
       </c>
       <c r="F32" s="30">
         <v>0</v>
@@ -8490,8 +8497,8 @@
       <c r="AY32" s="10"/>
       <c r="AZ32" s="10"/>
       <c r="BA32" s="10"/>
-      <c r="BB32" s="75"/>
-      <c r="BC32" s="59"/>
+      <c r="BB32" s="74"/>
+      <c r="BC32" s="58"/>
       <c r="BD32" s="10"/>
       <c r="BE32" s="10"/>
       <c r="BF32" s="10"/>
@@ -8538,16 +8545,16 @@
     <row r="33" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="23">
         <f>E32+1</f>
-        <v>41156</v>
+        <v>41143</v>
       </c>
       <c r="E33" s="24">
         <f>D33+10+CHOOSE(WEEKDAY(D33+10,2),0,0,0,0,0,2,1)</f>
-        <v>41166</v>
+        <v>41155</v>
       </c>
       <c r="F33" s="31">
         <v>0</v>
@@ -8598,8 +8605,8 @@
       <c r="AY33" s="10"/>
       <c r="AZ33" s="10"/>
       <c r="BA33" s="10"/>
-      <c r="BB33" s="75"/>
-      <c r="BC33" s="59"/>
+      <c r="BB33" s="74"/>
+      <c r="BC33" s="58"/>
       <c r="BD33" s="10"/>
       <c r="BE33" s="10"/>
       <c r="BF33" s="10"/>
@@ -8696,8 +8703,8 @@
       <c r="AY34" s="10"/>
       <c r="AZ34" s="10"/>
       <c r="BA34" s="10"/>
-      <c r="BB34" s="75"/>
-      <c r="BC34" s="59"/>
+      <c r="BB34" s="74"/>
+      <c r="BC34" s="58"/>
       <c r="BD34" s="10"/>
       <c r="BE34" s="10"/>
       <c r="BF34" s="10"/>
@@ -8748,22 +8755,22 @@
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
-      <c r="BB35" s="79"/>
-      <c r="BC35" s="80"/>
+      <c r="BB35" s="78"/>
+      <c r="BC35" s="79"/>
     </row>
     <row r="36" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="105" t="s">
+      <c r="A36" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="106"/>
-      <c r="C36" s="106"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="114"/>
       <c r="D36" s="35">
         <f>MIN(D37:D42)</f>
         <v>40308</v>
       </c>
       <c r="E36" s="35">
         <f>MAX(E37:E42)</f>
-        <v>41200</v>
+        <v>41189</v>
       </c>
       <c r="F36" s="38"/>
       <c r="H36" s="11"/>
@@ -8812,8 +8819,8 @@
       <c r="AY36" s="11"/>
       <c r="AZ36" s="11"/>
       <c r="BA36" s="11"/>
-      <c r="BB36" s="83"/>
-      <c r="BC36" s="84"/>
+      <c r="BB36" s="82"/>
+      <c r="BC36" s="83"/>
       <c r="BD36" s="11"/>
       <c r="BE36" s="11"/>
       <c r="BF36" s="11"/>
@@ -8865,11 +8872,11 @@
       <c r="C37" s="2"/>
       <c r="D37" s="23">
         <f>E33+1</f>
-        <v>41167</v>
+        <v>41156</v>
       </c>
       <c r="E37" s="24">
         <f>E38</f>
-        <v>41200</v>
+        <v>41189</v>
       </c>
       <c r="F37" s="32">
         <v>0</v>
@@ -8920,8 +8927,8 @@
       <c r="AY37" s="10"/>
       <c r="AZ37" s="10"/>
       <c r="BA37" s="10"/>
-      <c r="BB37" s="75"/>
-      <c r="BC37" s="59"/>
+      <c r="BB37" s="74"/>
+      <c r="BC37" s="58"/>
       <c r="BD37" s="10"/>
       <c r="BE37" s="10"/>
       <c r="BF37" s="10"/>
@@ -8973,11 +8980,11 @@
       </c>
       <c r="D38" s="14">
         <f>D37+13</f>
-        <v>41180</v>
+        <v>41169</v>
       </c>
       <c r="E38" s="21">
         <f>D38+20</f>
-        <v>41200</v>
+        <v>41189</v>
       </c>
       <c r="F38" s="30">
         <v>0</v>
@@ -9028,8 +9035,8 @@
       <c r="AY38" s="10"/>
       <c r="AZ38" s="10"/>
       <c r="BA38" s="10"/>
-      <c r="BB38" s="75"/>
-      <c r="BC38" s="59"/>
+      <c r="BB38" s="74"/>
+      <c r="BC38" s="58"/>
       <c r="BD38" s="10"/>
       <c r="BE38" s="10"/>
       <c r="BF38" s="10"/>
@@ -9135,8 +9142,8 @@
       <c r="AY39" s="10"/>
       <c r="AZ39" s="10"/>
       <c r="BA39" s="10"/>
-      <c r="BB39" s="75"/>
-      <c r="BC39" s="59"/>
+      <c r="BB39" s="74"/>
+      <c r="BC39" s="58"/>
       <c r="BD39" s="10"/>
       <c r="BE39" s="10"/>
       <c r="BF39" s="10"/>
@@ -9243,8 +9250,8 @@
       <c r="AY40" s="10"/>
       <c r="AZ40" s="10"/>
       <c r="BA40" s="10"/>
-      <c r="BB40" s="75"/>
-      <c r="BC40" s="59"/>
+      <c r="BB40" s="74"/>
+      <c r="BC40" s="58"/>
       <c r="BD40" s="10"/>
       <c r="BE40" s="10"/>
       <c r="BF40" s="10"/>
@@ -9350,8 +9357,8 @@
       <c r="AY41" s="10"/>
       <c r="AZ41" s="10"/>
       <c r="BA41" s="10"/>
-      <c r="BB41" s="75"/>
-      <c r="BC41" s="59"/>
+      <c r="BB41" s="74"/>
+      <c r="BC41" s="58"/>
       <c r="BD41" s="10"/>
       <c r="BE41" s="10"/>
       <c r="BF41" s="10"/>
@@ -9448,8 +9455,8 @@
       <c r="AY42" s="10"/>
       <c r="AZ42" s="10"/>
       <c r="BA42" s="10"/>
-      <c r="BB42" s="75"/>
-      <c r="BC42" s="59"/>
+      <c r="BB42" s="74"/>
+      <c r="BC42" s="58"/>
       <c r="BD42" s="10"/>
       <c r="BE42" s="10"/>
       <c r="BF42" s="10"/>
@@ -9546,8 +9553,8 @@
       <c r="AY43" s="2"/>
       <c r="AZ43" s="2"/>
       <c r="BA43" s="2"/>
-      <c r="BB43" s="79"/>
-      <c r="BC43" s="80"/>
+      <c r="BB43" s="78"/>
+      <c r="BC43" s="79"/>
       <c r="BD43" s="2"/>
       <c r="BE43" s="2"/>
       <c r="BF43" s="2"/>
@@ -9592,11 +9599,11 @@
       <c r="CS43" s="2"/>
     </row>
     <row r="44" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="105" t="s">
+      <c r="A44" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="106"/>
-      <c r="C44" s="106"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="114"/>
       <c r="D44" s="35">
         <f>MIN(D45:D49)</f>
         <v>40364</v>
@@ -9652,8 +9659,8 @@
       <c r="AY44" s="4"/>
       <c r="AZ44" s="4"/>
       <c r="BA44" s="4"/>
-      <c r="BB44" s="81"/>
-      <c r="BC44" s="82"/>
+      <c r="BB44" s="80"/>
+      <c r="BC44" s="81"/>
       <c r="BD44" s="4"/>
       <c r="BE44" s="4"/>
       <c r="BF44" s="4"/>
@@ -9760,8 +9767,8 @@
       <c r="AY45" s="10"/>
       <c r="AZ45" s="10"/>
       <c r="BA45" s="10"/>
-      <c r="BB45" s="75"/>
-      <c r="BC45" s="59"/>
+      <c r="BB45" s="74"/>
+      <c r="BC45" s="58"/>
       <c r="BD45" s="10"/>
       <c r="BE45" s="10"/>
       <c r="BF45" s="10"/>
@@ -9868,8 +9875,8 @@
       <c r="AY46" s="10"/>
       <c r="AZ46" s="10"/>
       <c r="BA46" s="10"/>
-      <c r="BB46" s="75"/>
-      <c r="BC46" s="59"/>
+      <c r="BB46" s="74"/>
+      <c r="BC46" s="58"/>
       <c r="BD46" s="10"/>
       <c r="BE46" s="10"/>
       <c r="BF46" s="10"/>
@@ -9976,8 +9983,8 @@
       <c r="AY47" s="10"/>
       <c r="AZ47" s="10"/>
       <c r="BA47" s="10"/>
-      <c r="BB47" s="75"/>
-      <c r="BC47" s="59"/>
+      <c r="BB47" s="74"/>
+      <c r="BC47" s="58"/>
       <c r="BD47" s="10"/>
       <c r="BE47" s="10"/>
       <c r="BF47" s="10"/>
@@ -10084,8 +10091,8 @@
       <c r="AY48" s="10"/>
       <c r="AZ48" s="10"/>
       <c r="BA48" s="10"/>
-      <c r="BB48" s="75"/>
-      <c r="BC48" s="59"/>
+      <c r="BB48" s="74"/>
+      <c r="BC48" s="58"/>
       <c r="BD48" s="10"/>
       <c r="BE48" s="10"/>
       <c r="BF48" s="10"/>
@@ -10182,8 +10189,8 @@
       <c r="AY49" s="10"/>
       <c r="AZ49" s="10"/>
       <c r="BA49" s="10"/>
-      <c r="BB49" s="75"/>
-      <c r="BC49" s="59"/>
+      <c r="BB49" s="74"/>
+      <c r="BC49" s="58"/>
       <c r="BD49" s="10"/>
       <c r="BE49" s="10"/>
       <c r="BF49" s="10"/>
@@ -10228,8 +10235,8 @@
       <c r="CS49" s="10"/>
     </row>
     <row r="50" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="BB50" s="85"/>
-      <c r="BC50" s="86"/>
+      <c r="BB50" s="84"/>
+      <c r="BC50" s="85"/>
     </row>
     <row r="52" spans="1:97" x14ac:dyDescent="0.25">
       <c r="C52" s="9"/>
@@ -10239,29 +10246,151 @@
     </row>
   </sheetData>
   <mergeCells count="192">
-    <mergeCell ref="AS4:AS5"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AK5"/>
-    <mergeCell ref="AL4:AL5"/>
-    <mergeCell ref="AM4:AM5"/>
-    <mergeCell ref="AN4:AN5"/>
-    <mergeCell ref="AY4:AY5"/>
-    <mergeCell ref="AZ4:AZ5"/>
-    <mergeCell ref="BA4:BA5"/>
-    <mergeCell ref="AT4:AT5"/>
-    <mergeCell ref="AU4:AU5"/>
-    <mergeCell ref="AV4:AV5"/>
-    <mergeCell ref="AW4:AW5"/>
-    <mergeCell ref="AX4:AX5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="CR6:CR7"/>
+    <mergeCell ref="CS6:CS7"/>
+    <mergeCell ref="CM6:CM7"/>
+    <mergeCell ref="CN6:CN7"/>
+    <mergeCell ref="CO6:CO7"/>
+    <mergeCell ref="CP6:CP7"/>
+    <mergeCell ref="CQ6:CQ7"/>
+    <mergeCell ref="CH6:CH7"/>
+    <mergeCell ref="CI6:CI7"/>
+    <mergeCell ref="CJ6:CJ7"/>
+    <mergeCell ref="CK6:CK7"/>
+    <mergeCell ref="CL6:CL7"/>
+    <mergeCell ref="CC6:CC7"/>
+    <mergeCell ref="CD6:CD7"/>
+    <mergeCell ref="CE6:CE7"/>
+    <mergeCell ref="CF6:CF7"/>
+    <mergeCell ref="CG6:CG7"/>
+    <mergeCell ref="BX6:BX7"/>
+    <mergeCell ref="BY6:BY7"/>
+    <mergeCell ref="BZ6:BZ7"/>
+    <mergeCell ref="CA6:CA7"/>
+    <mergeCell ref="CB6:CB7"/>
+    <mergeCell ref="BS6:BS7"/>
+    <mergeCell ref="BT6:BT7"/>
+    <mergeCell ref="BU6:BU7"/>
+    <mergeCell ref="BV6:BV7"/>
+    <mergeCell ref="BW6:BW7"/>
+    <mergeCell ref="BN6:BN7"/>
+    <mergeCell ref="BO6:BO7"/>
+    <mergeCell ref="BP6:BP7"/>
+    <mergeCell ref="BQ6:BQ7"/>
+    <mergeCell ref="BR6:BR7"/>
+    <mergeCell ref="BI6:BI7"/>
+    <mergeCell ref="BJ6:BJ7"/>
+    <mergeCell ref="BK6:BK7"/>
+    <mergeCell ref="BL6:BL7"/>
+    <mergeCell ref="BM6:BM7"/>
+    <mergeCell ref="BD6:BD7"/>
+    <mergeCell ref="BE6:BE7"/>
+    <mergeCell ref="BF6:BF7"/>
+    <mergeCell ref="BG6:BG7"/>
+    <mergeCell ref="BH6:BH7"/>
+    <mergeCell ref="AY6:AY7"/>
+    <mergeCell ref="AZ6:AZ7"/>
+    <mergeCell ref="BA6:BA7"/>
+    <mergeCell ref="BB6:BB7"/>
+    <mergeCell ref="BC6:BC7"/>
+    <mergeCell ref="AT6:AT7"/>
+    <mergeCell ref="AU6:AU7"/>
+    <mergeCell ref="AV6:AV7"/>
+    <mergeCell ref="AW6:AW7"/>
+    <mergeCell ref="AX6:AX7"/>
+    <mergeCell ref="AO6:AO7"/>
+    <mergeCell ref="AP6:AP7"/>
+    <mergeCell ref="AQ6:AQ7"/>
+    <mergeCell ref="AR6:AR7"/>
+    <mergeCell ref="AS6:AS7"/>
+    <mergeCell ref="AJ6:AJ7"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AL6:AL7"/>
+    <mergeCell ref="AM6:AM7"/>
+    <mergeCell ref="AN6:AN7"/>
+    <mergeCell ref="AE6:AE7"/>
+    <mergeCell ref="AF6:AF7"/>
+    <mergeCell ref="AG6:AG7"/>
+    <mergeCell ref="AH6:AH7"/>
+    <mergeCell ref="AI6:AI7"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="AC6:AC7"/>
+    <mergeCell ref="AD6:AD7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="CR4:CR5"/>
+    <mergeCell ref="CS4:CS5"/>
+    <mergeCell ref="CM4:CM5"/>
+    <mergeCell ref="CN4:CN5"/>
+    <mergeCell ref="CO4:CO5"/>
+    <mergeCell ref="CP4:CP5"/>
+    <mergeCell ref="CQ4:CQ5"/>
+    <mergeCell ref="CH4:CH5"/>
+    <mergeCell ref="CI4:CI5"/>
+    <mergeCell ref="CJ4:CJ5"/>
+    <mergeCell ref="CK4:CK5"/>
+    <mergeCell ref="CL4:CL5"/>
+    <mergeCell ref="CC4:CC5"/>
+    <mergeCell ref="CD4:CD5"/>
+    <mergeCell ref="CE4:CE5"/>
+    <mergeCell ref="CF4:CF5"/>
+    <mergeCell ref="CG4:CG5"/>
+    <mergeCell ref="BX4:BX5"/>
+    <mergeCell ref="BY4:BY5"/>
+    <mergeCell ref="BZ4:BZ5"/>
+    <mergeCell ref="CA4:CA5"/>
+    <mergeCell ref="CB4:CB5"/>
+    <mergeCell ref="BS4:BS5"/>
+    <mergeCell ref="BT4:BT5"/>
+    <mergeCell ref="BU4:BU5"/>
+    <mergeCell ref="BV4:BV5"/>
+    <mergeCell ref="BW4:BW5"/>
+    <mergeCell ref="BN4:BN5"/>
+    <mergeCell ref="BO4:BO5"/>
+    <mergeCell ref="BP4:BP5"/>
+    <mergeCell ref="BQ4:BQ5"/>
+    <mergeCell ref="BR4:BR5"/>
+    <mergeCell ref="BI4:BI5"/>
+    <mergeCell ref="BJ4:BJ5"/>
+    <mergeCell ref="BK4:BK5"/>
+    <mergeCell ref="BL4:BL5"/>
+    <mergeCell ref="BB4:BB5"/>
+    <mergeCell ref="BC4:BC5"/>
+    <mergeCell ref="BM4:BM5"/>
+    <mergeCell ref="BD4:BD5"/>
+    <mergeCell ref="BE4:BE5"/>
+    <mergeCell ref="BF4:BF5"/>
+    <mergeCell ref="BG4:BG5"/>
+    <mergeCell ref="BH4:BH5"/>
     <mergeCell ref="H2:CS3"/>
     <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
@@ -10286,151 +10415,29 @@
     <mergeCell ref="AP4:AP5"/>
     <mergeCell ref="AQ4:AQ5"/>
     <mergeCell ref="AR4:AR5"/>
-    <mergeCell ref="BI4:BI5"/>
-    <mergeCell ref="BJ4:BJ5"/>
-    <mergeCell ref="BK4:BK5"/>
-    <mergeCell ref="BL4:BL5"/>
-    <mergeCell ref="BB4:BB5"/>
-    <mergeCell ref="BC4:BC5"/>
-    <mergeCell ref="BM4:BM5"/>
-    <mergeCell ref="BD4:BD5"/>
-    <mergeCell ref="BE4:BE5"/>
-    <mergeCell ref="BF4:BF5"/>
-    <mergeCell ref="BG4:BG5"/>
-    <mergeCell ref="BH4:BH5"/>
-    <mergeCell ref="BS4:BS5"/>
-    <mergeCell ref="BT4:BT5"/>
-    <mergeCell ref="BU4:BU5"/>
-    <mergeCell ref="BV4:BV5"/>
-    <mergeCell ref="BW4:BW5"/>
-    <mergeCell ref="BN4:BN5"/>
-    <mergeCell ref="BO4:BO5"/>
-    <mergeCell ref="BP4:BP5"/>
-    <mergeCell ref="BQ4:BQ5"/>
-    <mergeCell ref="BR4:BR5"/>
-    <mergeCell ref="CC4:CC5"/>
-    <mergeCell ref="CD4:CD5"/>
-    <mergeCell ref="CE4:CE5"/>
-    <mergeCell ref="CF4:CF5"/>
-    <mergeCell ref="CG4:CG5"/>
-    <mergeCell ref="BX4:BX5"/>
-    <mergeCell ref="BY4:BY5"/>
-    <mergeCell ref="BZ4:BZ5"/>
-    <mergeCell ref="CA4:CA5"/>
-    <mergeCell ref="CB4:CB5"/>
-    <mergeCell ref="CR4:CR5"/>
-    <mergeCell ref="CS4:CS5"/>
-    <mergeCell ref="CM4:CM5"/>
-    <mergeCell ref="CN4:CN5"/>
-    <mergeCell ref="CO4:CO5"/>
-    <mergeCell ref="CP4:CP5"/>
-    <mergeCell ref="CQ4:CQ5"/>
-    <mergeCell ref="CH4:CH5"/>
-    <mergeCell ref="CI4:CI5"/>
-    <mergeCell ref="CJ4:CJ5"/>
-    <mergeCell ref="CK4:CK5"/>
-    <mergeCell ref="CL4:CL5"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="AE6:AE7"/>
-    <mergeCell ref="AF6:AF7"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="AH6:AH7"/>
-    <mergeCell ref="AI6:AI7"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="AC6:AC7"/>
-    <mergeCell ref="AD6:AD7"/>
-    <mergeCell ref="AO6:AO7"/>
-    <mergeCell ref="AP6:AP7"/>
-    <mergeCell ref="AQ6:AQ7"/>
-    <mergeCell ref="AR6:AR7"/>
-    <mergeCell ref="AS6:AS7"/>
-    <mergeCell ref="AJ6:AJ7"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AL6:AL7"/>
-    <mergeCell ref="AM6:AM7"/>
-    <mergeCell ref="AN6:AN7"/>
-    <mergeCell ref="AY6:AY7"/>
-    <mergeCell ref="AZ6:AZ7"/>
-    <mergeCell ref="BA6:BA7"/>
-    <mergeCell ref="BB6:BB7"/>
-    <mergeCell ref="BC6:BC7"/>
-    <mergeCell ref="AT6:AT7"/>
-    <mergeCell ref="AU6:AU7"/>
-    <mergeCell ref="AV6:AV7"/>
-    <mergeCell ref="AW6:AW7"/>
-    <mergeCell ref="AX6:AX7"/>
-    <mergeCell ref="BI6:BI7"/>
-    <mergeCell ref="BJ6:BJ7"/>
-    <mergeCell ref="BK6:BK7"/>
-    <mergeCell ref="BL6:BL7"/>
-    <mergeCell ref="BM6:BM7"/>
-    <mergeCell ref="BD6:BD7"/>
-    <mergeCell ref="BE6:BE7"/>
-    <mergeCell ref="BF6:BF7"/>
-    <mergeCell ref="BG6:BG7"/>
-    <mergeCell ref="BH6:BH7"/>
-    <mergeCell ref="BS6:BS7"/>
-    <mergeCell ref="BT6:BT7"/>
-    <mergeCell ref="BU6:BU7"/>
-    <mergeCell ref="BV6:BV7"/>
-    <mergeCell ref="BW6:BW7"/>
-    <mergeCell ref="BN6:BN7"/>
-    <mergeCell ref="BO6:BO7"/>
-    <mergeCell ref="BP6:BP7"/>
-    <mergeCell ref="BQ6:BQ7"/>
-    <mergeCell ref="BR6:BR7"/>
-    <mergeCell ref="CC6:CC7"/>
-    <mergeCell ref="CD6:CD7"/>
-    <mergeCell ref="CE6:CE7"/>
-    <mergeCell ref="CF6:CF7"/>
-    <mergeCell ref="CG6:CG7"/>
-    <mergeCell ref="BX6:BX7"/>
-    <mergeCell ref="BY6:BY7"/>
-    <mergeCell ref="BZ6:BZ7"/>
-    <mergeCell ref="CA6:CA7"/>
-    <mergeCell ref="CB6:CB7"/>
-    <mergeCell ref="CR6:CR7"/>
-    <mergeCell ref="CS6:CS7"/>
-    <mergeCell ref="CM6:CM7"/>
-    <mergeCell ref="CN6:CN7"/>
-    <mergeCell ref="CO6:CO7"/>
-    <mergeCell ref="CP6:CP7"/>
-    <mergeCell ref="CQ6:CQ7"/>
-    <mergeCell ref="CH6:CH7"/>
-    <mergeCell ref="CI6:CI7"/>
-    <mergeCell ref="CJ6:CJ7"/>
-    <mergeCell ref="CK6:CK7"/>
-    <mergeCell ref="CL6:CL7"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="AS4:AS5"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AL4:AL5"/>
+    <mergeCell ref="AM4:AM5"/>
+    <mergeCell ref="AN4:AN5"/>
+    <mergeCell ref="AY4:AY5"/>
+    <mergeCell ref="AZ4:AZ5"/>
+    <mergeCell ref="BA4:BA5"/>
+    <mergeCell ref="AT4:AT5"/>
+    <mergeCell ref="AU4:AU5"/>
+    <mergeCell ref="AV4:AV5"/>
+    <mergeCell ref="AW4:AW5"/>
+    <mergeCell ref="AX4:AX5"/>
   </mergeCells>
   <conditionalFormatting sqref="H15:Q16 H11:CS14 H17:T17 V15:V16 Z15:CS16 H18:CS18 AJ17:CS17 H28:CS28 H37:CS42 H45:CS49 H31:CS34">
     <cfRule type="expression" dxfId="118" priority="7">
@@ -10883,132 +10890,210 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" style="40" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" style="41" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="37.42578125" style="41"/>
+    <col min="1" max="1" width="8.28515625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="87.140625" style="40" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="122" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="120" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="12" t="s">
+    <row r="1" spans="1:5" s="121" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="119" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="122" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="40"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="122">
         <v>15</v>
       </c>
+      <c r="D2" s="120">
+        <f ca="1">TODAY()+C2</f>
+        <v>41081</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="40">
-        <v>0.1</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="120" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="45">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="122">
+        <v>8</v>
+      </c>
+      <c r="D3" s="120">
+        <f ca="1">D2+C3</f>
+        <v>41089</v>
+      </c>
+      <c r="E3" s="44"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="122">
+        <v>5</v>
+      </c>
+      <c r="D4" s="120">
+        <f t="shared" ref="D4:D12" ca="1" si="0">D3+C4</f>
+        <v>41094</v>
+      </c>
+      <c r="E4" s="44"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="122">
+        <v>5</v>
+      </c>
+      <c r="D5" s="120">
+        <f t="shared" ca="1" si="0"/>
+        <v>41099</v>
+      </c>
+      <c r="E5" s="44"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="122">
+        <v>7</v>
+      </c>
+      <c r="D6" s="120">
+        <f t="shared" ca="1" si="0"/>
+        <v>41106</v>
+      </c>
+      <c r="E6" s="44"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="122">
+        <v>5</v>
+      </c>
+      <c r="D7" s="120">
+        <f t="shared" ca="1" si="0"/>
+        <v>41111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="122">
+        <v>3</v>
+      </c>
+      <c r="D8" s="120">
+        <f t="shared" ca="1" si="0"/>
+        <v>41114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="122">
+        <v>5</v>
+      </c>
+      <c r="D9" s="120">
+        <f ca="1">D8+C9</f>
+        <v>41119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="122">
+        <v>5</v>
+      </c>
+      <c r="D10" s="120">
+        <f t="shared" ca="1" si="0"/>
+        <v>41124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="122">
+        <v>3</v>
+      </c>
+      <c r="D11" s="120">
+        <f t="shared" ca="1" si="0"/>
+        <v>41127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="45">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="45">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="120"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="45">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="120"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="45">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
+      <c r="B12" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="122">
+        <v>3</v>
+      </c>
+      <c r="D12" s="120">
+        <f t="shared" ca="1" si="0"/>
+        <v>41130</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="C2:C6"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Update of Gannt Chart: Include actual time line.
</commit_message>
<xml_diff>
--- a/Documentation/Gannt Chart.xlsx
+++ b/Documentation/Gannt Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
   <si>
     <t>Start</t>
   </si>
@@ -118,19 +118,10 @@
     <t>Estimated Date of completion</t>
   </si>
   <si>
-    <t>Number of Days</t>
-  </si>
-  <si>
     <t>Task Description/ Change Log</t>
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>System 6 Legacy</t>
-  </si>
-  <si>
-    <t>Building of API (Currently 10% done)</t>
   </si>
   <si>
     <t xml:space="preserve">Parsing of BOTLAIDS </t>
@@ -139,28 +130,13 @@
     <t>Creating Data Template</t>
   </si>
   <si>
-    <t>Integration of API and BOTLAIDS</t>
-  </si>
-  <si>
     <t>Integration of BOTLAID and Sample Data</t>
-  </si>
-  <si>
-    <t>Include UI, system integration</t>
   </si>
   <si>
     <t>1.1</t>
   </si>
   <si>
-    <t>Adapted a branch out ready for System 6 Renovation</t>
-  </si>
-  <si>
     <t>2.0</t>
-  </si>
-  <si>
-    <t>1.0R</t>
-  </si>
-  <si>
-    <t>2.0R</t>
   </si>
   <si>
     <t>Able to take in multiple BOTLAIDS (back end)</t>
@@ -170,6 +146,18 @@
   </si>
   <si>
     <t>Able to read multiple campagin in 1 excel file, change in UI to select multiple BOTLAID</t>
+  </si>
+  <si>
+    <t>Number of Days Estimated</t>
+  </si>
+  <si>
+    <t>Actual Days taken</t>
+  </si>
+  <si>
+    <t>Actual Date of Completion</t>
+  </si>
+  <si>
+    <t>Include UI, system integration, finalise Data template</t>
   </si>
 </sst>
 </file>
@@ -181,7 +169,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="166" formatCode="mmm"/>
     <numFmt numFmtId="167" formatCode="m/d;@"/>
-    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1062,7 +1050,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1281,6 +1269,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1326,18 +1326,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5012,10 +5004,10 @@
     <row r="1" spans="1:98" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:98" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="116"/>
+      <c r="C2" s="120"/>
       <c r="D2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5023,105 +5015,105 @@
         <v>1</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="107" t="s">
+      <c r="H2" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="108"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="108"/>
-      <c r="M2" s="108"/>
-      <c r="N2" s="108"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="108"/>
-      <c r="R2" s="108"/>
-      <c r="S2" s="108"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="108"/>
-      <c r="V2" s="108"/>
-      <c r="W2" s="108"/>
-      <c r="X2" s="108"/>
-      <c r="Y2" s="108"/>
-      <c r="Z2" s="108"/>
-      <c r="AA2" s="108"/>
-      <c r="AB2" s="108"/>
-      <c r="AC2" s="108"/>
-      <c r="AD2" s="108"/>
-      <c r="AE2" s="108"/>
-      <c r="AF2" s="108"/>
-      <c r="AG2" s="108"/>
-      <c r="AH2" s="108"/>
-      <c r="AI2" s="108"/>
-      <c r="AJ2" s="108"/>
-      <c r="AK2" s="108"/>
-      <c r="AL2" s="108"/>
-      <c r="AM2" s="108"/>
-      <c r="AN2" s="108"/>
-      <c r="AO2" s="108"/>
-      <c r="AP2" s="108"/>
-      <c r="AQ2" s="108"/>
-      <c r="AR2" s="108"/>
-      <c r="AS2" s="108"/>
-      <c r="AT2" s="108"/>
-      <c r="AU2" s="108"/>
-      <c r="AV2" s="108"/>
-      <c r="AW2" s="108"/>
-      <c r="AX2" s="108"/>
-      <c r="AY2" s="108"/>
-      <c r="AZ2" s="108"/>
-      <c r="BA2" s="108"/>
-      <c r="BB2" s="108"/>
-      <c r="BC2" s="108"/>
-      <c r="BD2" s="108"/>
-      <c r="BE2" s="108"/>
-      <c r="BF2" s="108"/>
-      <c r="BG2" s="108"/>
-      <c r="BH2" s="108"/>
-      <c r="BI2" s="108"/>
-      <c r="BJ2" s="108"/>
-      <c r="BK2" s="108"/>
-      <c r="BL2" s="108"/>
-      <c r="BM2" s="108"/>
-      <c r="BN2" s="108"/>
-      <c r="BO2" s="108"/>
-      <c r="BP2" s="108"/>
-      <c r="BQ2" s="108"/>
-      <c r="BR2" s="108"/>
-      <c r="BS2" s="108"/>
-      <c r="BT2" s="108"/>
-      <c r="BU2" s="108"/>
-      <c r="BV2" s="108"/>
-      <c r="BW2" s="108"/>
-      <c r="BX2" s="108"/>
-      <c r="BY2" s="108"/>
-      <c r="BZ2" s="108"/>
-      <c r="CA2" s="108"/>
-      <c r="CB2" s="108"/>
-      <c r="CC2" s="108"/>
-      <c r="CD2" s="108"/>
-      <c r="CE2" s="108"/>
-      <c r="CF2" s="108"/>
-      <c r="CG2" s="108"/>
-      <c r="CH2" s="108"/>
-      <c r="CI2" s="108"/>
-      <c r="CJ2" s="108"/>
-      <c r="CK2" s="108"/>
-      <c r="CL2" s="108"/>
-      <c r="CM2" s="108"/>
-      <c r="CN2" s="108"/>
-      <c r="CO2" s="108"/>
-      <c r="CP2" s="108"/>
-      <c r="CQ2" s="108"/>
-      <c r="CR2" s="108"/>
-      <c r="CS2" s="108"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="112"/>
+      <c r="R2" s="112"/>
+      <c r="S2" s="112"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="112"/>
+      <c r="V2" s="112"/>
+      <c r="W2" s="112"/>
+      <c r="X2" s="112"/>
+      <c r="Y2" s="112"/>
+      <c r="Z2" s="112"/>
+      <c r="AA2" s="112"/>
+      <c r="AB2" s="112"/>
+      <c r="AC2" s="112"/>
+      <c r="AD2" s="112"/>
+      <c r="AE2" s="112"/>
+      <c r="AF2" s="112"/>
+      <c r="AG2" s="112"/>
+      <c r="AH2" s="112"/>
+      <c r="AI2" s="112"/>
+      <c r="AJ2" s="112"/>
+      <c r="AK2" s="112"/>
+      <c r="AL2" s="112"/>
+      <c r="AM2" s="112"/>
+      <c r="AN2" s="112"/>
+      <c r="AO2" s="112"/>
+      <c r="AP2" s="112"/>
+      <c r="AQ2" s="112"/>
+      <c r="AR2" s="112"/>
+      <c r="AS2" s="112"/>
+      <c r="AT2" s="112"/>
+      <c r="AU2" s="112"/>
+      <c r="AV2" s="112"/>
+      <c r="AW2" s="112"/>
+      <c r="AX2" s="112"/>
+      <c r="AY2" s="112"/>
+      <c r="AZ2" s="112"/>
+      <c r="BA2" s="112"/>
+      <c r="BB2" s="112"/>
+      <c r="BC2" s="112"/>
+      <c r="BD2" s="112"/>
+      <c r="BE2" s="112"/>
+      <c r="BF2" s="112"/>
+      <c r="BG2" s="112"/>
+      <c r="BH2" s="112"/>
+      <c r="BI2" s="112"/>
+      <c r="BJ2" s="112"/>
+      <c r="BK2" s="112"/>
+      <c r="BL2" s="112"/>
+      <c r="BM2" s="112"/>
+      <c r="BN2" s="112"/>
+      <c r="BO2" s="112"/>
+      <c r="BP2" s="112"/>
+      <c r="BQ2" s="112"/>
+      <c r="BR2" s="112"/>
+      <c r="BS2" s="112"/>
+      <c r="BT2" s="112"/>
+      <c r="BU2" s="112"/>
+      <c r="BV2" s="112"/>
+      <c r="BW2" s="112"/>
+      <c r="BX2" s="112"/>
+      <c r="BY2" s="112"/>
+      <c r="BZ2" s="112"/>
+      <c r="CA2" s="112"/>
+      <c r="CB2" s="112"/>
+      <c r="CC2" s="112"/>
+      <c r="CD2" s="112"/>
+      <c r="CE2" s="112"/>
+      <c r="CF2" s="112"/>
+      <c r="CG2" s="112"/>
+      <c r="CH2" s="112"/>
+      <c r="CI2" s="112"/>
+      <c r="CJ2" s="112"/>
+      <c r="CK2" s="112"/>
+      <c r="CL2" s="112"/>
+      <c r="CM2" s="112"/>
+      <c r="CN2" s="112"/>
+      <c r="CO2" s="112"/>
+      <c r="CP2" s="112"/>
+      <c r="CQ2" s="112"/>
+      <c r="CR2" s="112"/>
+      <c r="CS2" s="112"/>
     </row>
     <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="121" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="117"/>
+      <c r="C3" s="121"/>
       <c r="D3" s="14">
         <v>41112</v>
       </c>
@@ -5129,461 +5121,461 @@
         <v>41115</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="109"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="110"/>
-      <c r="P3" s="110"/>
-      <c r="Q3" s="110"/>
-      <c r="R3" s="110"/>
-      <c r="S3" s="110"/>
-      <c r="T3" s="110"/>
-      <c r="U3" s="110"/>
-      <c r="V3" s="110"/>
-      <c r="W3" s="110"/>
-      <c r="X3" s="110"/>
-      <c r="Y3" s="110"/>
-      <c r="Z3" s="110"/>
-      <c r="AA3" s="110"/>
-      <c r="AB3" s="110"/>
-      <c r="AC3" s="110"/>
-      <c r="AD3" s="110"/>
-      <c r="AE3" s="110"/>
-      <c r="AF3" s="110"/>
-      <c r="AG3" s="110"/>
-      <c r="AH3" s="110"/>
-      <c r="AI3" s="110"/>
-      <c r="AJ3" s="110"/>
-      <c r="AK3" s="110"/>
-      <c r="AL3" s="110"/>
-      <c r="AM3" s="110"/>
-      <c r="AN3" s="110"/>
-      <c r="AO3" s="110"/>
-      <c r="AP3" s="110"/>
-      <c r="AQ3" s="110"/>
-      <c r="AR3" s="110"/>
-      <c r="AS3" s="110"/>
-      <c r="AT3" s="110"/>
-      <c r="AU3" s="110"/>
-      <c r="AV3" s="110"/>
-      <c r="AW3" s="110"/>
-      <c r="AX3" s="110"/>
-      <c r="AY3" s="110"/>
-      <c r="AZ3" s="110"/>
-      <c r="BA3" s="110"/>
-      <c r="BB3" s="110"/>
-      <c r="BC3" s="110"/>
-      <c r="BD3" s="110"/>
-      <c r="BE3" s="110"/>
-      <c r="BF3" s="110"/>
-      <c r="BG3" s="110"/>
-      <c r="BH3" s="110"/>
-      <c r="BI3" s="110"/>
-      <c r="BJ3" s="110"/>
-      <c r="BK3" s="110"/>
-      <c r="BL3" s="110"/>
-      <c r="BM3" s="110"/>
-      <c r="BN3" s="110"/>
-      <c r="BO3" s="110"/>
-      <c r="BP3" s="110"/>
-      <c r="BQ3" s="110"/>
-      <c r="BR3" s="110"/>
-      <c r="BS3" s="110"/>
-      <c r="BT3" s="110"/>
-      <c r="BU3" s="110"/>
-      <c r="BV3" s="110"/>
-      <c r="BW3" s="110"/>
-      <c r="BX3" s="110"/>
-      <c r="BY3" s="110"/>
-      <c r="BZ3" s="110"/>
-      <c r="CA3" s="110"/>
-      <c r="CB3" s="110"/>
-      <c r="CC3" s="110"/>
-      <c r="CD3" s="110"/>
-      <c r="CE3" s="110"/>
-      <c r="CF3" s="110"/>
-      <c r="CG3" s="110"/>
-      <c r="CH3" s="110"/>
-      <c r="CI3" s="110"/>
-      <c r="CJ3" s="110"/>
-      <c r="CK3" s="110"/>
-      <c r="CL3" s="110"/>
-      <c r="CM3" s="110"/>
-      <c r="CN3" s="110"/>
-      <c r="CO3" s="110"/>
-      <c r="CP3" s="110"/>
-      <c r="CQ3" s="110"/>
-      <c r="CR3" s="110"/>
-      <c r="CS3" s="110"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="114"/>
+      <c r="L3" s="114"/>
+      <c r="M3" s="114"/>
+      <c r="N3" s="114"/>
+      <c r="O3" s="114"/>
+      <c r="P3" s="114"/>
+      <c r="Q3" s="114"/>
+      <c r="R3" s="114"/>
+      <c r="S3" s="114"/>
+      <c r="T3" s="114"/>
+      <c r="U3" s="114"/>
+      <c r="V3" s="114"/>
+      <c r="W3" s="114"/>
+      <c r="X3" s="114"/>
+      <c r="Y3" s="114"/>
+      <c r="Z3" s="114"/>
+      <c r="AA3" s="114"/>
+      <c r="AB3" s="114"/>
+      <c r="AC3" s="114"/>
+      <c r="AD3" s="114"/>
+      <c r="AE3" s="114"/>
+      <c r="AF3" s="114"/>
+      <c r="AG3" s="114"/>
+      <c r="AH3" s="114"/>
+      <c r="AI3" s="114"/>
+      <c r="AJ3" s="114"/>
+      <c r="AK3" s="114"/>
+      <c r="AL3" s="114"/>
+      <c r="AM3" s="114"/>
+      <c r="AN3" s="114"/>
+      <c r="AO3" s="114"/>
+      <c r="AP3" s="114"/>
+      <c r="AQ3" s="114"/>
+      <c r="AR3" s="114"/>
+      <c r="AS3" s="114"/>
+      <c r="AT3" s="114"/>
+      <c r="AU3" s="114"/>
+      <c r="AV3" s="114"/>
+      <c r="AW3" s="114"/>
+      <c r="AX3" s="114"/>
+      <c r="AY3" s="114"/>
+      <c r="AZ3" s="114"/>
+      <c r="BA3" s="114"/>
+      <c r="BB3" s="114"/>
+      <c r="BC3" s="114"/>
+      <c r="BD3" s="114"/>
+      <c r="BE3" s="114"/>
+      <c r="BF3" s="114"/>
+      <c r="BG3" s="114"/>
+      <c r="BH3" s="114"/>
+      <c r="BI3" s="114"/>
+      <c r="BJ3" s="114"/>
+      <c r="BK3" s="114"/>
+      <c r="BL3" s="114"/>
+      <c r="BM3" s="114"/>
+      <c r="BN3" s="114"/>
+      <c r="BO3" s="114"/>
+      <c r="BP3" s="114"/>
+      <c r="BQ3" s="114"/>
+      <c r="BR3" s="114"/>
+      <c r="BS3" s="114"/>
+      <c r="BT3" s="114"/>
+      <c r="BU3" s="114"/>
+      <c r="BV3" s="114"/>
+      <c r="BW3" s="114"/>
+      <c r="BX3" s="114"/>
+      <c r="BY3" s="114"/>
+      <c r="BZ3" s="114"/>
+      <c r="CA3" s="114"/>
+      <c r="CB3" s="114"/>
+      <c r="CC3" s="114"/>
+      <c r="CD3" s="114"/>
+      <c r="CE3" s="114"/>
+      <c r="CF3" s="114"/>
+      <c r="CG3" s="114"/>
+      <c r="CH3" s="114"/>
+      <c r="CI3" s="114"/>
+      <c r="CJ3" s="114"/>
+      <c r="CK3" s="114"/>
+      <c r="CL3" s="114"/>
+      <c r="CM3" s="114"/>
+      <c r="CN3" s="114"/>
+      <c r="CO3" s="114"/>
+      <c r="CP3" s="114"/>
+      <c r="CQ3" s="114"/>
+      <c r="CR3" s="114"/>
+      <c r="CS3" s="114"/>
     </row>
     <row r="4" spans="1:98" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="122"/>
       <c r="D4" s="14"/>
       <c r="E4" s="15"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="104">
+      <c r="H4" s="108">
         <f>IF(MONTH(H6)&lt;&gt;MONTH(E6),H6,"")</f>
         <v>41057</v>
       </c>
-      <c r="I4" s="104" t="str">
+      <c r="I4" s="108" t="str">
         <f t="shared" ref="I4:BT4" si="0">IF(MONTH(I6)&lt;&gt;MONTH(H6),I6,"")</f>
         <v/>
       </c>
-      <c r="J4" s="104" t="str">
+      <c r="J4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="104" t="str">
+      <c r="K4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L4" s="104">
+      <c r="L4" s="108">
         <f t="shared" si="0"/>
         <v>41061</v>
       </c>
-      <c r="M4" s="105" t="str">
+      <c r="M4" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N4" s="105" t="str">
+      <c r="N4" s="109" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="O4" s="104" t="str">
+      <c r="O4" s="108" t="str">
         <f>IF(MONTH(O6)&lt;&gt;MONTH(N6),O6,"")</f>
         <v/>
       </c>
-      <c r="P4" s="104" t="str">
+      <c r="P4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q4" s="104" t="str">
+      <c r="Q4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R4" s="104" t="str">
+      <c r="R4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S4" s="104" t="str">
+      <c r="S4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="T4" s="104" t="str">
+      <c r="T4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="U4" s="104" t="str">
+      <c r="U4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V4" s="104" t="str">
+      <c r="V4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="W4" s="104" t="str">
+      <c r="W4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="X4" s="104" t="str">
+      <c r="X4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Y4" s="104" t="str">
+      <c r="Y4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Z4" s="104" t="str">
+      <c r="Z4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AA4" s="104" t="str">
+      <c r="AA4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AB4" s="104" t="str">
+      <c r="AB4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AC4" s="104" t="str">
+      <c r="AC4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AD4" s="104" t="str">
+      <c r="AD4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE4" s="104" t="str">
+      <c r="AE4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AF4" s="104" t="str">
+      <c r="AF4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AG4" s="104">
+      <c r="AG4" s="108">
         <f t="shared" si="0"/>
         <v>41092</v>
       </c>
-      <c r="AH4" s="104" t="str">
+      <c r="AH4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AI4" s="104" t="str">
+      <c r="AI4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AJ4" s="104" t="str">
+      <c r="AJ4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AK4" s="104" t="str">
+      <c r="AK4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AL4" s="104" t="str">
+      <c r="AL4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AM4" s="104" t="str">
+      <c r="AM4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AN4" s="104" t="str">
+      <c r="AN4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AO4" s="104" t="str">
+      <c r="AO4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AP4" s="104" t="str">
+      <c r="AP4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AQ4" s="104" t="str">
+      <c r="AQ4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AR4" s="104" t="str">
+      <c r="AR4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AS4" s="104" t="str">
+      <c r="AS4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AT4" s="104" t="str">
+      <c r="AT4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AU4" s="104" t="str">
+      <c r="AU4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AV4" s="104" t="str">
+      <c r="AV4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AW4" s="104" t="str">
+      <c r="AW4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AX4" s="104" t="str">
+      <c r="AX4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AY4" s="104" t="str">
+      <c r="AY4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AZ4" s="104" t="str">
+      <c r="AZ4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BA4" s="104" t="str">
+      <c r="BA4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BB4" s="104" t="str">
+      <c r="BB4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BC4" s="104">
+      <c r="BC4" s="108">
         <f t="shared" si="0"/>
         <v>41122</v>
       </c>
-      <c r="BD4" s="104" t="str">
+      <c r="BD4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BE4" s="104" t="str">
+      <c r="BE4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BF4" s="104" t="str">
+      <c r="BF4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BG4" s="104" t="str">
+      <c r="BG4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BH4" s="104" t="str">
+      <c r="BH4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BI4" s="104" t="str">
+      <c r="BI4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BJ4" s="104" t="str">
+      <c r="BJ4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BK4" s="104" t="str">
+      <c r="BK4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BL4" s="104" t="str">
+      <c r="BL4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BM4" s="104" t="str">
+      <c r="BM4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BN4" s="104" t="str">
+      <c r="BN4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BO4" s="104" t="str">
+      <c r="BO4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BP4" s="104" t="str">
+      <c r="BP4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BQ4" s="104" t="str">
+      <c r="BQ4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BR4" s="104" t="str">
+      <c r="BR4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BS4" s="104" t="str">
+      <c r="BS4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BT4" s="104" t="str">
+      <c r="BT4" s="108" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BU4" s="104" t="str">
+      <c r="BU4" s="108" t="str">
         <f t="shared" ref="BU4:CS4" si="1">IF(MONTH(BU6)&lt;&gt;MONTH(BT6),BU6,"")</f>
         <v/>
       </c>
-      <c r="BV4" s="104" t="str">
+      <c r="BV4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BW4" s="104" t="str">
+      <c r="BW4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BX4" s="104" t="str">
+      <c r="BX4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BY4" s="104" t="str">
+      <c r="BY4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BZ4" s="104">
+      <c r="BZ4" s="108">
         <f t="shared" si="1"/>
         <v>41155</v>
       </c>
-      <c r="CA4" s="104" t="str">
+      <c r="CA4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CB4" s="104" t="str">
+      <c r="CB4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CC4" s="104" t="str">
+      <c r="CC4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CD4" s="104" t="str">
+      <c r="CD4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CE4" s="104" t="str">
+      <c r="CE4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CF4" s="104" t="str">
+      <c r="CF4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CG4" s="104" t="str">
+      <c r="CG4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CH4" s="104" t="str">
+      <c r="CH4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CI4" s="104" t="str">
+      <c r="CI4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CJ4" s="104" t="str">
+      <c r="CJ4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CK4" s="104" t="str">
+      <c r="CK4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CL4" s="104" t="str">
+      <c r="CL4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CM4" s="104" t="str">
+      <c r="CM4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CN4" s="104" t="str">
+      <c r="CN4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CO4" s="104" t="str">
+      <c r="CO4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CP4" s="104" t="str">
+      <c r="CP4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CQ4" s="104" t="str">
+      <c r="CQ4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CR4" s="104" t="str">
+      <c r="CR4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CS4" s="104" t="str">
+      <c r="CS4" s="108" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5591,467 +5583,467 @@
     </row>
     <row r="5" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="122"/>
       <c r="D5" s="14"/>
       <c r="E5" s="15"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="106"/>
-      <c r="N5" s="106"/>
-      <c r="O5" s="104"/>
-      <c r="P5" s="104"/>
-      <c r="Q5" s="104"/>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="104"/>
-      <c r="V5" s="104"/>
-      <c r="W5" s="104"/>
-      <c r="X5" s="104"/>
-      <c r="Y5" s="104"/>
-      <c r="Z5" s="104"/>
-      <c r="AA5" s="104"/>
-      <c r="AB5" s="104"/>
-      <c r="AC5" s="104"/>
-      <c r="AD5" s="104"/>
-      <c r="AE5" s="104"/>
-      <c r="AF5" s="104"/>
-      <c r="AG5" s="104"/>
-      <c r="AH5" s="104"/>
-      <c r="AI5" s="104"/>
-      <c r="AJ5" s="104"/>
-      <c r="AK5" s="104"/>
-      <c r="AL5" s="104"/>
-      <c r="AM5" s="104"/>
-      <c r="AN5" s="104"/>
-      <c r="AO5" s="104"/>
-      <c r="AP5" s="104"/>
-      <c r="AQ5" s="104"/>
-      <c r="AR5" s="104"/>
-      <c r="AS5" s="104"/>
-      <c r="AT5" s="104"/>
-      <c r="AU5" s="104"/>
-      <c r="AV5" s="104"/>
-      <c r="AW5" s="104"/>
-      <c r="AX5" s="104"/>
-      <c r="AY5" s="104"/>
-      <c r="AZ5" s="104"/>
-      <c r="BA5" s="104"/>
-      <c r="BB5" s="104"/>
-      <c r="BC5" s="104"/>
-      <c r="BD5" s="104"/>
-      <c r="BE5" s="104"/>
-      <c r="BF5" s="104"/>
-      <c r="BG5" s="104"/>
-      <c r="BH5" s="104"/>
-      <c r="BI5" s="104"/>
-      <c r="BJ5" s="104"/>
-      <c r="BK5" s="104"/>
-      <c r="BL5" s="104"/>
-      <c r="BM5" s="104"/>
-      <c r="BN5" s="104"/>
-      <c r="BO5" s="104"/>
-      <c r="BP5" s="104"/>
-      <c r="BQ5" s="104"/>
-      <c r="BR5" s="104"/>
-      <c r="BS5" s="104"/>
-      <c r="BT5" s="104"/>
-      <c r="BU5" s="104"/>
-      <c r="BV5" s="104"/>
-      <c r="BW5" s="104"/>
-      <c r="BX5" s="104"/>
-      <c r="BY5" s="104"/>
-      <c r="BZ5" s="104"/>
-      <c r="CA5" s="104"/>
-      <c r="CB5" s="104"/>
-      <c r="CC5" s="104"/>
-      <c r="CD5" s="104"/>
-      <c r="CE5" s="104"/>
-      <c r="CF5" s="104"/>
-      <c r="CG5" s="104"/>
-      <c r="CH5" s="104"/>
-      <c r="CI5" s="104"/>
-      <c r="CJ5" s="104"/>
-      <c r="CK5" s="104"/>
-      <c r="CL5" s="104"/>
-      <c r="CM5" s="104"/>
-      <c r="CN5" s="104"/>
-      <c r="CO5" s="104"/>
-      <c r="CP5" s="104"/>
-      <c r="CQ5" s="104"/>
-      <c r="CR5" s="104"/>
-      <c r="CS5" s="104"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="110"/>
+      <c r="N5" s="110"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="108"/>
+      <c r="S5" s="108"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="108"/>
+      <c r="V5" s="108"/>
+      <c r="W5" s="108"/>
+      <c r="X5" s="108"/>
+      <c r="Y5" s="108"/>
+      <c r="Z5" s="108"/>
+      <c r="AA5" s="108"/>
+      <c r="AB5" s="108"/>
+      <c r="AC5" s="108"/>
+      <c r="AD5" s="108"/>
+      <c r="AE5" s="108"/>
+      <c r="AF5" s="108"/>
+      <c r="AG5" s="108"/>
+      <c r="AH5" s="108"/>
+      <c r="AI5" s="108"/>
+      <c r="AJ5" s="108"/>
+      <c r="AK5" s="108"/>
+      <c r="AL5" s="108"/>
+      <c r="AM5" s="108"/>
+      <c r="AN5" s="108"/>
+      <c r="AO5" s="108"/>
+      <c r="AP5" s="108"/>
+      <c r="AQ5" s="108"/>
+      <c r="AR5" s="108"/>
+      <c r="AS5" s="108"/>
+      <c r="AT5" s="108"/>
+      <c r="AU5" s="108"/>
+      <c r="AV5" s="108"/>
+      <c r="AW5" s="108"/>
+      <c r="AX5" s="108"/>
+      <c r="AY5" s="108"/>
+      <c r="AZ5" s="108"/>
+      <c r="BA5" s="108"/>
+      <c r="BB5" s="108"/>
+      <c r="BC5" s="108"/>
+      <c r="BD5" s="108"/>
+      <c r="BE5" s="108"/>
+      <c r="BF5" s="108"/>
+      <c r="BG5" s="108"/>
+      <c r="BH5" s="108"/>
+      <c r="BI5" s="108"/>
+      <c r="BJ5" s="108"/>
+      <c r="BK5" s="108"/>
+      <c r="BL5" s="108"/>
+      <c r="BM5" s="108"/>
+      <c r="BN5" s="108"/>
+      <c r="BO5" s="108"/>
+      <c r="BP5" s="108"/>
+      <c r="BQ5" s="108"/>
+      <c r="BR5" s="108"/>
+      <c r="BS5" s="108"/>
+      <c r="BT5" s="108"/>
+      <c r="BU5" s="108"/>
+      <c r="BV5" s="108"/>
+      <c r="BW5" s="108"/>
+      <c r="BX5" s="108"/>
+      <c r="BY5" s="108"/>
+      <c r="BZ5" s="108"/>
+      <c r="CA5" s="108"/>
+      <c r="CB5" s="108"/>
+      <c r="CC5" s="108"/>
+      <c r="CD5" s="108"/>
+      <c r="CE5" s="108"/>
+      <c r="CF5" s="108"/>
+      <c r="CG5" s="108"/>
+      <c r="CH5" s="108"/>
+      <c r="CI5" s="108"/>
+      <c r="CJ5" s="108"/>
+      <c r="CK5" s="108"/>
+      <c r="CL5" s="108"/>
+      <c r="CM5" s="108"/>
+      <c r="CN5" s="108"/>
+      <c r="CO5" s="108"/>
+      <c r="CP5" s="108"/>
+      <c r="CQ5" s="108"/>
+      <c r="CR5" s="108"/>
+      <c r="CS5" s="108"/>
       <c r="CT5" s="12"/>
     </row>
     <row r="6" spans="1:98" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="122"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15"/>
       <c r="F6" s="29"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="111">
+      <c r="H6" s="115">
         <v>41057</v>
       </c>
-      <c r="I6" s="111">
+      <c r="I6" s="115">
         <f>H6+IF(WEEKDAY(H6)=6,3,1)</f>
         <v>41058</v>
       </c>
-      <c r="J6" s="111">
+      <c r="J6" s="115">
         <f t="shared" ref="J6:AS6" si="2">I6+IF(WEEKDAY(I6)=6,3,1)</f>
         <v>41059</v>
       </c>
-      <c r="K6" s="111">
+      <c r="K6" s="115">
         <f t="shared" si="2"/>
         <v>41060</v>
       </c>
-      <c r="L6" s="111">
+      <c r="L6" s="115">
         <f t="shared" si="2"/>
         <v>41061</v>
       </c>
-      <c r="M6" s="111">
+      <c r="M6" s="115">
         <f t="shared" si="2"/>
         <v>41064</v>
       </c>
-      <c r="N6" s="111">
+      <c r="N6" s="115">
         <f t="shared" si="2"/>
         <v>41065</v>
       </c>
-      <c r="O6" s="111">
+      <c r="O6" s="115">
         <f t="shared" si="2"/>
         <v>41066</v>
       </c>
-      <c r="P6" s="111">
+      <c r="P6" s="115">
         <f t="shared" si="2"/>
         <v>41067</v>
       </c>
-      <c r="Q6" s="111">
+      <c r="Q6" s="115">
         <f t="shared" si="2"/>
         <v>41068</v>
       </c>
-      <c r="R6" s="111">
+      <c r="R6" s="115">
         <f t="shared" si="2"/>
         <v>41071</v>
       </c>
-      <c r="S6" s="111">
+      <c r="S6" s="115">
         <f t="shared" si="2"/>
         <v>41072</v>
       </c>
-      <c r="T6" s="111">
+      <c r="T6" s="115">
         <f t="shared" si="2"/>
         <v>41073</v>
       </c>
-      <c r="U6" s="111">
+      <c r="U6" s="115">
         <f t="shared" si="2"/>
         <v>41074</v>
       </c>
-      <c r="V6" s="111">
+      <c r="V6" s="115">
         <f t="shared" si="2"/>
         <v>41075</v>
       </c>
-      <c r="W6" s="111">
+      <c r="W6" s="115">
         <f t="shared" si="2"/>
         <v>41078</v>
       </c>
-      <c r="X6" s="111">
+      <c r="X6" s="115">
         <f t="shared" si="2"/>
         <v>41079</v>
       </c>
-      <c r="Y6" s="111">
+      <c r="Y6" s="115">
         <f t="shared" si="2"/>
         <v>41080</v>
       </c>
-      <c r="Z6" s="111">
+      <c r="Z6" s="115">
         <f t="shared" si="2"/>
         <v>41081</v>
       </c>
-      <c r="AA6" s="111">
+      <c r="AA6" s="115">
         <f t="shared" si="2"/>
         <v>41082</v>
       </c>
-      <c r="AB6" s="111">
+      <c r="AB6" s="115">
         <f t="shared" si="2"/>
         <v>41085</v>
       </c>
-      <c r="AC6" s="111">
+      <c r="AC6" s="115">
         <f t="shared" si="2"/>
         <v>41086</v>
       </c>
-      <c r="AD6" s="111">
+      <c r="AD6" s="115">
         <f t="shared" si="2"/>
         <v>41087</v>
       </c>
-      <c r="AE6" s="111">
+      <c r="AE6" s="115">
         <f t="shared" si="2"/>
         <v>41088</v>
       </c>
-      <c r="AF6" s="111">
+      <c r="AF6" s="115">
         <f t="shared" si="2"/>
         <v>41089</v>
       </c>
-      <c r="AG6" s="111">
+      <c r="AG6" s="115">
         <f t="shared" si="2"/>
         <v>41092</v>
       </c>
-      <c r="AH6" s="111">
+      <c r="AH6" s="115">
         <f t="shared" si="2"/>
         <v>41093</v>
       </c>
-      <c r="AI6" s="111">
+      <c r="AI6" s="115">
         <f t="shared" si="2"/>
         <v>41094</v>
       </c>
-      <c r="AJ6" s="111">
+      <c r="AJ6" s="115">
         <f t="shared" si="2"/>
         <v>41095</v>
       </c>
-      <c r="AK6" s="111">
+      <c r="AK6" s="115">
         <f t="shared" si="2"/>
         <v>41096</v>
       </c>
-      <c r="AL6" s="111">
+      <c r="AL6" s="115">
         <f t="shared" si="2"/>
         <v>41099</v>
       </c>
-      <c r="AM6" s="111">
+      <c r="AM6" s="115">
         <f t="shared" si="2"/>
         <v>41100</v>
       </c>
-      <c r="AN6" s="111">
+      <c r="AN6" s="115">
         <f t="shared" si="2"/>
         <v>41101</v>
       </c>
-      <c r="AO6" s="111">
+      <c r="AO6" s="115">
         <f t="shared" si="2"/>
         <v>41102</v>
       </c>
-      <c r="AP6" s="111">
+      <c r="AP6" s="115">
         <f t="shared" si="2"/>
         <v>41103</v>
       </c>
-      <c r="AQ6" s="111">
+      <c r="AQ6" s="115">
         <f t="shared" si="2"/>
         <v>41106</v>
       </c>
-      <c r="AR6" s="111">
+      <c r="AR6" s="115">
         <f t="shared" si="2"/>
         <v>41107</v>
       </c>
-      <c r="AS6" s="111">
+      <c r="AS6" s="115">
         <f t="shared" si="2"/>
         <v>41108</v>
       </c>
-      <c r="AT6" s="111">
+      <c r="AT6" s="115">
         <f t="shared" ref="AT6:CS6" si="3">AS6+IF(WEEKDAY(AS6)=6,3,1)</f>
         <v>41109</v>
       </c>
-      <c r="AU6" s="111">
+      <c r="AU6" s="115">
         <f t="shared" si="3"/>
         <v>41110</v>
       </c>
-      <c r="AV6" s="111">
+      <c r="AV6" s="115">
         <f t="shared" si="3"/>
         <v>41113</v>
       </c>
-      <c r="AW6" s="111">
+      <c r="AW6" s="115">
         <f t="shared" si="3"/>
         <v>41114</v>
       </c>
-      <c r="AX6" s="111">
+      <c r="AX6" s="115">
         <f t="shared" si="3"/>
         <v>41115</v>
       </c>
-      <c r="AY6" s="111">
+      <c r="AY6" s="115">
         <f t="shared" si="3"/>
         <v>41116</v>
       </c>
-      <c r="AZ6" s="111">
+      <c r="AZ6" s="115">
         <f t="shared" si="3"/>
         <v>41117</v>
       </c>
-      <c r="BA6" s="111">
+      <c r="BA6" s="115">
         <f t="shared" si="3"/>
         <v>41120</v>
       </c>
-      <c r="BB6" s="111">
+      <c r="BB6" s="115">
         <f t="shared" si="3"/>
         <v>41121</v>
       </c>
-      <c r="BC6" s="111">
+      <c r="BC6" s="115">
         <f t="shared" si="3"/>
         <v>41122</v>
       </c>
-      <c r="BD6" s="111">
+      <c r="BD6" s="115">
         <f t="shared" si="3"/>
         <v>41123</v>
       </c>
-      <c r="BE6" s="111">
+      <c r="BE6" s="115">
         <f t="shared" si="3"/>
         <v>41124</v>
       </c>
-      <c r="BF6" s="111">
+      <c r="BF6" s="115">
         <f t="shared" si="3"/>
         <v>41127</v>
       </c>
-      <c r="BG6" s="111">
+      <c r="BG6" s="115">
         <f t="shared" si="3"/>
         <v>41128</v>
       </c>
-      <c r="BH6" s="111">
+      <c r="BH6" s="115">
         <f t="shared" si="3"/>
         <v>41129</v>
       </c>
-      <c r="BI6" s="111">
+      <c r="BI6" s="115">
         <f t="shared" si="3"/>
         <v>41130</v>
       </c>
-      <c r="BJ6" s="111">
+      <c r="BJ6" s="115">
         <f t="shared" si="3"/>
         <v>41131</v>
       </c>
-      <c r="BK6" s="111">
+      <c r="BK6" s="115">
         <f t="shared" si="3"/>
         <v>41134</v>
       </c>
-      <c r="BL6" s="111">
+      <c r="BL6" s="115">
         <f t="shared" si="3"/>
         <v>41135</v>
       </c>
-      <c r="BM6" s="111">
+      <c r="BM6" s="115">
         <f t="shared" si="3"/>
         <v>41136</v>
       </c>
-      <c r="BN6" s="111">
+      <c r="BN6" s="115">
         <f t="shared" si="3"/>
         <v>41137</v>
       </c>
-      <c r="BO6" s="111">
+      <c r="BO6" s="115">
         <f t="shared" si="3"/>
         <v>41138</v>
       </c>
-      <c r="BP6" s="111">
+      <c r="BP6" s="115">
         <f t="shared" si="3"/>
         <v>41141</v>
       </c>
-      <c r="BQ6" s="111">
+      <c r="BQ6" s="115">
         <f t="shared" si="3"/>
         <v>41142</v>
       </c>
-      <c r="BR6" s="111">
+      <c r="BR6" s="115">
         <f t="shared" si="3"/>
         <v>41143</v>
       </c>
-      <c r="BS6" s="111">
+      <c r="BS6" s="115">
         <f t="shared" si="3"/>
         <v>41144</v>
       </c>
-      <c r="BT6" s="111">
+      <c r="BT6" s="115">
         <f t="shared" si="3"/>
         <v>41145</v>
       </c>
-      <c r="BU6" s="111">
+      <c r="BU6" s="115">
         <f t="shared" si="3"/>
         <v>41148</v>
       </c>
-      <c r="BV6" s="111">
+      <c r="BV6" s="115">
         <f t="shared" si="3"/>
         <v>41149</v>
       </c>
-      <c r="BW6" s="111">
+      <c r="BW6" s="115">
         <f t="shared" si="3"/>
         <v>41150</v>
       </c>
-      <c r="BX6" s="111">
+      <c r="BX6" s="115">
         <f t="shared" si="3"/>
         <v>41151</v>
       </c>
-      <c r="BY6" s="111">
+      <c r="BY6" s="115">
         <f t="shared" si="3"/>
         <v>41152</v>
       </c>
-      <c r="BZ6" s="111">
+      <c r="BZ6" s="115">
         <f t="shared" si="3"/>
         <v>41155</v>
       </c>
-      <c r="CA6" s="111">
+      <c r="CA6" s="115">
         <f t="shared" si="3"/>
         <v>41156</v>
       </c>
-      <c r="CB6" s="111">
+      <c r="CB6" s="115">
         <f t="shared" si="3"/>
         <v>41157</v>
       </c>
-      <c r="CC6" s="111">
+      <c r="CC6" s="115">
         <f t="shared" si="3"/>
         <v>41158</v>
       </c>
-      <c r="CD6" s="111">
+      <c r="CD6" s="115">
         <f t="shared" si="3"/>
         <v>41159</v>
       </c>
-      <c r="CE6" s="111">
+      <c r="CE6" s="115">
         <f t="shared" si="3"/>
         <v>41162</v>
       </c>
-      <c r="CF6" s="111">
+      <c r="CF6" s="115">
         <f t="shared" si="3"/>
         <v>41163</v>
       </c>
-      <c r="CG6" s="111">
+      <c r="CG6" s="115">
         <f t="shared" si="3"/>
         <v>41164</v>
       </c>
-      <c r="CH6" s="111">
+      <c r="CH6" s="115">
         <f t="shared" si="3"/>
         <v>41165</v>
       </c>
-      <c r="CI6" s="111">
+      <c r="CI6" s="115">
         <f t="shared" si="3"/>
         <v>41166</v>
       </c>
-      <c r="CJ6" s="111">
+      <c r="CJ6" s="115">
         <f t="shared" si="3"/>
         <v>41169</v>
       </c>
-      <c r="CK6" s="111">
+      <c r="CK6" s="115">
         <f t="shared" si="3"/>
         <v>41170</v>
       </c>
-      <c r="CL6" s="111">
+      <c r="CL6" s="115">
         <f t="shared" si="3"/>
         <v>41171</v>
       </c>
-      <c r="CM6" s="111">
+      <c r="CM6" s="115">
         <f t="shared" si="3"/>
         <v>41172</v>
       </c>
-      <c r="CN6" s="111">
+      <c r="CN6" s="115">
         <f t="shared" si="3"/>
         <v>41173</v>
       </c>
-      <c r="CO6" s="111">
+      <c r="CO6" s="115">
         <f t="shared" si="3"/>
         <v>41176</v>
       </c>
-      <c r="CP6" s="111">
+      <c r="CP6" s="115">
         <f t="shared" si="3"/>
         <v>41177</v>
       </c>
-      <c r="CQ6" s="111">
+      <c r="CQ6" s="115">
         <f t="shared" si="3"/>
         <v>41178</v>
       </c>
-      <c r="CR6" s="111">
+      <c r="CR6" s="115">
         <f t="shared" si="3"/>
         <v>41179</v>
       </c>
-      <c r="CS6" s="111">
+      <c r="CS6" s="115">
         <f t="shared" si="3"/>
         <v>41180</v>
       </c>
@@ -6059,100 +6051,100 @@
     </row>
     <row r="7" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
+      <c r="B7" s="122"/>
+      <c r="C7" s="122"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
-      <c r="J7" s="112"/>
-      <c r="K7" s="112"/>
-      <c r="L7" s="112"/>
-      <c r="M7" s="112"/>
-      <c r="N7" s="112"/>
-      <c r="O7" s="112"/>
-      <c r="P7" s="112"/>
-      <c r="Q7" s="112"/>
-      <c r="R7" s="112"/>
-      <c r="S7" s="112"/>
-      <c r="T7" s="112"/>
-      <c r="U7" s="112"/>
-      <c r="V7" s="112"/>
-      <c r="W7" s="112"/>
-      <c r="X7" s="112"/>
-      <c r="Y7" s="112"/>
-      <c r="Z7" s="112"/>
-      <c r="AA7" s="112"/>
-      <c r="AB7" s="112"/>
-      <c r="AC7" s="112"/>
-      <c r="AD7" s="112"/>
-      <c r="AE7" s="112"/>
-      <c r="AF7" s="112"/>
-      <c r="AG7" s="112"/>
-      <c r="AH7" s="112"/>
-      <c r="AI7" s="112"/>
-      <c r="AJ7" s="112"/>
-      <c r="AK7" s="112"/>
-      <c r="AL7" s="112"/>
-      <c r="AM7" s="112"/>
-      <c r="AN7" s="112"/>
-      <c r="AO7" s="112"/>
-      <c r="AP7" s="112"/>
-      <c r="AQ7" s="112"/>
-      <c r="AR7" s="112"/>
-      <c r="AS7" s="112"/>
-      <c r="AT7" s="112"/>
-      <c r="AU7" s="112"/>
-      <c r="AV7" s="112"/>
-      <c r="AW7" s="112"/>
-      <c r="AX7" s="112"/>
-      <c r="AY7" s="112"/>
-      <c r="AZ7" s="112"/>
-      <c r="BA7" s="112"/>
-      <c r="BB7" s="112"/>
-      <c r="BC7" s="112"/>
-      <c r="BD7" s="112"/>
-      <c r="BE7" s="112"/>
-      <c r="BF7" s="112"/>
-      <c r="BG7" s="112"/>
-      <c r="BH7" s="112"/>
-      <c r="BI7" s="112"/>
-      <c r="BJ7" s="112"/>
-      <c r="BK7" s="112"/>
-      <c r="BL7" s="112"/>
-      <c r="BM7" s="112"/>
-      <c r="BN7" s="112"/>
-      <c r="BO7" s="112"/>
-      <c r="BP7" s="112"/>
-      <c r="BQ7" s="112"/>
-      <c r="BR7" s="112"/>
-      <c r="BS7" s="112"/>
-      <c r="BT7" s="112"/>
-      <c r="BU7" s="112"/>
-      <c r="BV7" s="112"/>
-      <c r="BW7" s="112"/>
-      <c r="BX7" s="112"/>
-      <c r="BY7" s="112"/>
-      <c r="BZ7" s="112"/>
-      <c r="CA7" s="112"/>
-      <c r="CB7" s="112"/>
-      <c r="CC7" s="112"/>
-      <c r="CD7" s="112"/>
-      <c r="CE7" s="112"/>
-      <c r="CF7" s="112"/>
-      <c r="CG7" s="112"/>
-      <c r="CH7" s="112"/>
-      <c r="CI7" s="112"/>
-      <c r="CJ7" s="112"/>
-      <c r="CK7" s="112"/>
-      <c r="CL7" s="112"/>
-      <c r="CM7" s="112"/>
-      <c r="CN7" s="112"/>
-      <c r="CO7" s="112"/>
-      <c r="CP7" s="112"/>
-      <c r="CQ7" s="112"/>
-      <c r="CR7" s="112"/>
-      <c r="CS7" s="112"/>
+      <c r="H7" s="116"/>
+      <c r="I7" s="116"/>
+      <c r="J7" s="116"/>
+      <c r="K7" s="116"/>
+      <c r="L7" s="116"/>
+      <c r="M7" s="116"/>
+      <c r="N7" s="116"/>
+      <c r="O7" s="116"/>
+      <c r="P7" s="116"/>
+      <c r="Q7" s="116"/>
+      <c r="R7" s="116"/>
+      <c r="S7" s="116"/>
+      <c r="T7" s="116"/>
+      <c r="U7" s="116"/>
+      <c r="V7" s="116"/>
+      <c r="W7" s="116"/>
+      <c r="X7" s="116"/>
+      <c r="Y7" s="116"/>
+      <c r="Z7" s="116"/>
+      <c r="AA7" s="116"/>
+      <c r="AB7" s="116"/>
+      <c r="AC7" s="116"/>
+      <c r="AD7" s="116"/>
+      <c r="AE7" s="116"/>
+      <c r="AF7" s="116"/>
+      <c r="AG7" s="116"/>
+      <c r="AH7" s="116"/>
+      <c r="AI7" s="116"/>
+      <c r="AJ7" s="116"/>
+      <c r="AK7" s="116"/>
+      <c r="AL7" s="116"/>
+      <c r="AM7" s="116"/>
+      <c r="AN7" s="116"/>
+      <c r="AO7" s="116"/>
+      <c r="AP7" s="116"/>
+      <c r="AQ7" s="116"/>
+      <c r="AR7" s="116"/>
+      <c r="AS7" s="116"/>
+      <c r="AT7" s="116"/>
+      <c r="AU7" s="116"/>
+      <c r="AV7" s="116"/>
+      <c r="AW7" s="116"/>
+      <c r="AX7" s="116"/>
+      <c r="AY7" s="116"/>
+      <c r="AZ7" s="116"/>
+      <c r="BA7" s="116"/>
+      <c r="BB7" s="116"/>
+      <c r="BC7" s="116"/>
+      <c r="BD7" s="116"/>
+      <c r="BE7" s="116"/>
+      <c r="BF7" s="116"/>
+      <c r="BG7" s="116"/>
+      <c r="BH7" s="116"/>
+      <c r="BI7" s="116"/>
+      <c r="BJ7" s="116"/>
+      <c r="BK7" s="116"/>
+      <c r="BL7" s="116"/>
+      <c r="BM7" s="116"/>
+      <c r="BN7" s="116"/>
+      <c r="BO7" s="116"/>
+      <c r="BP7" s="116"/>
+      <c r="BQ7" s="116"/>
+      <c r="BR7" s="116"/>
+      <c r="BS7" s="116"/>
+      <c r="BT7" s="116"/>
+      <c r="BU7" s="116"/>
+      <c r="BV7" s="116"/>
+      <c r="BW7" s="116"/>
+      <c r="BX7" s="116"/>
+      <c r="BY7" s="116"/>
+      <c r="BZ7" s="116"/>
+      <c r="CA7" s="116"/>
+      <c r="CB7" s="116"/>
+      <c r="CC7" s="116"/>
+      <c r="CD7" s="116"/>
+      <c r="CE7" s="116"/>
+      <c r="CF7" s="116"/>
+      <c r="CG7" s="116"/>
+      <c r="CH7" s="116"/>
+      <c r="CI7" s="116"/>
+      <c r="CJ7" s="116"/>
+      <c r="CK7" s="116"/>
+      <c r="CL7" s="116"/>
+      <c r="CM7" s="116"/>
+      <c r="CN7" s="116"/>
+      <c r="CO7" s="116"/>
+      <c r="CP7" s="116"/>
+      <c r="CQ7" s="116"/>
+      <c r="CR7" s="116"/>
+      <c r="CS7" s="116"/>
       <c r="CT7" s="13"/>
     </row>
     <row r="8" spans="1:98" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6168,18 +6160,18 @@
       </c>
     </row>
     <row r="10" spans="1:98" x14ac:dyDescent="0.25">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="114"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="118"/>
       <c r="D10" s="35">
         <f ca="1">MIN(D11:D18)</f>
-        <v>41066</v>
+        <v>41078</v>
       </c>
       <c r="E10" s="35">
         <f ca="1">MAX(E11:E18)</f>
-        <v>41094</v>
+        <v>41097</v>
       </c>
       <c r="F10" s="36"/>
       <c r="H10" s="4"/>
@@ -6383,11 +6375,11 @@
       <c r="C12" s="2"/>
       <c r="D12" s="14">
         <f ca="1">TODAY()</f>
-        <v>41066</v>
+        <v>41082</v>
       </c>
       <c r="E12" s="21">
         <f ca="1">D12+5+CHOOSE(WEEKDAY(D12+5,2),0,0,0,0,0,2,1)</f>
-        <v>41071</v>
+        <v>41087</v>
       </c>
       <c r="F12" s="37">
         <v>0.6</v>
@@ -6491,11 +6483,11 @@
       <c r="C13" s="2"/>
       <c r="D13" s="14">
         <f ca="1">E12+1</f>
-        <v>41072</v>
+        <v>41088</v>
       </c>
       <c r="E13" s="21">
         <f ca="1">D13+6+CHOOSE(WEEKDAY(D13+5,2),0,0,0,0,0,2,1)</f>
-        <v>41079</v>
+        <v>41094</v>
       </c>
       <c r="F13" s="37"/>
       <c r="H13" s="10"/>
@@ -6597,11 +6589,11 @@
       <c r="C14" s="2"/>
       <c r="D14" s="14">
         <f ca="1">E13</f>
-        <v>41079</v>
+        <v>41094</v>
       </c>
       <c r="E14" s="21">
         <f ca="1">D14+3</f>
-        <v>41082</v>
+        <v>41097</v>
       </c>
       <c r="F14" s="37"/>
       <c r="H14" s="10"/>
@@ -7196,18 +7188,18 @@
       <c r="CS19" s="3"/>
     </row>
     <row r="20" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="114"/>
-      <c r="C20" s="114"/>
-      <c r="D20" s="35">
+      <c r="B20" s="118"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="35" t="e">
         <f>MIN(D21:D28)</f>
-        <v>41095</v>
-      </c>
-      <c r="E20" s="35">
+        <v>#REF!</v>
+      </c>
+      <c r="E20" s="35" t="e">
         <f>MAX(E21:E28)</f>
-        <v>41124</v>
+        <v>#REF!</v>
       </c>
       <c r="F20" s="38"/>
       <c r="H20" s="11"/>
@@ -7311,8 +7303,8 @@
         <v>41095</v>
       </c>
       <c r="E21" s="24">
-        <f>D21+Versioning!E3+1</f>
-        <v>41096</v>
+        <f>D21+Versioning!E2+1</f>
+        <v>41107</v>
       </c>
       <c r="F21" s="30">
         <v>0.25</v>
@@ -7410,11 +7402,11 @@
       <c r="C22" s="2"/>
       <c r="D22" s="23">
         <f>E21</f>
-        <v>41096</v>
+        <v>41107</v>
       </c>
       <c r="E22" s="24">
         <f>D22+2++CHOOSE(WEEKDAY(D22+2,2),0,0,0,0,0,2,1)</f>
-        <v>41099</v>
+        <v>41109</v>
       </c>
       <c r="F22" s="30"/>
       <c r="H22" s="10"/>
@@ -7509,11 +7501,11 @@
       <c r="C23" s="2"/>
       <c r="D23" s="14">
         <f>E22+1+CHOOSE(WEEKDAY(E22+1,2),0,0,0,0,0,2,1)</f>
-        <v>41100</v>
+        <v>41110</v>
       </c>
       <c r="E23" s="24">
-        <f>D23+Versioning!E4-1</f>
-        <v>41099</v>
+        <f>D23+Versioning!E3-1</f>
+        <v>41109</v>
       </c>
       <c r="F23" s="30">
         <v>0.4</v>
@@ -7720,9 +7712,9 @@
         <f>E24+1</f>
         <v>41121</v>
       </c>
-      <c r="E25" s="24">
-        <f>D25+Versioning!E5+CHOOSE(WEEKDAY(D25+Versioning!E5,2),0,0,0,0,0,2,1)</f>
-        <v>41121</v>
+      <c r="E25" s="24" t="e">
+        <f>D25+Versioning!#REF!+CHOOSE(WEEKDAY(D25+Versioning!#REF!,2),0,0,0,0,0,2,1)</f>
+        <v>#REF!</v>
       </c>
       <c r="F25" s="31"/>
       <c r="H25" s="10"/>
@@ -7820,13 +7812,13 @@
         <v>28</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="14">
+      <c r="D26" s="14" t="e">
         <f>E25</f>
-        <v>41121</v>
-      </c>
-      <c r="E26" s="24">
+        <v>#REF!</v>
+      </c>
+      <c r="E26" s="24" t="e">
         <f>D26+2+CHOOSE(WEEKDAY(D26+3,2),0,0,0,0,0,2,1)</f>
-        <v>41123</v>
+        <v>#REF!</v>
       </c>
       <c r="F26" s="31"/>
       <c r="H26" s="10"/>
@@ -7923,13 +7915,13 @@
       <c r="C27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="14" t="e">
         <f>E26+1</f>
-        <v>41124</v>
-      </c>
-      <c r="E27" s="24">
-        <f>D27+Versioning!E6+CHOOSE(WEEKDAY(D27+Versioning!E6,2),0,0,0,0,0,2,1)</f>
-        <v>41124</v>
+        <v>#REF!</v>
+      </c>
+      <c r="E27" s="24" t="e">
+        <f>D27+Versioning!E4+CHOOSE(WEEKDAY(D27+Versioning!E4,2),0,0,0,0,0,2,1)</f>
+        <v>#REF!</v>
       </c>
       <c r="F27" s="31">
         <v>0</v>
@@ -8221,18 +8213,18 @@
       <c r="CS29" s="2"/>
     </row>
     <row r="30" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="113" t="s">
+      <c r="A30" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="35">
+      <c r="B30" s="118"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="35" t="e">
         <f>MIN(D31:D34)</f>
-        <v>41125</v>
-      </c>
-      <c r="E30" s="35">
+        <v>#REF!</v>
+      </c>
+      <c r="E30" s="35" t="e">
         <f>MAX(E31:E34)</f>
-        <v>41155</v>
+        <v>#REF!</v>
       </c>
       <c r="F30" s="38"/>
       <c r="H30" s="4"/>
@@ -8332,13 +8324,13 @@
         <v>25</v>
       </c>
       <c r="C31" s="2"/>
-      <c r="D31" s="23">
+      <c r="D31" s="23" t="e">
         <f>E27+1</f>
-        <v>41125</v>
-      </c>
-      <c r="E31" s="24">
+        <v>#REF!</v>
+      </c>
+      <c r="E31" s="24" t="e">
         <f>D31+7+CHOOSE(WEEKDAY(D31+7,2),0,0,0,0,0,2,1)</f>
-        <v>41134</v>
+        <v>#REF!</v>
       </c>
       <c r="F31" s="32">
         <v>0</v>
@@ -8440,13 +8432,13 @@
         <v>26</v>
       </c>
       <c r="C32" s="2"/>
-      <c r="D32" s="23">
+      <c r="D32" s="23" t="e">
         <f>E31+1</f>
-        <v>41135</v>
-      </c>
-      <c r="E32" s="24">
+        <v>#REF!</v>
+      </c>
+      <c r="E32" s="24" t="e">
         <f>D32+7+CHOOSE(WEEKDAY(D32+7,2),0,0,0,0,0,2,1)</f>
-        <v>41142</v>
+        <v>#REF!</v>
       </c>
       <c r="F32" s="30">
         <v>0</v>
@@ -8548,13 +8540,13 @@
         <v>27</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="23">
+      <c r="D33" s="23" t="e">
         <f>E32+1</f>
-        <v>41143</v>
-      </c>
-      <c r="E33" s="24">
+        <v>#REF!</v>
+      </c>
+      <c r="E33" s="24" t="e">
         <f>D33+10+CHOOSE(WEEKDAY(D33+10,2),0,0,0,0,0,2,1)</f>
-        <v>41155</v>
+        <v>#REF!</v>
       </c>
       <c r="F33" s="31">
         <v>0</v>
@@ -8759,18 +8751,18 @@
       <c r="BC35" s="79"/>
     </row>
     <row r="36" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="113" t="s">
+      <c r="A36" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="114"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="35">
+      <c r="B36" s="118"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="35" t="e">
         <f>MIN(D37:D42)</f>
-        <v>40308</v>
-      </c>
-      <c r="E36" s="35">
+        <v>#REF!</v>
+      </c>
+      <c r="E36" s="35" t="e">
         <f>MAX(E37:E42)</f>
-        <v>41189</v>
+        <v>#REF!</v>
       </c>
       <c r="F36" s="38"/>
       <c r="H36" s="11"/>
@@ -8870,13 +8862,13 @@
         <v>4</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="D37" s="23">
+      <c r="D37" s="23" t="e">
         <f>E33+1</f>
-        <v>41156</v>
-      </c>
-      <c r="E37" s="24">
+        <v>#REF!</v>
+      </c>
+      <c r="E37" s="24" t="e">
         <f>E38</f>
-        <v>41189</v>
+        <v>#REF!</v>
       </c>
       <c r="F37" s="32">
         <v>0</v>
@@ -8978,13 +8970,13 @@
       <c r="C38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="14" t="e">
         <f>D37+13</f>
-        <v>41169</v>
-      </c>
-      <c r="E38" s="21">
+        <v>#REF!</v>
+      </c>
+      <c r="E38" s="21" t="e">
         <f>D38+20</f>
-        <v>41189</v>
+        <v>#REF!</v>
       </c>
       <c r="F38" s="30">
         <v>0</v>
@@ -9599,11 +9591,11 @@
       <c r="CS43" s="2"/>
     </row>
     <row r="44" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="113" t="s">
+      <c r="A44" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
+      <c r="B44" s="118"/>
+      <c r="C44" s="118"/>
       <c r="D44" s="35">
         <f>MIN(D45:D49)</f>
         <v>40364</v>
@@ -10890,207 +10882,154 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.28515625" style="39" customWidth="1"/>
     <col min="2" max="2" width="87.140625" style="40" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="122" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" style="120" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="107" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" style="105" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" style="124" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="121" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+    <row r="1" spans="1:6" s="106" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="104" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="122" t="s">
         <v>32</v>
+      </c>
+      <c r="C1" s="107" t="s">
+        <v>42</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="40"/>
+      <c r="E1" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="123" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="122">
-        <v>15</v>
-      </c>
-      <c r="D2" s="120">
-        <f ca="1">TODAY()+C2</f>
+      <c r="C2" s="107">
+        <v>8</v>
+      </c>
+      <c r="D2" s="105">
+        <f>(DATE(2012,6,10)+$C2+$C2/7)+IF(WEEKDAY((DATE(2012,6,10)+$C2+$C2/7),2)=6,2,0)+IF(WEEKDAY((DATE(2012,6,10)+$C2+$C2/7),2)=7,1,0)</f>
+        <v>41079.142857142855</v>
+      </c>
+      <c r="E2" s="44">
+        <f>F2-DATE(2012,6,10)</f>
+        <v>11</v>
+      </c>
+      <c r="F2" s="105">
         <v>41081</v>
       </c>
-      <c r="E2" s="44" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="122">
-        <v>8</v>
-      </c>
-      <c r="D3" s="120">
-        <f ca="1">D2+C3</f>
-        <v>41089</v>
+      <c r="C3" s="107">
+        <v>5</v>
+      </c>
+      <c r="D3" s="105">
+        <f>($D2+$C3+$C3/7)+IF(WEEKDAY(($D2+$C3+$C3/7),2)=6,2,0)+IF(WEEKDAY(($D2+$C3+$C3/7),2)=7,1,0)</f>
+        <v>41085.857142857138</v>
       </c>
       <c r="E3" s="44"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="122">
-        <v>5</v>
-      </c>
-      <c r="D4" s="120">
-        <f t="shared" ref="D4:D12" ca="1" si="0">D3+C4</f>
-        <v>41094</v>
+        <v>36</v>
+      </c>
+      <c r="C4" s="107">
+        <v>7</v>
+      </c>
+      <c r="D4" s="105">
+        <f t="shared" ref="D4:D8" si="0">($D3+$C4+$C4/7)+IF(WEEKDAY(($D3+$C4+$C4/7),2)=6,2,0)+IF(WEEKDAY(($D3+$C4+$C4/7),2)=7,1,0)</f>
+        <v>41093.857142857138</v>
       </c>
       <c r="E4" s="44"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="B5" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="107">
+        <v>7</v>
+      </c>
+      <c r="D5" s="105">
+        <f t="shared" si="0"/>
+        <v>41101.857142857138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="122">
+      <c r="C6" s="107">
         <v>5</v>
       </c>
-      <c r="D5" s="120">
-        <f t="shared" ca="1" si="0"/>
-        <v>41099</v>
-      </c>
-      <c r="E5" s="44"/>
+      <c r="D6" s="105">
+        <f t="shared" si="0"/>
+        <v>41107.57142857142</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="40" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="122">
-        <v>7</v>
-      </c>
-      <c r="D6" s="120">
-        <f t="shared" ca="1" si="0"/>
-        <v>41106</v>
-      </c>
-      <c r="E6" s="44"/>
+      <c r="B7" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="107">
+        <v>5</v>
+      </c>
+      <c r="D7" s="105">
+        <f t="shared" si="0"/>
+        <v>41113.285714285703</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="40" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="122">
+      <c r="C8" s="107">
         <v>5</v>
       </c>
-      <c r="D7" s="120">
-        <f t="shared" ca="1" si="0"/>
-        <v>41111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="122">
-        <v>3</v>
-      </c>
-      <c r="D8" s="120">
-        <f t="shared" ca="1" si="0"/>
-        <v>41114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="122">
-        <v>5</v>
-      </c>
-      <c r="D9" s="120">
-        <f ca="1">D8+C9</f>
-        <v>41119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="122">
-        <v>5</v>
-      </c>
-      <c r="D10" s="120">
-        <f t="shared" ca="1" si="0"/>
-        <v>41124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="122">
-        <v>3</v>
-      </c>
-      <c r="D11" s="120">
-        <f t="shared" ca="1" si="0"/>
-        <v>41127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="122">
-        <v>3</v>
-      </c>
-      <c r="D12" s="120">
-        <f t="shared" ca="1" si="0"/>
-        <v>41130</v>
+      <c r="D8" s="105">
+        <f t="shared" si="0"/>
+        <v>41119.999999999985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the formula for gannt chart
</commit_message>
<xml_diff>
--- a/Documentation/Gannt Chart.xlsx
+++ b/Documentation/Gannt Chart.xlsx
@@ -1050,7 +1050,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1281,33 +1281,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1326,10 +1299,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5004,10 +5003,10 @@
     <row r="1" spans="1:98" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:98" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="110" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="120"/>
+      <c r="C2" s="111"/>
       <c r="D2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5015,105 +5014,105 @@
         <v>1</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="H2" s="111" t="s">
+      <c r="H2" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="P2" s="112"/>
-      <c r="Q2" s="112"/>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="112"/>
-      <c r="X2" s="112"/>
-      <c r="Y2" s="112"/>
-      <c r="Z2" s="112"/>
-      <c r="AA2" s="112"/>
-      <c r="AB2" s="112"/>
-      <c r="AC2" s="112"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="112"/>
-      <c r="AF2" s="112"/>
-      <c r="AG2" s="112"/>
-      <c r="AH2" s="112"/>
-      <c r="AI2" s="112"/>
-      <c r="AJ2" s="112"/>
-      <c r="AK2" s="112"/>
-      <c r="AL2" s="112"/>
-      <c r="AM2" s="112"/>
-      <c r="AN2" s="112"/>
-      <c r="AO2" s="112"/>
-      <c r="AP2" s="112"/>
-      <c r="AQ2" s="112"/>
-      <c r="AR2" s="112"/>
-      <c r="AS2" s="112"/>
-      <c r="AT2" s="112"/>
-      <c r="AU2" s="112"/>
-      <c r="AV2" s="112"/>
-      <c r="AW2" s="112"/>
-      <c r="AX2" s="112"/>
-      <c r="AY2" s="112"/>
-      <c r="AZ2" s="112"/>
-      <c r="BA2" s="112"/>
-      <c r="BB2" s="112"/>
-      <c r="BC2" s="112"/>
-      <c r="BD2" s="112"/>
-      <c r="BE2" s="112"/>
-      <c r="BF2" s="112"/>
-      <c r="BG2" s="112"/>
-      <c r="BH2" s="112"/>
-      <c r="BI2" s="112"/>
-      <c r="BJ2" s="112"/>
-      <c r="BK2" s="112"/>
-      <c r="BL2" s="112"/>
-      <c r="BM2" s="112"/>
-      <c r="BN2" s="112"/>
-      <c r="BO2" s="112"/>
-      <c r="BP2" s="112"/>
-      <c r="BQ2" s="112"/>
-      <c r="BR2" s="112"/>
-      <c r="BS2" s="112"/>
-      <c r="BT2" s="112"/>
-      <c r="BU2" s="112"/>
-      <c r="BV2" s="112"/>
-      <c r="BW2" s="112"/>
-      <c r="BX2" s="112"/>
-      <c r="BY2" s="112"/>
-      <c r="BZ2" s="112"/>
-      <c r="CA2" s="112"/>
-      <c r="CB2" s="112"/>
-      <c r="CC2" s="112"/>
-      <c r="CD2" s="112"/>
-      <c r="CE2" s="112"/>
-      <c r="CF2" s="112"/>
-      <c r="CG2" s="112"/>
-      <c r="CH2" s="112"/>
-      <c r="CI2" s="112"/>
-      <c r="CJ2" s="112"/>
-      <c r="CK2" s="112"/>
-      <c r="CL2" s="112"/>
-      <c r="CM2" s="112"/>
-      <c r="CN2" s="112"/>
-      <c r="CO2" s="112"/>
-      <c r="CP2" s="112"/>
-      <c r="CQ2" s="112"/>
-      <c r="CR2" s="112"/>
-      <c r="CS2" s="112"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="118"/>
+      <c r="W2" s="118"/>
+      <c r="X2" s="118"/>
+      <c r="Y2" s="118"/>
+      <c r="Z2" s="118"/>
+      <c r="AA2" s="118"/>
+      <c r="AB2" s="118"/>
+      <c r="AC2" s="118"/>
+      <c r="AD2" s="118"/>
+      <c r="AE2" s="118"/>
+      <c r="AF2" s="118"/>
+      <c r="AG2" s="118"/>
+      <c r="AH2" s="118"/>
+      <c r="AI2" s="118"/>
+      <c r="AJ2" s="118"/>
+      <c r="AK2" s="118"/>
+      <c r="AL2" s="118"/>
+      <c r="AM2" s="118"/>
+      <c r="AN2" s="118"/>
+      <c r="AO2" s="118"/>
+      <c r="AP2" s="118"/>
+      <c r="AQ2" s="118"/>
+      <c r="AR2" s="118"/>
+      <c r="AS2" s="118"/>
+      <c r="AT2" s="118"/>
+      <c r="AU2" s="118"/>
+      <c r="AV2" s="118"/>
+      <c r="AW2" s="118"/>
+      <c r="AX2" s="118"/>
+      <c r="AY2" s="118"/>
+      <c r="AZ2" s="118"/>
+      <c r="BA2" s="118"/>
+      <c r="BB2" s="118"/>
+      <c r="BC2" s="118"/>
+      <c r="BD2" s="118"/>
+      <c r="BE2" s="118"/>
+      <c r="BF2" s="118"/>
+      <c r="BG2" s="118"/>
+      <c r="BH2" s="118"/>
+      <c r="BI2" s="118"/>
+      <c r="BJ2" s="118"/>
+      <c r="BK2" s="118"/>
+      <c r="BL2" s="118"/>
+      <c r="BM2" s="118"/>
+      <c r="BN2" s="118"/>
+      <c r="BO2" s="118"/>
+      <c r="BP2" s="118"/>
+      <c r="BQ2" s="118"/>
+      <c r="BR2" s="118"/>
+      <c r="BS2" s="118"/>
+      <c r="BT2" s="118"/>
+      <c r="BU2" s="118"/>
+      <c r="BV2" s="118"/>
+      <c r="BW2" s="118"/>
+      <c r="BX2" s="118"/>
+      <c r="BY2" s="118"/>
+      <c r="BZ2" s="118"/>
+      <c r="CA2" s="118"/>
+      <c r="CB2" s="118"/>
+      <c r="CC2" s="118"/>
+      <c r="CD2" s="118"/>
+      <c r="CE2" s="118"/>
+      <c r="CF2" s="118"/>
+      <c r="CG2" s="118"/>
+      <c r="CH2" s="118"/>
+      <c r="CI2" s="118"/>
+      <c r="CJ2" s="118"/>
+      <c r="CK2" s="118"/>
+      <c r="CL2" s="118"/>
+      <c r="CM2" s="118"/>
+      <c r="CN2" s="118"/>
+      <c r="CO2" s="118"/>
+      <c r="CP2" s="118"/>
+      <c r="CQ2" s="118"/>
+      <c r="CR2" s="118"/>
+      <c r="CS2" s="118"/>
     </row>
     <row r="3" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="121"/>
+      <c r="C3" s="112"/>
       <c r="D3" s="14">
         <v>41112</v>
       </c>
@@ -5121,461 +5120,461 @@
         <v>41115</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="114"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="114"/>
-      <c r="U3" s="114"/>
-      <c r="V3" s="114"/>
-      <c r="W3" s="114"/>
-      <c r="X3" s="114"/>
-      <c r="Y3" s="114"/>
-      <c r="Z3" s="114"/>
-      <c r="AA3" s="114"/>
-      <c r="AB3" s="114"/>
-      <c r="AC3" s="114"/>
-      <c r="AD3" s="114"/>
-      <c r="AE3" s="114"/>
-      <c r="AF3" s="114"/>
-      <c r="AG3" s="114"/>
-      <c r="AH3" s="114"/>
-      <c r="AI3" s="114"/>
-      <c r="AJ3" s="114"/>
-      <c r="AK3" s="114"/>
-      <c r="AL3" s="114"/>
-      <c r="AM3" s="114"/>
-      <c r="AN3" s="114"/>
-      <c r="AO3" s="114"/>
-      <c r="AP3" s="114"/>
-      <c r="AQ3" s="114"/>
-      <c r="AR3" s="114"/>
-      <c r="AS3" s="114"/>
-      <c r="AT3" s="114"/>
-      <c r="AU3" s="114"/>
-      <c r="AV3" s="114"/>
-      <c r="AW3" s="114"/>
-      <c r="AX3" s="114"/>
-      <c r="AY3" s="114"/>
-      <c r="AZ3" s="114"/>
-      <c r="BA3" s="114"/>
-      <c r="BB3" s="114"/>
-      <c r="BC3" s="114"/>
-      <c r="BD3" s="114"/>
-      <c r="BE3" s="114"/>
-      <c r="BF3" s="114"/>
-      <c r="BG3" s="114"/>
-      <c r="BH3" s="114"/>
-      <c r="BI3" s="114"/>
-      <c r="BJ3" s="114"/>
-      <c r="BK3" s="114"/>
-      <c r="BL3" s="114"/>
-      <c r="BM3" s="114"/>
-      <c r="BN3" s="114"/>
-      <c r="BO3" s="114"/>
-      <c r="BP3" s="114"/>
-      <c r="BQ3" s="114"/>
-      <c r="BR3" s="114"/>
-      <c r="BS3" s="114"/>
-      <c r="BT3" s="114"/>
-      <c r="BU3" s="114"/>
-      <c r="BV3" s="114"/>
-      <c r="BW3" s="114"/>
-      <c r="BX3" s="114"/>
-      <c r="BY3" s="114"/>
-      <c r="BZ3" s="114"/>
-      <c r="CA3" s="114"/>
-      <c r="CB3" s="114"/>
-      <c r="CC3" s="114"/>
-      <c r="CD3" s="114"/>
-      <c r="CE3" s="114"/>
-      <c r="CF3" s="114"/>
-      <c r="CG3" s="114"/>
-      <c r="CH3" s="114"/>
-      <c r="CI3" s="114"/>
-      <c r="CJ3" s="114"/>
-      <c r="CK3" s="114"/>
-      <c r="CL3" s="114"/>
-      <c r="CM3" s="114"/>
-      <c r="CN3" s="114"/>
-      <c r="CO3" s="114"/>
-      <c r="CP3" s="114"/>
-      <c r="CQ3" s="114"/>
-      <c r="CR3" s="114"/>
-      <c r="CS3" s="114"/>
+      <c r="H3" s="119"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="120"/>
+      <c r="R3" s="120"/>
+      <c r="S3" s="120"/>
+      <c r="T3" s="120"/>
+      <c r="U3" s="120"/>
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
+      <c r="X3" s="120"/>
+      <c r="Y3" s="120"/>
+      <c r="Z3" s="120"/>
+      <c r="AA3" s="120"/>
+      <c r="AB3" s="120"/>
+      <c r="AC3" s="120"/>
+      <c r="AD3" s="120"/>
+      <c r="AE3" s="120"/>
+      <c r="AF3" s="120"/>
+      <c r="AG3" s="120"/>
+      <c r="AH3" s="120"/>
+      <c r="AI3" s="120"/>
+      <c r="AJ3" s="120"/>
+      <c r="AK3" s="120"/>
+      <c r="AL3" s="120"/>
+      <c r="AM3" s="120"/>
+      <c r="AN3" s="120"/>
+      <c r="AO3" s="120"/>
+      <c r="AP3" s="120"/>
+      <c r="AQ3" s="120"/>
+      <c r="AR3" s="120"/>
+      <c r="AS3" s="120"/>
+      <c r="AT3" s="120"/>
+      <c r="AU3" s="120"/>
+      <c r="AV3" s="120"/>
+      <c r="AW3" s="120"/>
+      <c r="AX3" s="120"/>
+      <c r="AY3" s="120"/>
+      <c r="AZ3" s="120"/>
+      <c r="BA3" s="120"/>
+      <c r="BB3" s="120"/>
+      <c r="BC3" s="120"/>
+      <c r="BD3" s="120"/>
+      <c r="BE3" s="120"/>
+      <c r="BF3" s="120"/>
+      <c r="BG3" s="120"/>
+      <c r="BH3" s="120"/>
+      <c r="BI3" s="120"/>
+      <c r="BJ3" s="120"/>
+      <c r="BK3" s="120"/>
+      <c r="BL3" s="120"/>
+      <c r="BM3" s="120"/>
+      <c r="BN3" s="120"/>
+      <c r="BO3" s="120"/>
+      <c r="BP3" s="120"/>
+      <c r="BQ3" s="120"/>
+      <c r="BR3" s="120"/>
+      <c r="BS3" s="120"/>
+      <c r="BT3" s="120"/>
+      <c r="BU3" s="120"/>
+      <c r="BV3" s="120"/>
+      <c r="BW3" s="120"/>
+      <c r="BX3" s="120"/>
+      <c r="BY3" s="120"/>
+      <c r="BZ3" s="120"/>
+      <c r="CA3" s="120"/>
+      <c r="CB3" s="120"/>
+      <c r="CC3" s="120"/>
+      <c r="CD3" s="120"/>
+      <c r="CE3" s="120"/>
+      <c r="CF3" s="120"/>
+      <c r="CG3" s="120"/>
+      <c r="CH3" s="120"/>
+      <c r="CI3" s="120"/>
+      <c r="CJ3" s="120"/>
+      <c r="CK3" s="120"/>
+      <c r="CL3" s="120"/>
+      <c r="CM3" s="120"/>
+      <c r="CN3" s="120"/>
+      <c r="CO3" s="120"/>
+      <c r="CP3" s="120"/>
+      <c r="CQ3" s="120"/>
+      <c r="CR3" s="120"/>
+      <c r="CS3" s="120"/>
     </row>
     <row r="4" spans="1:98" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="122"/>
-      <c r="C4" s="122"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
       <c r="D4" s="14"/>
       <c r="E4" s="15"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="108">
+      <c r="H4" s="116">
         <f>IF(MONTH(H6)&lt;&gt;MONTH(E6),H6,"")</f>
         <v>41057</v>
       </c>
-      <c r="I4" s="108" t="str">
+      <c r="I4" s="116" t="str">
         <f t="shared" ref="I4:BT4" si="0">IF(MONTH(I6)&lt;&gt;MONTH(H6),I6,"")</f>
         <v/>
       </c>
-      <c r="J4" s="108" t="str">
+      <c r="J4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K4" s="108" t="str">
+      <c r="K4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L4" s="108">
+      <c r="L4" s="116">
         <f t="shared" si="0"/>
         <v>41061</v>
       </c>
-      <c r="M4" s="109" t="str">
+      <c r="M4" s="121" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N4" s="109" t="str">
+      <c r="N4" s="121" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="O4" s="108" t="str">
+      <c r="O4" s="116" t="str">
         <f>IF(MONTH(O6)&lt;&gt;MONTH(N6),O6,"")</f>
         <v/>
       </c>
-      <c r="P4" s="108" t="str">
+      <c r="P4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q4" s="108" t="str">
+      <c r="Q4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R4" s="108" t="str">
+      <c r="R4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="S4" s="108" t="str">
+      <c r="S4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="T4" s="108" t="str">
+      <c r="T4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="U4" s="108" t="str">
+      <c r="U4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="V4" s="108" t="str">
+      <c r="V4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="W4" s="108" t="str">
+      <c r="W4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="X4" s="108" t="str">
+      <c r="X4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Y4" s="108" t="str">
+      <c r="Y4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Z4" s="108" t="str">
+      <c r="Z4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AA4" s="108" t="str">
+      <c r="AA4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AB4" s="108" t="str">
+      <c r="AB4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AC4" s="108" t="str">
+      <c r="AC4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AD4" s="108" t="str">
+      <c r="AD4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE4" s="108" t="str">
+      <c r="AE4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AF4" s="108" t="str">
+      <c r="AF4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AG4" s="108">
+      <c r="AG4" s="116">
         <f t="shared" si="0"/>
         <v>41092</v>
       </c>
-      <c r="AH4" s="108" t="str">
+      <c r="AH4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AI4" s="108" t="str">
+      <c r="AI4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AJ4" s="108" t="str">
+      <c r="AJ4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AK4" s="108" t="str">
+      <c r="AK4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AL4" s="108" t="str">
+      <c r="AL4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AM4" s="108" t="str">
+      <c r="AM4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AN4" s="108" t="str">
+      <c r="AN4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AO4" s="108" t="str">
+      <c r="AO4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AP4" s="108" t="str">
+      <c r="AP4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AQ4" s="108" t="str">
+      <c r="AQ4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AR4" s="108" t="str">
+      <c r="AR4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AS4" s="108" t="str">
+      <c r="AS4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AT4" s="108" t="str">
+      <c r="AT4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AU4" s="108" t="str">
+      <c r="AU4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AV4" s="108" t="str">
+      <c r="AV4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AW4" s="108" t="str">
+      <c r="AW4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AX4" s="108" t="str">
+      <c r="AX4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AY4" s="108" t="str">
+      <c r="AY4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AZ4" s="108" t="str">
+      <c r="AZ4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BA4" s="108" t="str">
+      <c r="BA4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BB4" s="108" t="str">
+      <c r="BB4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BC4" s="108">
+      <c r="BC4" s="116">
         <f t="shared" si="0"/>
         <v>41122</v>
       </c>
-      <c r="BD4" s="108" t="str">
+      <c r="BD4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BE4" s="108" t="str">
+      <c r="BE4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BF4" s="108" t="str">
+      <c r="BF4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BG4" s="108" t="str">
+      <c r="BG4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BH4" s="108" t="str">
+      <c r="BH4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BI4" s="108" t="str">
+      <c r="BI4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BJ4" s="108" t="str">
+      <c r="BJ4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BK4" s="108" t="str">
+      <c r="BK4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BL4" s="108" t="str">
+      <c r="BL4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BM4" s="108" t="str">
+      <c r="BM4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BN4" s="108" t="str">
+      <c r="BN4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BO4" s="108" t="str">
+      <c r="BO4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BP4" s="108" t="str">
+      <c r="BP4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BQ4" s="108" t="str">
+      <c r="BQ4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BR4" s="108" t="str">
+      <c r="BR4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BS4" s="108" t="str">
+      <c r="BS4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BT4" s="108" t="str">
+      <c r="BT4" s="116" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="BU4" s="108" t="str">
+      <c r="BU4" s="116" t="str">
         <f t="shared" ref="BU4:CS4" si="1">IF(MONTH(BU6)&lt;&gt;MONTH(BT6),BU6,"")</f>
         <v/>
       </c>
-      <c r="BV4" s="108" t="str">
+      <c r="BV4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BW4" s="108" t="str">
+      <c r="BW4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BX4" s="108" t="str">
+      <c r="BX4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BY4" s="108" t="str">
+      <c r="BY4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="BZ4" s="108">
+      <c r="BZ4" s="116">
         <f t="shared" si="1"/>
         <v>41155</v>
       </c>
-      <c r="CA4" s="108" t="str">
+      <c r="CA4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CB4" s="108" t="str">
+      <c r="CB4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CC4" s="108" t="str">
+      <c r="CC4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CD4" s="108" t="str">
+      <c r="CD4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CE4" s="108" t="str">
+      <c r="CE4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CF4" s="108" t="str">
+      <c r="CF4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CG4" s="108" t="str">
+      <c r="CG4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CH4" s="108" t="str">
+      <c r="CH4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CI4" s="108" t="str">
+      <c r="CI4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CJ4" s="108" t="str">
+      <c r="CJ4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CK4" s="108" t="str">
+      <c r="CK4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CL4" s="108" t="str">
+      <c r="CL4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CM4" s="108" t="str">
+      <c r="CM4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CN4" s="108" t="str">
+      <c r="CN4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CO4" s="108" t="str">
+      <c r="CO4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CP4" s="108" t="str">
+      <c r="CP4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CQ4" s="108" t="str">
+      <c r="CQ4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CR4" s="108" t="str">
+      <c r="CR4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="CS4" s="108" t="str">
+      <c r="CS4" s="116" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
@@ -5583,467 +5582,467 @@
     </row>
     <row r="5" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="122"/>
-      <c r="C5" s="122"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="113"/>
       <c r="D5" s="14"/>
       <c r="E5" s="15"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="108"/>
-      <c r="L5" s="108"/>
-      <c r="M5" s="110"/>
-      <c r="N5" s="110"/>
-      <c r="O5" s="108"/>
-      <c r="P5" s="108"/>
-      <c r="Q5" s="108"/>
-      <c r="R5" s="108"/>
-      <c r="S5" s="108"/>
-      <c r="T5" s="108"/>
-      <c r="U5" s="108"/>
-      <c r="V5" s="108"/>
-      <c r="W5" s="108"/>
-      <c r="X5" s="108"/>
-      <c r="Y5" s="108"/>
-      <c r="Z5" s="108"/>
-      <c r="AA5" s="108"/>
-      <c r="AB5" s="108"/>
-      <c r="AC5" s="108"/>
-      <c r="AD5" s="108"/>
-      <c r="AE5" s="108"/>
-      <c r="AF5" s="108"/>
-      <c r="AG5" s="108"/>
-      <c r="AH5" s="108"/>
-      <c r="AI5" s="108"/>
-      <c r="AJ5" s="108"/>
-      <c r="AK5" s="108"/>
-      <c r="AL5" s="108"/>
-      <c r="AM5" s="108"/>
-      <c r="AN5" s="108"/>
-      <c r="AO5" s="108"/>
-      <c r="AP5" s="108"/>
-      <c r="AQ5" s="108"/>
-      <c r="AR5" s="108"/>
-      <c r="AS5" s="108"/>
-      <c r="AT5" s="108"/>
-      <c r="AU5" s="108"/>
-      <c r="AV5" s="108"/>
-      <c r="AW5" s="108"/>
-      <c r="AX5" s="108"/>
-      <c r="AY5" s="108"/>
-      <c r="AZ5" s="108"/>
-      <c r="BA5" s="108"/>
-      <c r="BB5" s="108"/>
-      <c r="BC5" s="108"/>
-      <c r="BD5" s="108"/>
-      <c r="BE5" s="108"/>
-      <c r="BF5" s="108"/>
-      <c r="BG5" s="108"/>
-      <c r="BH5" s="108"/>
-      <c r="BI5" s="108"/>
-      <c r="BJ5" s="108"/>
-      <c r="BK5" s="108"/>
-      <c r="BL5" s="108"/>
-      <c r="BM5" s="108"/>
-      <c r="BN5" s="108"/>
-      <c r="BO5" s="108"/>
-      <c r="BP5" s="108"/>
-      <c r="BQ5" s="108"/>
-      <c r="BR5" s="108"/>
-      <c r="BS5" s="108"/>
-      <c r="BT5" s="108"/>
-      <c r="BU5" s="108"/>
-      <c r="BV5" s="108"/>
-      <c r="BW5" s="108"/>
-      <c r="BX5" s="108"/>
-      <c r="BY5" s="108"/>
-      <c r="BZ5" s="108"/>
-      <c r="CA5" s="108"/>
-      <c r="CB5" s="108"/>
-      <c r="CC5" s="108"/>
-      <c r="CD5" s="108"/>
-      <c r="CE5" s="108"/>
-      <c r="CF5" s="108"/>
-      <c r="CG5" s="108"/>
-      <c r="CH5" s="108"/>
-      <c r="CI5" s="108"/>
-      <c r="CJ5" s="108"/>
-      <c r="CK5" s="108"/>
-      <c r="CL5" s="108"/>
-      <c r="CM5" s="108"/>
-      <c r="CN5" s="108"/>
-      <c r="CO5" s="108"/>
-      <c r="CP5" s="108"/>
-      <c r="CQ5" s="108"/>
-      <c r="CR5" s="108"/>
-      <c r="CS5" s="108"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
+      <c r="M5" s="122"/>
+      <c r="N5" s="122"/>
+      <c r="O5" s="116"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="116"/>
+      <c r="R5" s="116"/>
+      <c r="S5" s="116"/>
+      <c r="T5" s="116"/>
+      <c r="U5" s="116"/>
+      <c r="V5" s="116"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="116"/>
+      <c r="Y5" s="116"/>
+      <c r="Z5" s="116"/>
+      <c r="AA5" s="116"/>
+      <c r="AB5" s="116"/>
+      <c r="AC5" s="116"/>
+      <c r="AD5" s="116"/>
+      <c r="AE5" s="116"/>
+      <c r="AF5" s="116"/>
+      <c r="AG5" s="116"/>
+      <c r="AH5" s="116"/>
+      <c r="AI5" s="116"/>
+      <c r="AJ5" s="116"/>
+      <c r="AK5" s="116"/>
+      <c r="AL5" s="116"/>
+      <c r="AM5" s="116"/>
+      <c r="AN5" s="116"/>
+      <c r="AO5" s="116"/>
+      <c r="AP5" s="116"/>
+      <c r="AQ5" s="116"/>
+      <c r="AR5" s="116"/>
+      <c r="AS5" s="116"/>
+      <c r="AT5" s="116"/>
+      <c r="AU5" s="116"/>
+      <c r="AV5" s="116"/>
+      <c r="AW5" s="116"/>
+      <c r="AX5" s="116"/>
+      <c r="AY5" s="116"/>
+      <c r="AZ5" s="116"/>
+      <c r="BA5" s="116"/>
+      <c r="BB5" s="116"/>
+      <c r="BC5" s="116"/>
+      <c r="BD5" s="116"/>
+      <c r="BE5" s="116"/>
+      <c r="BF5" s="116"/>
+      <c r="BG5" s="116"/>
+      <c r="BH5" s="116"/>
+      <c r="BI5" s="116"/>
+      <c r="BJ5" s="116"/>
+      <c r="BK5" s="116"/>
+      <c r="BL5" s="116"/>
+      <c r="BM5" s="116"/>
+      <c r="BN5" s="116"/>
+      <c r="BO5" s="116"/>
+      <c r="BP5" s="116"/>
+      <c r="BQ5" s="116"/>
+      <c r="BR5" s="116"/>
+      <c r="BS5" s="116"/>
+      <c r="BT5" s="116"/>
+      <c r="BU5" s="116"/>
+      <c r="BV5" s="116"/>
+      <c r="BW5" s="116"/>
+      <c r="BX5" s="116"/>
+      <c r="BY5" s="116"/>
+      <c r="BZ5" s="116"/>
+      <c r="CA5" s="116"/>
+      <c r="CB5" s="116"/>
+      <c r="CC5" s="116"/>
+      <c r="CD5" s="116"/>
+      <c r="CE5" s="116"/>
+      <c r="CF5" s="116"/>
+      <c r="CG5" s="116"/>
+      <c r="CH5" s="116"/>
+      <c r="CI5" s="116"/>
+      <c r="CJ5" s="116"/>
+      <c r="CK5" s="116"/>
+      <c r="CL5" s="116"/>
+      <c r="CM5" s="116"/>
+      <c r="CN5" s="116"/>
+      <c r="CO5" s="116"/>
+      <c r="CP5" s="116"/>
+      <c r="CQ5" s="116"/>
+      <c r="CR5" s="116"/>
+      <c r="CS5" s="116"/>
       <c r="CT5" s="12"/>
     </row>
     <row r="6" spans="1:98" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="122"/>
-      <c r="C6" s="122"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="113"/>
       <c r="D6" s="14"/>
       <c r="E6" s="15"/>
       <c r="F6" s="29"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="115">
+      <c r="H6" s="114">
         <v>41057</v>
       </c>
-      <c r="I6" s="115">
+      <c r="I6" s="114">
         <f>H6+IF(WEEKDAY(H6)=6,3,1)</f>
         <v>41058</v>
       </c>
-      <c r="J6" s="115">
+      <c r="J6" s="114">
         <f t="shared" ref="J6:AS6" si="2">I6+IF(WEEKDAY(I6)=6,3,1)</f>
         <v>41059</v>
       </c>
-      <c r="K6" s="115">
+      <c r="K6" s="114">
         <f t="shared" si="2"/>
         <v>41060</v>
       </c>
-      <c r="L6" s="115">
+      <c r="L6" s="114">
         <f t="shared" si="2"/>
         <v>41061</v>
       </c>
-      <c r="M6" s="115">
+      <c r="M6" s="114">
         <f t="shared" si="2"/>
         <v>41064</v>
       </c>
-      <c r="N6" s="115">
+      <c r="N6" s="114">
         <f t="shared" si="2"/>
         <v>41065</v>
       </c>
-      <c r="O6" s="115">
+      <c r="O6" s="114">
         <f t="shared" si="2"/>
         <v>41066</v>
       </c>
-      <c r="P6" s="115">
+      <c r="P6" s="114">
         <f t="shared" si="2"/>
         <v>41067</v>
       </c>
-      <c r="Q6" s="115">
+      <c r="Q6" s="114">
         <f t="shared" si="2"/>
         <v>41068</v>
       </c>
-      <c r="R6" s="115">
+      <c r="R6" s="114">
         <f t="shared" si="2"/>
         <v>41071</v>
       </c>
-      <c r="S6" s="115">
+      <c r="S6" s="114">
         <f t="shared" si="2"/>
         <v>41072</v>
       </c>
-      <c r="T6" s="115">
+      <c r="T6" s="114">
         <f t="shared" si="2"/>
         <v>41073</v>
       </c>
-      <c r="U6" s="115">
+      <c r="U6" s="114">
         <f t="shared" si="2"/>
         <v>41074</v>
       </c>
-      <c r="V6" s="115">
+      <c r="V6" s="114">
         <f t="shared" si="2"/>
         <v>41075</v>
       </c>
-      <c r="W6" s="115">
+      <c r="W6" s="114">
         <f t="shared" si="2"/>
         <v>41078</v>
       </c>
-      <c r="X6" s="115">
+      <c r="X6" s="114">
         <f t="shared" si="2"/>
         <v>41079</v>
       </c>
-      <c r="Y6" s="115">
+      <c r="Y6" s="114">
         <f t="shared" si="2"/>
         <v>41080</v>
       </c>
-      <c r="Z6" s="115">
+      <c r="Z6" s="114">
         <f t="shared" si="2"/>
         <v>41081</v>
       </c>
-      <c r="AA6" s="115">
+      <c r="AA6" s="114">
         <f t="shared" si="2"/>
         <v>41082</v>
       </c>
-      <c r="AB6" s="115">
+      <c r="AB6" s="114">
         <f t="shared" si="2"/>
         <v>41085</v>
       </c>
-      <c r="AC6" s="115">
+      <c r="AC6" s="114">
         <f t="shared" si="2"/>
         <v>41086</v>
       </c>
-      <c r="AD6" s="115">
+      <c r="AD6" s="114">
         <f t="shared" si="2"/>
         <v>41087</v>
       </c>
-      <c r="AE6" s="115">
+      <c r="AE6" s="114">
         <f t="shared" si="2"/>
         <v>41088</v>
       </c>
-      <c r="AF6" s="115">
+      <c r="AF6" s="114">
         <f t="shared" si="2"/>
         <v>41089</v>
       </c>
-      <c r="AG6" s="115">
+      <c r="AG6" s="114">
         <f t="shared" si="2"/>
         <v>41092</v>
       </c>
-      <c r="AH6" s="115">
+      <c r="AH6" s="114">
         <f t="shared" si="2"/>
         <v>41093</v>
       </c>
-      <c r="AI6" s="115">
+      <c r="AI6" s="114">
         <f t="shared" si="2"/>
         <v>41094</v>
       </c>
-      <c r="AJ6" s="115">
+      <c r="AJ6" s="114">
         <f t="shared" si="2"/>
         <v>41095</v>
       </c>
-      <c r="AK6" s="115">
+      <c r="AK6" s="114">
         <f t="shared" si="2"/>
         <v>41096</v>
       </c>
-      <c r="AL6" s="115">
+      <c r="AL6" s="114">
         <f t="shared" si="2"/>
         <v>41099</v>
       </c>
-      <c r="AM6" s="115">
+      <c r="AM6" s="114">
         <f t="shared" si="2"/>
         <v>41100</v>
       </c>
-      <c r="AN6" s="115">
+      <c r="AN6" s="114">
         <f t="shared" si="2"/>
         <v>41101</v>
       </c>
-      <c r="AO6" s="115">
+      <c r="AO6" s="114">
         <f t="shared" si="2"/>
         <v>41102</v>
       </c>
-      <c r="AP6" s="115">
+      <c r="AP6" s="114">
         <f t="shared" si="2"/>
         <v>41103</v>
       </c>
-      <c r="AQ6" s="115">
+      <c r="AQ6" s="114">
         <f t="shared" si="2"/>
         <v>41106</v>
       </c>
-      <c r="AR6" s="115">
+      <c r="AR6" s="114">
         <f t="shared" si="2"/>
         <v>41107</v>
       </c>
-      <c r="AS6" s="115">
+      <c r="AS6" s="114">
         <f t="shared" si="2"/>
         <v>41108</v>
       </c>
-      <c r="AT6" s="115">
+      <c r="AT6" s="114">
         <f t="shared" ref="AT6:CS6" si="3">AS6+IF(WEEKDAY(AS6)=6,3,1)</f>
         <v>41109</v>
       </c>
-      <c r="AU6" s="115">
+      <c r="AU6" s="114">
         <f t="shared" si="3"/>
         <v>41110</v>
       </c>
-      <c r="AV6" s="115">
+      <c r="AV6" s="114">
         <f t="shared" si="3"/>
         <v>41113</v>
       </c>
-      <c r="AW6" s="115">
+      <c r="AW6" s="114">
         <f t="shared" si="3"/>
         <v>41114</v>
       </c>
-      <c r="AX6" s="115">
+      <c r="AX6" s="114">
         <f t="shared" si="3"/>
         <v>41115</v>
       </c>
-      <c r="AY6" s="115">
+      <c r="AY6" s="114">
         <f t="shared" si="3"/>
         <v>41116</v>
       </c>
-      <c r="AZ6" s="115">
+      <c r="AZ6" s="114">
         <f t="shared" si="3"/>
         <v>41117</v>
       </c>
-      <c r="BA6" s="115">
+      <c r="BA6" s="114">
         <f t="shared" si="3"/>
         <v>41120</v>
       </c>
-      <c r="BB6" s="115">
+      <c r="BB6" s="114">
         <f t="shared" si="3"/>
         <v>41121</v>
       </c>
-      <c r="BC6" s="115">
+      <c r="BC6" s="114">
         <f t="shared" si="3"/>
         <v>41122</v>
       </c>
-      <c r="BD6" s="115">
+      <c r="BD6" s="114">
         <f t="shared" si="3"/>
         <v>41123</v>
       </c>
-      <c r="BE6" s="115">
+      <c r="BE6" s="114">
         <f t="shared" si="3"/>
         <v>41124</v>
       </c>
-      <c r="BF6" s="115">
+      <c r="BF6" s="114">
         <f t="shared" si="3"/>
         <v>41127</v>
       </c>
-      <c r="BG6" s="115">
+      <c r="BG6" s="114">
         <f t="shared" si="3"/>
         <v>41128</v>
       </c>
-      <c r="BH6" s="115">
+      <c r="BH6" s="114">
         <f t="shared" si="3"/>
         <v>41129</v>
       </c>
-      <c r="BI6" s="115">
+      <c r="BI6" s="114">
         <f t="shared" si="3"/>
         <v>41130</v>
       </c>
-      <c r="BJ6" s="115">
+      <c r="BJ6" s="114">
         <f t="shared" si="3"/>
         <v>41131</v>
       </c>
-      <c r="BK6" s="115">
+      <c r="BK6" s="114">
         <f t="shared" si="3"/>
         <v>41134</v>
       </c>
-      <c r="BL6" s="115">
+      <c r="BL6" s="114">
         <f t="shared" si="3"/>
         <v>41135</v>
       </c>
-      <c r="BM6" s="115">
+      <c r="BM6" s="114">
         <f t="shared" si="3"/>
         <v>41136</v>
       </c>
-      <c r="BN6" s="115">
+      <c r="BN6" s="114">
         <f t="shared" si="3"/>
         <v>41137</v>
       </c>
-      <c r="BO6" s="115">
+      <c r="BO6" s="114">
         <f t="shared" si="3"/>
         <v>41138</v>
       </c>
-      <c r="BP6" s="115">
+      <c r="BP6" s="114">
         <f t="shared" si="3"/>
         <v>41141</v>
       </c>
-      <c r="BQ6" s="115">
+      <c r="BQ6" s="114">
         <f t="shared" si="3"/>
         <v>41142</v>
       </c>
-      <c r="BR6" s="115">
+      <c r="BR6" s="114">
         <f t="shared" si="3"/>
         <v>41143</v>
       </c>
-      <c r="BS6" s="115">
+      <c r="BS6" s="114">
         <f t="shared" si="3"/>
         <v>41144</v>
       </c>
-      <c r="BT6" s="115">
+      <c r="BT6" s="114">
         <f t="shared" si="3"/>
         <v>41145</v>
       </c>
-      <c r="BU6" s="115">
+      <c r="BU6" s="114">
         <f t="shared" si="3"/>
         <v>41148</v>
       </c>
-      <c r="BV6" s="115">
+      <c r="BV6" s="114">
         <f t="shared" si="3"/>
         <v>41149</v>
       </c>
-      <c r="BW6" s="115">
+      <c r="BW6" s="114">
         <f t="shared" si="3"/>
         <v>41150</v>
       </c>
-      <c r="BX6" s="115">
+      <c r="BX6" s="114">
         <f t="shared" si="3"/>
         <v>41151</v>
       </c>
-      <c r="BY6" s="115">
+      <c r="BY6" s="114">
         <f t="shared" si="3"/>
         <v>41152</v>
       </c>
-      <c r="BZ6" s="115">
+      <c r="BZ6" s="114">
         <f t="shared" si="3"/>
         <v>41155</v>
       </c>
-      <c r="CA6" s="115">
+      <c r="CA6" s="114">
         <f t="shared" si="3"/>
         <v>41156</v>
       </c>
-      <c r="CB6" s="115">
+      <c r="CB6" s="114">
         <f t="shared" si="3"/>
         <v>41157</v>
       </c>
-      <c r="CC6" s="115">
+      <c r="CC6" s="114">
         <f t="shared" si="3"/>
         <v>41158</v>
       </c>
-      <c r="CD6" s="115">
+      <c r="CD6" s="114">
         <f t="shared" si="3"/>
         <v>41159</v>
       </c>
-      <c r="CE6" s="115">
+      <c r="CE6" s="114">
         <f t="shared" si="3"/>
         <v>41162</v>
       </c>
-      <c r="CF6" s="115">
+      <c r="CF6" s="114">
         <f t="shared" si="3"/>
         <v>41163</v>
       </c>
-      <c r="CG6" s="115">
+      <c r="CG6" s="114">
         <f t="shared" si="3"/>
         <v>41164</v>
       </c>
-      <c r="CH6" s="115">
+      <c r="CH6" s="114">
         <f t="shared" si="3"/>
         <v>41165</v>
       </c>
-      <c r="CI6" s="115">
+      <c r="CI6" s="114">
         <f t="shared" si="3"/>
         <v>41166</v>
       </c>
-      <c r="CJ6" s="115">
+      <c r="CJ6" s="114">
         <f t="shared" si="3"/>
         <v>41169</v>
       </c>
-      <c r="CK6" s="115">
+      <c r="CK6" s="114">
         <f t="shared" si="3"/>
         <v>41170</v>
       </c>
-      <c r="CL6" s="115">
+      <c r="CL6" s="114">
         <f t="shared" si="3"/>
         <v>41171</v>
       </c>
-      <c r="CM6" s="115">
+      <c r="CM6" s="114">
         <f t="shared" si="3"/>
         <v>41172</v>
       </c>
-      <c r="CN6" s="115">
+      <c r="CN6" s="114">
         <f t="shared" si="3"/>
         <v>41173</v>
       </c>
-      <c r="CO6" s="115">
+      <c r="CO6" s="114">
         <f t="shared" si="3"/>
         <v>41176</v>
       </c>
-      <c r="CP6" s="115">
+      <c r="CP6" s="114">
         <f t="shared" si="3"/>
         <v>41177</v>
       </c>
-      <c r="CQ6" s="115">
+      <c r="CQ6" s="114">
         <f t="shared" si="3"/>
         <v>41178</v>
       </c>
-      <c r="CR6" s="115">
+      <c r="CR6" s="114">
         <f t="shared" si="3"/>
         <v>41179</v>
       </c>
-      <c r="CS6" s="115">
+      <c r="CS6" s="114">
         <f t="shared" si="3"/>
         <v>41180</v>
       </c>
@@ -6051,100 +6050,100 @@
     </row>
     <row r="7" spans="1:98" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
-      <c r="B7" s="122"/>
-      <c r="C7" s="122"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="113"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
-      <c r="H7" s="116"/>
-      <c r="I7" s="116"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="116"/>
-      <c r="M7" s="116"/>
-      <c r="N7" s="116"/>
-      <c r="O7" s="116"/>
-      <c r="P7" s="116"/>
-      <c r="Q7" s="116"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="116"/>
-      <c r="T7" s="116"/>
-      <c r="U7" s="116"/>
-      <c r="V7" s="116"/>
-      <c r="W7" s="116"/>
-      <c r="X7" s="116"/>
-      <c r="Y7" s="116"/>
-      <c r="Z7" s="116"/>
-      <c r="AA7" s="116"/>
-      <c r="AB7" s="116"/>
-      <c r="AC7" s="116"/>
-      <c r="AD7" s="116"/>
-      <c r="AE7" s="116"/>
-      <c r="AF7" s="116"/>
-      <c r="AG7" s="116"/>
-      <c r="AH7" s="116"/>
-      <c r="AI7" s="116"/>
-      <c r="AJ7" s="116"/>
-      <c r="AK7" s="116"/>
-      <c r="AL7" s="116"/>
-      <c r="AM7" s="116"/>
-      <c r="AN7" s="116"/>
-      <c r="AO7" s="116"/>
-      <c r="AP7" s="116"/>
-      <c r="AQ7" s="116"/>
-      <c r="AR7" s="116"/>
-      <c r="AS7" s="116"/>
-      <c r="AT7" s="116"/>
-      <c r="AU7" s="116"/>
-      <c r="AV7" s="116"/>
-      <c r="AW7" s="116"/>
-      <c r="AX7" s="116"/>
-      <c r="AY7" s="116"/>
-      <c r="AZ7" s="116"/>
-      <c r="BA7" s="116"/>
-      <c r="BB7" s="116"/>
-      <c r="BC7" s="116"/>
-      <c r="BD7" s="116"/>
-      <c r="BE7" s="116"/>
-      <c r="BF7" s="116"/>
-      <c r="BG7" s="116"/>
-      <c r="BH7" s="116"/>
-      <c r="BI7" s="116"/>
-      <c r="BJ7" s="116"/>
-      <c r="BK7" s="116"/>
-      <c r="BL7" s="116"/>
-      <c r="BM7" s="116"/>
-      <c r="BN7" s="116"/>
-      <c r="BO7" s="116"/>
-      <c r="BP7" s="116"/>
-      <c r="BQ7" s="116"/>
-      <c r="BR7" s="116"/>
-      <c r="BS7" s="116"/>
-      <c r="BT7" s="116"/>
-      <c r="BU7" s="116"/>
-      <c r="BV7" s="116"/>
-      <c r="BW7" s="116"/>
-      <c r="BX7" s="116"/>
-      <c r="BY7" s="116"/>
-      <c r="BZ7" s="116"/>
-      <c r="CA7" s="116"/>
-      <c r="CB7" s="116"/>
-      <c r="CC7" s="116"/>
-      <c r="CD7" s="116"/>
-      <c r="CE7" s="116"/>
-      <c r="CF7" s="116"/>
-      <c r="CG7" s="116"/>
-      <c r="CH7" s="116"/>
-      <c r="CI7" s="116"/>
-      <c r="CJ7" s="116"/>
-      <c r="CK7" s="116"/>
-      <c r="CL7" s="116"/>
-      <c r="CM7" s="116"/>
-      <c r="CN7" s="116"/>
-      <c r="CO7" s="116"/>
-      <c r="CP7" s="116"/>
-      <c r="CQ7" s="116"/>
-      <c r="CR7" s="116"/>
-      <c r="CS7" s="116"/>
+      <c r="H7" s="115"/>
+      <c r="I7" s="115"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="115"/>
+      <c r="L7" s="115"/>
+      <c r="M7" s="115"/>
+      <c r="N7" s="115"/>
+      <c r="O7" s="115"/>
+      <c r="P7" s="115"/>
+      <c r="Q7" s="115"/>
+      <c r="R7" s="115"/>
+      <c r="S7" s="115"/>
+      <c r="T7" s="115"/>
+      <c r="U7" s="115"/>
+      <c r="V7" s="115"/>
+      <c r="W7" s="115"/>
+      <c r="X7" s="115"/>
+      <c r="Y7" s="115"/>
+      <c r="Z7" s="115"/>
+      <c r="AA7" s="115"/>
+      <c r="AB7" s="115"/>
+      <c r="AC7" s="115"/>
+      <c r="AD7" s="115"/>
+      <c r="AE7" s="115"/>
+      <c r="AF7" s="115"/>
+      <c r="AG7" s="115"/>
+      <c r="AH7" s="115"/>
+      <c r="AI7" s="115"/>
+      <c r="AJ7" s="115"/>
+      <c r="AK7" s="115"/>
+      <c r="AL7" s="115"/>
+      <c r="AM7" s="115"/>
+      <c r="AN7" s="115"/>
+      <c r="AO7" s="115"/>
+      <c r="AP7" s="115"/>
+      <c r="AQ7" s="115"/>
+      <c r="AR7" s="115"/>
+      <c r="AS7" s="115"/>
+      <c r="AT7" s="115"/>
+      <c r="AU7" s="115"/>
+      <c r="AV7" s="115"/>
+      <c r="AW7" s="115"/>
+      <c r="AX7" s="115"/>
+      <c r="AY7" s="115"/>
+      <c r="AZ7" s="115"/>
+      <c r="BA7" s="115"/>
+      <c r="BB7" s="115"/>
+      <c r="BC7" s="115"/>
+      <c r="BD7" s="115"/>
+      <c r="BE7" s="115"/>
+      <c r="BF7" s="115"/>
+      <c r="BG7" s="115"/>
+      <c r="BH7" s="115"/>
+      <c r="BI7" s="115"/>
+      <c r="BJ7" s="115"/>
+      <c r="BK7" s="115"/>
+      <c r="BL7" s="115"/>
+      <c r="BM7" s="115"/>
+      <c r="BN7" s="115"/>
+      <c r="BO7" s="115"/>
+      <c r="BP7" s="115"/>
+      <c r="BQ7" s="115"/>
+      <c r="BR7" s="115"/>
+      <c r="BS7" s="115"/>
+      <c r="BT7" s="115"/>
+      <c r="BU7" s="115"/>
+      <c r="BV7" s="115"/>
+      <c r="BW7" s="115"/>
+      <c r="BX7" s="115"/>
+      <c r="BY7" s="115"/>
+      <c r="BZ7" s="115"/>
+      <c r="CA7" s="115"/>
+      <c r="CB7" s="115"/>
+      <c r="CC7" s="115"/>
+      <c r="CD7" s="115"/>
+      <c r="CE7" s="115"/>
+      <c r="CF7" s="115"/>
+      <c r="CG7" s="115"/>
+      <c r="CH7" s="115"/>
+      <c r="CI7" s="115"/>
+      <c r="CJ7" s="115"/>
+      <c r="CK7" s="115"/>
+      <c r="CL7" s="115"/>
+      <c r="CM7" s="115"/>
+      <c r="CN7" s="115"/>
+      <c r="CO7" s="115"/>
+      <c r="CP7" s="115"/>
+      <c r="CQ7" s="115"/>
+      <c r="CR7" s="115"/>
+      <c r="CS7" s="115"/>
       <c r="CT7" s="13"/>
     </row>
     <row r="8" spans="1:98" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6160,18 +6159,18 @@
       </c>
     </row>
     <row r="10" spans="1:98" x14ac:dyDescent="0.25">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="118"/>
-      <c r="C10" s="118"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="109"/>
       <c r="D10" s="35">
         <f ca="1">MIN(D11:D18)</f>
         <v>41078</v>
       </c>
       <c r="E10" s="35">
         <f ca="1">MAX(E11:E18)</f>
-        <v>41097</v>
+        <v>41103</v>
       </c>
       <c r="F10" s="36"/>
       <c r="H10" s="4"/>
@@ -6375,11 +6374,11 @@
       <c r="C12" s="2"/>
       <c r="D12" s="14">
         <f ca="1">TODAY()</f>
-        <v>41082</v>
+        <v>41087</v>
       </c>
       <c r="E12" s="21">
         <f ca="1">D12+5+CHOOSE(WEEKDAY(D12+5,2),0,0,0,0,0,2,1)</f>
-        <v>41087</v>
+        <v>41092</v>
       </c>
       <c r="F12" s="37">
         <v>0.6</v>
@@ -6483,11 +6482,11 @@
       <c r="C13" s="2"/>
       <c r="D13" s="14">
         <f ca="1">E12+1</f>
-        <v>41088</v>
+        <v>41093</v>
       </c>
       <c r="E13" s="21">
         <f ca="1">D13+6+CHOOSE(WEEKDAY(D13+5,2),0,0,0,0,0,2,1)</f>
-        <v>41094</v>
+        <v>41100</v>
       </c>
       <c r="F13" s="37"/>
       <c r="H13" s="10"/>
@@ -6589,11 +6588,11 @@
       <c r="C14" s="2"/>
       <c r="D14" s="14">
         <f ca="1">E13</f>
-        <v>41094</v>
+        <v>41100</v>
       </c>
       <c r="E14" s="21">
         <f ca="1">D14+3</f>
-        <v>41097</v>
+        <v>41103</v>
       </c>
       <c r="F14" s="37"/>
       <c r="H14" s="10"/>
@@ -7188,11 +7187,11 @@
       <c r="CS19" s="3"/>
     </row>
     <row r="20" spans="1:97" x14ac:dyDescent="0.25">
-      <c r="A20" s="117" t="s">
+      <c r="A20" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="118"/>
-      <c r="C20" s="118"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="109"/>
       <c r="D20" s="35" t="e">
         <f>MIN(D21:D28)</f>
         <v>#REF!</v>
@@ -7505,7 +7504,7 @@
       </c>
       <c r="E23" s="24">
         <f>D23+Versioning!E3-1</f>
-        <v>41109</v>
+        <v>41115</v>
       </c>
       <c r="F23" s="30">
         <v>0.4</v>
@@ -8213,11 +8212,11 @@
       <c r="CS29" s="2"/>
     </row>
     <row r="30" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="117" t="s">
+      <c r="A30" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="118"/>
-      <c r="C30" s="118"/>
+      <c r="B30" s="109"/>
+      <c r="C30" s="109"/>
       <c r="D30" s="35" t="e">
         <f>MIN(D31:D34)</f>
         <v>#REF!</v>
@@ -8751,11 +8750,11 @@
       <c r="BC35" s="79"/>
     </row>
     <row r="36" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="117" t="s">
+      <c r="A36" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="118"/>
-      <c r="C36" s="118"/>
+      <c r="B36" s="109"/>
+      <c r="C36" s="109"/>
       <c r="D36" s="35" t="e">
         <f>MIN(D37:D42)</f>
         <v>#REF!</v>
@@ -9591,11 +9590,11 @@
       <c r="CS43" s="2"/>
     </row>
     <row r="44" spans="1:97" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="117" t="s">
+      <c r="A44" s="108" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="118"/>
-      <c r="C44" s="118"/>
+      <c r="B44" s="109"/>
+      <c r="C44" s="109"/>
       <c r="D44" s="35">
         <f>MIN(D45:D49)</f>
         <v>40364</v>
@@ -10238,151 +10237,29 @@
     </row>
   </sheetData>
   <mergeCells count="192">
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="CR6:CR7"/>
-    <mergeCell ref="CS6:CS7"/>
-    <mergeCell ref="CM6:CM7"/>
-    <mergeCell ref="CN6:CN7"/>
-    <mergeCell ref="CO6:CO7"/>
-    <mergeCell ref="CP6:CP7"/>
-    <mergeCell ref="CQ6:CQ7"/>
-    <mergeCell ref="CH6:CH7"/>
-    <mergeCell ref="CI6:CI7"/>
-    <mergeCell ref="CJ6:CJ7"/>
-    <mergeCell ref="CK6:CK7"/>
-    <mergeCell ref="CL6:CL7"/>
-    <mergeCell ref="CC6:CC7"/>
-    <mergeCell ref="CD6:CD7"/>
-    <mergeCell ref="CE6:CE7"/>
-    <mergeCell ref="CF6:CF7"/>
-    <mergeCell ref="CG6:CG7"/>
-    <mergeCell ref="BX6:BX7"/>
-    <mergeCell ref="BY6:BY7"/>
-    <mergeCell ref="BZ6:BZ7"/>
-    <mergeCell ref="CA6:CA7"/>
-    <mergeCell ref="CB6:CB7"/>
-    <mergeCell ref="BS6:BS7"/>
-    <mergeCell ref="BT6:BT7"/>
-    <mergeCell ref="BU6:BU7"/>
-    <mergeCell ref="BV6:BV7"/>
-    <mergeCell ref="BW6:BW7"/>
-    <mergeCell ref="BN6:BN7"/>
-    <mergeCell ref="BO6:BO7"/>
-    <mergeCell ref="BP6:BP7"/>
-    <mergeCell ref="BQ6:BQ7"/>
-    <mergeCell ref="BR6:BR7"/>
-    <mergeCell ref="BI6:BI7"/>
-    <mergeCell ref="BJ6:BJ7"/>
-    <mergeCell ref="BK6:BK7"/>
-    <mergeCell ref="BL6:BL7"/>
-    <mergeCell ref="BM6:BM7"/>
-    <mergeCell ref="BD6:BD7"/>
-    <mergeCell ref="BE6:BE7"/>
-    <mergeCell ref="BF6:BF7"/>
-    <mergeCell ref="BG6:BG7"/>
-    <mergeCell ref="BH6:BH7"/>
-    <mergeCell ref="AY6:AY7"/>
-    <mergeCell ref="AZ6:AZ7"/>
-    <mergeCell ref="BA6:BA7"/>
-    <mergeCell ref="BB6:BB7"/>
-    <mergeCell ref="BC6:BC7"/>
-    <mergeCell ref="AT6:AT7"/>
-    <mergeCell ref="AU6:AU7"/>
-    <mergeCell ref="AV6:AV7"/>
-    <mergeCell ref="AW6:AW7"/>
-    <mergeCell ref="AX6:AX7"/>
-    <mergeCell ref="AO6:AO7"/>
-    <mergeCell ref="AP6:AP7"/>
-    <mergeCell ref="AQ6:AQ7"/>
-    <mergeCell ref="AR6:AR7"/>
-    <mergeCell ref="AS6:AS7"/>
-    <mergeCell ref="AJ6:AJ7"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AL6:AL7"/>
-    <mergeCell ref="AM6:AM7"/>
-    <mergeCell ref="AN6:AN7"/>
-    <mergeCell ref="AE6:AE7"/>
-    <mergeCell ref="AF6:AF7"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="AH6:AH7"/>
-    <mergeCell ref="AI6:AI7"/>
-    <mergeCell ref="Z6:Z7"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AB6:AB7"/>
-    <mergeCell ref="AC6:AC7"/>
-    <mergeCell ref="AD6:AD7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="Y6:Y7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="CR4:CR5"/>
-    <mergeCell ref="CS4:CS5"/>
-    <mergeCell ref="CM4:CM5"/>
-    <mergeCell ref="CN4:CN5"/>
-    <mergeCell ref="CO4:CO5"/>
-    <mergeCell ref="CP4:CP5"/>
-    <mergeCell ref="CQ4:CQ5"/>
-    <mergeCell ref="CH4:CH5"/>
-    <mergeCell ref="CI4:CI5"/>
-    <mergeCell ref="CJ4:CJ5"/>
-    <mergeCell ref="CK4:CK5"/>
-    <mergeCell ref="CL4:CL5"/>
-    <mergeCell ref="CC4:CC5"/>
-    <mergeCell ref="CD4:CD5"/>
-    <mergeCell ref="CE4:CE5"/>
-    <mergeCell ref="CF4:CF5"/>
-    <mergeCell ref="CG4:CG5"/>
-    <mergeCell ref="BX4:BX5"/>
-    <mergeCell ref="BY4:BY5"/>
-    <mergeCell ref="BZ4:BZ5"/>
-    <mergeCell ref="CA4:CA5"/>
-    <mergeCell ref="CB4:CB5"/>
-    <mergeCell ref="BS4:BS5"/>
-    <mergeCell ref="BT4:BT5"/>
-    <mergeCell ref="BU4:BU5"/>
-    <mergeCell ref="BV4:BV5"/>
-    <mergeCell ref="BW4:BW5"/>
-    <mergeCell ref="BN4:BN5"/>
-    <mergeCell ref="BO4:BO5"/>
-    <mergeCell ref="BP4:BP5"/>
-    <mergeCell ref="BQ4:BQ5"/>
-    <mergeCell ref="BR4:BR5"/>
-    <mergeCell ref="BI4:BI5"/>
-    <mergeCell ref="BJ4:BJ5"/>
-    <mergeCell ref="BK4:BK5"/>
-    <mergeCell ref="BL4:BL5"/>
-    <mergeCell ref="BB4:BB5"/>
-    <mergeCell ref="BC4:BC5"/>
-    <mergeCell ref="BM4:BM5"/>
-    <mergeCell ref="BD4:BD5"/>
-    <mergeCell ref="BE4:BE5"/>
-    <mergeCell ref="BF4:BF5"/>
-    <mergeCell ref="BG4:BG5"/>
-    <mergeCell ref="BH4:BH5"/>
+    <mergeCell ref="AS4:AS5"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AK4:AK5"/>
+    <mergeCell ref="AL4:AL5"/>
+    <mergeCell ref="AM4:AM5"/>
+    <mergeCell ref="AN4:AN5"/>
+    <mergeCell ref="AY4:AY5"/>
+    <mergeCell ref="AZ4:AZ5"/>
+    <mergeCell ref="BA4:BA5"/>
+    <mergeCell ref="AT4:AT5"/>
+    <mergeCell ref="AU4:AU5"/>
+    <mergeCell ref="AV4:AV5"/>
+    <mergeCell ref="AW4:AW5"/>
+    <mergeCell ref="AX4:AX5"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="T4:T5"/>
     <mergeCell ref="H2:CS3"/>
     <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
@@ -10407,29 +10284,151 @@
     <mergeCell ref="AP4:AP5"/>
     <mergeCell ref="AQ4:AQ5"/>
     <mergeCell ref="AR4:AR5"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="AS4:AS5"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AK4:AK5"/>
-    <mergeCell ref="AL4:AL5"/>
-    <mergeCell ref="AM4:AM5"/>
-    <mergeCell ref="AN4:AN5"/>
-    <mergeCell ref="AY4:AY5"/>
-    <mergeCell ref="AZ4:AZ5"/>
-    <mergeCell ref="BA4:BA5"/>
-    <mergeCell ref="AT4:AT5"/>
-    <mergeCell ref="AU4:AU5"/>
-    <mergeCell ref="AV4:AV5"/>
-    <mergeCell ref="AW4:AW5"/>
-    <mergeCell ref="AX4:AX5"/>
+    <mergeCell ref="BI4:BI5"/>
+    <mergeCell ref="BJ4:BJ5"/>
+    <mergeCell ref="BK4:BK5"/>
+    <mergeCell ref="BL4:BL5"/>
+    <mergeCell ref="BB4:BB5"/>
+    <mergeCell ref="BC4:BC5"/>
+    <mergeCell ref="BM4:BM5"/>
+    <mergeCell ref="BD4:BD5"/>
+    <mergeCell ref="BE4:BE5"/>
+    <mergeCell ref="BF4:BF5"/>
+    <mergeCell ref="BG4:BG5"/>
+    <mergeCell ref="BH4:BH5"/>
+    <mergeCell ref="BS4:BS5"/>
+    <mergeCell ref="BT4:BT5"/>
+    <mergeCell ref="BU4:BU5"/>
+    <mergeCell ref="BV4:BV5"/>
+    <mergeCell ref="BW4:BW5"/>
+    <mergeCell ref="BN4:BN5"/>
+    <mergeCell ref="BO4:BO5"/>
+    <mergeCell ref="BP4:BP5"/>
+    <mergeCell ref="BQ4:BQ5"/>
+    <mergeCell ref="BR4:BR5"/>
+    <mergeCell ref="CC4:CC5"/>
+    <mergeCell ref="CD4:CD5"/>
+    <mergeCell ref="CE4:CE5"/>
+    <mergeCell ref="CF4:CF5"/>
+    <mergeCell ref="CG4:CG5"/>
+    <mergeCell ref="BX4:BX5"/>
+    <mergeCell ref="BY4:BY5"/>
+    <mergeCell ref="BZ4:BZ5"/>
+    <mergeCell ref="CA4:CA5"/>
+    <mergeCell ref="CB4:CB5"/>
+    <mergeCell ref="CR4:CR5"/>
+    <mergeCell ref="CS4:CS5"/>
+    <mergeCell ref="CM4:CM5"/>
+    <mergeCell ref="CN4:CN5"/>
+    <mergeCell ref="CO4:CO5"/>
+    <mergeCell ref="CP4:CP5"/>
+    <mergeCell ref="CQ4:CQ5"/>
+    <mergeCell ref="CH4:CH5"/>
+    <mergeCell ref="CI4:CI5"/>
+    <mergeCell ref="CJ4:CJ5"/>
+    <mergeCell ref="CK4:CK5"/>
+    <mergeCell ref="CL4:CL5"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="Y6:Y7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="AE6:AE7"/>
+    <mergeCell ref="AF6:AF7"/>
+    <mergeCell ref="AG6:AG7"/>
+    <mergeCell ref="AH6:AH7"/>
+    <mergeCell ref="AI6:AI7"/>
+    <mergeCell ref="Z6:Z7"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AB6:AB7"/>
+    <mergeCell ref="AC6:AC7"/>
+    <mergeCell ref="AD6:AD7"/>
+    <mergeCell ref="AO6:AO7"/>
+    <mergeCell ref="AP6:AP7"/>
+    <mergeCell ref="AQ6:AQ7"/>
+    <mergeCell ref="AR6:AR7"/>
+    <mergeCell ref="AS6:AS7"/>
+    <mergeCell ref="AJ6:AJ7"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AL6:AL7"/>
+    <mergeCell ref="AM6:AM7"/>
+    <mergeCell ref="AN6:AN7"/>
+    <mergeCell ref="AY6:AY7"/>
+    <mergeCell ref="AZ6:AZ7"/>
+    <mergeCell ref="BA6:BA7"/>
+    <mergeCell ref="BB6:BB7"/>
+    <mergeCell ref="BC6:BC7"/>
+    <mergeCell ref="AT6:AT7"/>
+    <mergeCell ref="AU6:AU7"/>
+    <mergeCell ref="AV6:AV7"/>
+    <mergeCell ref="AW6:AW7"/>
+    <mergeCell ref="AX6:AX7"/>
+    <mergeCell ref="BI6:BI7"/>
+    <mergeCell ref="BJ6:BJ7"/>
+    <mergeCell ref="BK6:BK7"/>
+    <mergeCell ref="BL6:BL7"/>
+    <mergeCell ref="BM6:BM7"/>
+    <mergeCell ref="BD6:BD7"/>
+    <mergeCell ref="BE6:BE7"/>
+    <mergeCell ref="BF6:BF7"/>
+    <mergeCell ref="BG6:BG7"/>
+    <mergeCell ref="BH6:BH7"/>
+    <mergeCell ref="BS6:BS7"/>
+    <mergeCell ref="BT6:BT7"/>
+    <mergeCell ref="BU6:BU7"/>
+    <mergeCell ref="BV6:BV7"/>
+    <mergeCell ref="BW6:BW7"/>
+    <mergeCell ref="BN6:BN7"/>
+    <mergeCell ref="BO6:BO7"/>
+    <mergeCell ref="BP6:BP7"/>
+    <mergeCell ref="BQ6:BQ7"/>
+    <mergeCell ref="BR6:BR7"/>
+    <mergeCell ref="CC6:CC7"/>
+    <mergeCell ref="CD6:CD7"/>
+    <mergeCell ref="CE6:CE7"/>
+    <mergeCell ref="CF6:CF7"/>
+    <mergeCell ref="CG6:CG7"/>
+    <mergeCell ref="BX6:BX7"/>
+    <mergeCell ref="BY6:BY7"/>
+    <mergeCell ref="BZ6:BZ7"/>
+    <mergeCell ref="CA6:CA7"/>
+    <mergeCell ref="CB6:CB7"/>
+    <mergeCell ref="CR6:CR7"/>
+    <mergeCell ref="CS6:CS7"/>
+    <mergeCell ref="CM6:CM7"/>
+    <mergeCell ref="CN6:CN7"/>
+    <mergeCell ref="CO6:CO7"/>
+    <mergeCell ref="CP6:CP7"/>
+    <mergeCell ref="CQ6:CQ7"/>
+    <mergeCell ref="CH6:CH7"/>
+    <mergeCell ref="CI6:CI7"/>
+    <mergeCell ref="CJ6:CJ7"/>
+    <mergeCell ref="CK6:CK7"/>
+    <mergeCell ref="CL6:CL7"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <conditionalFormatting sqref="H15:Q16 H11:CS14 H17:T17 V15:V16 Z15:CS16 H18:CS18 AJ17:CS17 H28:CS28 H37:CS42 H45:CS49 H31:CS34">
     <cfRule type="expression" dxfId="118" priority="7">
@@ -10885,7 +10884,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10895,7 +10894,7 @@
     <col min="3" max="3" width="14.85546875" style="107" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" style="105" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" style="124" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="123" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="106" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -10914,7 +10913,7 @@
       <c r="E1" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="105" t="s">
         <v>44</v>
       </c>
     </row>
@@ -10929,8 +10928,8 @@
         <v>8</v>
       </c>
       <c r="D2" s="105">
-        <f>(DATE(2012,6,10)+$C2+$C2/7)+IF(WEEKDAY((DATE(2012,6,10)+$C2+$C2/7),2)=6,2,0)+IF(WEEKDAY((DATE(2012,6,10)+$C2+$C2/7),2)=7,1,0)</f>
-        <v>41079.142857142855</v>
+        <f>(DATE(2012,6,10)+$C2+$C2/7*2)+IF(WEEKDAY((DATE(2012,6,10)+$C2+$C2/7*2),2)=6,2,0)+IF(WEEKDAY((DATE(2012,6,10)+$C2+$C2/7*2),2)=7,1,0)</f>
+        <v>41080.285714285717</v>
       </c>
       <c r="E2" s="44">
         <f>F2-DATE(2012,6,10)</f>
@@ -10951,10 +10950,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="105">
-        <f>($D2+$C3+$C3/7)+IF(WEEKDAY(($D2+$C3+$C3/7),2)=6,2,0)+IF(WEEKDAY(($D2+$C3+$C3/7),2)=7,1,0)</f>
-        <v>41085.857142857138</v>
-      </c>
-      <c r="E3" s="44"/>
+        <f>($D2+$C3+$C3/7*2)+IF(WEEKDAY(($D2+$C3+$C3/7*2),2)=6,2,0)+IF(WEEKDAY(($D2+$C3+$C3/7*2),2)=7,1,0)</f>
+        <v>41086.71428571429</v>
+      </c>
+      <c r="E3" s="44">
+        <f>F3-F2</f>
+        <v>6</v>
+      </c>
+      <c r="F3" s="123">
+        <v>41087</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
@@ -10967,8 +10972,8 @@
         <v>7</v>
       </c>
       <c r="D4" s="105">
-        <f t="shared" ref="D4:D8" si="0">($D3+$C4+$C4/7)+IF(WEEKDAY(($D3+$C4+$C4/7),2)=6,2,0)+IF(WEEKDAY(($D3+$C4+$C4/7),2)=7,1,0)</f>
-        <v>41093.857142857138</v>
+        <f t="shared" ref="D4:D8" si="0">($D3+$C4+$C4/7*2)+IF(WEEKDAY(($D3+$C4+$C4/7*2),2)=6,2,0)+IF(WEEKDAY(($D3+$C4+$C4/7*2),2)=7,1,0)</f>
+        <v>41095.71428571429</v>
       </c>
       <c r="E4" s="44"/>
     </row>
@@ -10984,8 +10989,9 @@
       </c>
       <c r="D5" s="105">
         <f t="shared" si="0"/>
-        <v>41101.857142857138</v>
-      </c>
+        <v>41106.71428571429</v>
+      </c>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="39" t="s">
@@ -10999,8 +11005,9 @@
       </c>
       <c r="D6" s="105">
         <f t="shared" si="0"/>
-        <v>41107.57142857142</v>
-      </c>
+        <v>41113.142857142862</v>
+      </c>
+      <c r="E6" s="44"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
@@ -11014,8 +11021,9 @@
       </c>
       <c r="D7" s="105">
         <f t="shared" si="0"/>
-        <v>41113.285714285703</v>
-      </c>
+        <v>41120.571428571435</v>
+      </c>
+      <c r="E7" s="44"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
@@ -11029,8 +11037,9 @@
       </c>
       <c r="D8" s="105">
         <f t="shared" si="0"/>
-        <v>41119.999999999985</v>
-      </c>
+        <v>41127.000000000007</v>
+      </c>
+      <c r="E8" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>